<commit_message>
Add AGG, MWTIX factors
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACEFE12-EE88-4375-96A0-DDFCC1D24F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034C9F5B-E626-4125-92C2-5C938D259E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="6" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="data_new" sheetId="7" r:id="rId3"/>
     <sheet name="lior" sheetId="9" r:id="rId4"/>
     <sheet name="data" sheetId="3" r:id="rId5"/>
-    <sheet name="data_old" sheetId="8" r:id="rId6"/>
-    <sheet name="read" sheetId="4" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId8"/>
-    <sheet name="read_old" sheetId="1" r:id="rId9"/>
+    <sheet name="read" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId7"/>
+    <sheet name="read_old" sheetId="1" r:id="rId8"/>
+    <sheet name="data_old" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="430">
   <si>
     <t>SPX</t>
   </si>
@@ -1365,6 +1365,12 @@
   </si>
   <si>
     <t>HYB</t>
+  </si>
+  <si>
+    <t>hyper_factor</t>
+  </si>
+  <si>
+    <t>MWTIX</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1462,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1585,8 +1594,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{26B58CFA-74FB-41FD-AB02-EC6D3EA4F4A1}">
-      <tableStyleElement type="wholeTable" dxfId="23"/>
-      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1659,18 +1668,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:I62" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:I62" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:J64" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:J64" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="13"/>
+    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="12">
       <calculatedColumnFormula>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1679,18 +1689,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:I45" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="1">
       <calculatedColumnFormula>IF(data_old[[#This Row],[description_override]]="",data_old[[#This Row],[Description_GPT]],data_old[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2017,9 +2027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6F81C3-35A2-4C92-A3A4-30A9105A6D5B}">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5595,7 +5603,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -5622,7 +5630,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
         <v>126</v>
@@ -5649,7 +5657,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
         <v>131</v>
@@ -5676,7 +5684,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
         <v>49</v>
@@ -5703,7 +5711,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C48" t="s">
         <v>135</v>
@@ -5730,7 +5738,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
         <v>344</v>
@@ -5757,7 +5765,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C50" t="s">
         <v>53</v>
@@ -5784,7 +5792,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
@@ -5811,7 +5819,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
@@ -5838,7 +5846,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
         <v>346</v>
@@ -5865,7 +5873,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C54" t="s">
         <v>345</v>
@@ -5894,7 +5902,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
         <v>97</v>
@@ -5921,7 +5929,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
         <v>349</v>
@@ -5948,7 +5956,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C57" t="s">
         <v>75</v>
@@ -5975,7 +5983,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C58" t="s">
         <v>99</v>
@@ -6002,7 +6010,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C59" t="s">
         <v>57</v>
@@ -6029,7 +6037,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C60" t="s">
         <v>59</v>
@@ -6056,7 +6064,7 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C61" t="s">
         <v>61</v>
@@ -6083,7 +6091,7 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C62" t="s">
         <v>63</v>
@@ -6110,7 +6118,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
         <v>66</v>
@@ -6137,7 +6145,7 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C64" t="s">
         <v>69</v>
@@ -6164,7 +6172,7 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
         <v>72</v>
@@ -6198,9 +6206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB67FE54-23CB-424E-AA4C-48055BA2B8E2}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6210,7 +6216,7 @@
       </c>
       <c r="B1" cm="1">
         <f t="array" ref="B1:B9">_xlfn.XMATCH(A1:A9,data[factor_name])</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" cm="1">
         <f t="array" ref="D1:D32">_xlfn.XLOOKUP(_xlfn._TRO_ALL(A:A),data[factor_name],data[Active])</f>
@@ -6222,7 +6228,7 @@
         <v>334</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -6233,7 +6239,7 @@
         <v>335</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -6244,7 +6250,7 @@
         <v>336</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -6255,7 +6261,7 @@
         <v>337</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -6471,23 +6477,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" customWidth="1"/>
-    <col min="9" max="9" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>322</v>
       </c>
@@ -6513,10 +6520,13 @@
         <v>151</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -6541,12 +6551,15 @@
       <c r="H2" s="4">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="str">
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>S&amp;P 500</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
@@ -6571,12 +6584,13 @@
       <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="4" t="str">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Russell 2000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
@@ -6601,12 +6615,13 @@
       <c r="H4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="str">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>S&amp;P 400</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
@@ -6631,12 +6646,13 @@
       <c r="H5" s="4">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="str">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Nasdaq 100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -6661,13 +6677,14 @@
       <c r="H6" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="4" t="str">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Dow Jones 30</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>425</v>
       </c>
@@ -6688,14 +6705,15 @@
       <c r="H7" s="4">
         <v>1</v>
       </c>
-      <c r="I7" s="8" t="str">
+      <c r="I7" s="4"/>
+      <c r="J7" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Technology</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="2"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>425</v>
       </c>
@@ -6716,13 +6734,14 @@
       <c r="H8" s="4">
         <v>1</v>
       </c>
-      <c r="I8" s="8" t="str">
+      <c r="I8" s="4"/>
+      <c r="J8" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Industrials</v>
       </c>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>425</v>
       </c>
@@ -6743,12 +6762,13 @@
       <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="I9" s="8" t="str">
+      <c r="I9" s="4"/>
+      <c r="J9" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Financials</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>425</v>
       </c>
@@ -6769,12 +6789,13 @@
       <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="8" t="str">
+      <c r="I10" s="4"/>
+      <c r="J10" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Regional Banks</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>425</v>
       </c>
@@ -6795,12 +6816,13 @@
       <c r="H11" s="4">
         <v>1</v>
       </c>
-      <c r="I11" s="8" t="str">
+      <c r="I11" s="4"/>
+      <c r="J11" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Communications</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>425</v>
       </c>
@@ -6821,12 +6843,13 @@
       <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="I12" s="8" t="str">
+      <c r="I12" s="4"/>
+      <c r="J12" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Energy</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>425</v>
       </c>
@@ -6847,12 +6870,13 @@
       <c r="H13" s="4">
         <v>1</v>
       </c>
-      <c r="I13" s="8" t="str">
+      <c r="I13" s="4"/>
+      <c r="J13" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Discretionary</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>425</v>
       </c>
@@ -6873,12 +6897,13 @@
       <c r="H14" s="4">
         <v>1</v>
       </c>
-      <c r="I14" s="8" t="str">
+      <c r="I14" s="4"/>
+      <c r="J14" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Materials</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>425</v>
       </c>
@@ -6899,12 +6924,13 @@
       <c r="H15" s="4">
         <v>1</v>
       </c>
-      <c r="I15" s="8" t="str">
+      <c r="I15" s="4"/>
+      <c r="J15" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Health Care</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>425</v>
       </c>
@@ -6925,12 +6951,13 @@
       <c r="H16" s="4">
         <v>1</v>
       </c>
-      <c r="I16" s="8" t="str">
+      <c r="I16" s="4"/>
+      <c r="J16" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Utilities</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>425</v>
       </c>
@@ -6951,12 +6978,13 @@
       <c r="H17" s="4">
         <v>1</v>
       </c>
-      <c r="I17" s="8" t="str">
+      <c r="I17" s="4"/>
+      <c r="J17" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Staples</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -6975,12 +7003,13 @@
       <c r="H18" s="4">
         <v>1</v>
       </c>
-      <c r="I18" s="8" t="str">
+      <c r="I18" s="4"/>
+      <c r="J18" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares U.S. Real Estate ETF</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -6999,12 +7028,13 @@
       <c r="H19" s="4">
         <v>1</v>
       </c>
-      <c r="I19" s="8" t="str">
+      <c r="I19" s="4"/>
+      <c r="J19" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Vanguard Real Estate ETF</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -7025,12 +7055,13 @@
       <c r="H20" s="4">
         <v>1</v>
       </c>
-      <c r="I20" s="8" t="str">
+      <c r="I20" s="4"/>
+      <c r="J20" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>AI</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -7051,12 +7082,13 @@
       <c r="H21" s="4">
         <v>1</v>
       </c>
-      <c r="I21" s="8" t="str">
+      <c r="I21" s="4"/>
+      <c r="J21" s="8" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Preferred</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>39</v>
       </c>
@@ -7081,12 +7113,13 @@
       <c r="H22" s="4">
         <v>1</v>
       </c>
-      <c r="I22" s="4" t="str">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Eurostoxx 50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -7107,12 +7140,13 @@
       <c r="H23" s="4">
         <v>0</v>
       </c>
-      <c r="I23" s="4" t="str">
+      <c r="I23" s="4"/>
+      <c r="J23" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Eurostoxx Banks</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
@@ -7133,12 +7167,13 @@
       <c r="H24" s="4">
         <v>1</v>
       </c>
-      <c r="I24" s="4" t="str">
+      <c r="I24" s="4"/>
+      <c r="J24" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares FTSE United Kingdom ETF</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
@@ -7163,12 +7198,13 @@
       <c r="H25" s="4">
         <v>1</v>
       </c>
-      <c r="I25" s="4" t="str">
+      <c r="I25" s="4"/>
+      <c r="J25" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>DAX (Germany)</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
@@ -7189,12 +7225,13 @@
       <c r="H26" s="4">
         <v>1</v>
       </c>
-      <c r="I26" s="4" t="str">
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares MSCI Canada ETF</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>39</v>
       </c>
@@ -7215,12 +7252,13 @@
       <c r="H27" s="4">
         <v>0</v>
       </c>
-      <c r="I27" s="4" t="str">
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>FTSE MIB (Italy)</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
@@ -7245,12 +7283,13 @@
       <c r="H28" s="4">
         <v>1</v>
       </c>
-      <c r="I28" s="4" t="str">
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>CAC 40 (France)</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
@@ -7271,12 +7310,13 @@
       <c r="H29" s="4">
         <v>1</v>
       </c>
-      <c r="I29" s="4" t="str">
+      <c r="I29" s="4"/>
+      <c r="J29" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares MSCI Italy ETF</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
@@ -7301,12 +7341,13 @@
       <c r="H30" s="4">
         <v>0</v>
       </c>
-      <c r="I30" s="4" t="str">
+      <c r="I30" s="4"/>
+      <c r="J30" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>IBEX 35 (Spain)</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -7327,12 +7368,13 @@
       <c r="H31" s="4">
         <v>0</v>
       </c>
-      <c r="I31" s="4" t="str">
+      <c r="I31" s="4"/>
+      <c r="J31" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares MSCI Spain ETF</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
@@ -7357,12 +7399,13 @@
       <c r="H32" s="4">
         <v>1</v>
       </c>
-      <c r="I32" s="4" t="str">
+      <c r="I32" s="4"/>
+      <c r="J32" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Nikkei 225</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>39</v>
       </c>
@@ -7387,12 +7430,13 @@
       <c r="H33" s="4">
         <v>1</v>
       </c>
-      <c r="I33" s="4" t="str">
+      <c r="I33" s="4"/>
+      <c r="J33" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>TOPIX</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
@@ -7415,12 +7459,13 @@
       <c r="H34" s="4">
         <v>1</v>
       </c>
-      <c r="I34" s="4" t="str">
+      <c r="I34" s="4"/>
+      <c r="J34" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares China Large-Cap ETF</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
@@ -7443,12 +7488,13 @@
       <c r="H35" s="4">
         <v>1</v>
       </c>
-      <c r="I35" s="4" t="str">
+      <c r="I35" s="4"/>
+      <c r="J35" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>39</v>
       </c>
@@ -7469,12 +7515,13 @@
       <c r="H36" s="4">
         <v>1</v>
       </c>
-      <c r="I36" s="4" t="str">
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>KraneShares CSI China Internet ETF</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>46</v>
       </c>
@@ -7497,12 +7544,13 @@
       <c r="H37" s="4">
         <v>1</v>
       </c>
-      <c r="I37" s="4" t="str">
+      <c r="I37" s="4"/>
+      <c r="J37" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares iBoxx $ Investment Grade Corporate Bond ETF</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
@@ -7525,12 +7573,13 @@
       <c r="H38" s="4">
         <v>1</v>
       </c>
-      <c r="I38" s="4" t="str">
+      <c r="I38" s="4"/>
+      <c r="J38" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares iBoxx $ High Yield Corporate Bond ETF</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>46</v>
       </c>
@@ -7549,12 +7598,13 @@
       <c r="H39" s="4">
         <v>1</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="4"/>
+      <c r="J39" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>46</v>
       </c>
@@ -7573,169 +7623,179 @@
       <c r="H40" s="4">
         <v>1</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="4"/>
+      <c r="J40" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4">
+        <v>1</v>
+      </c>
+      <c r="I42" s="4">
+        <v>1</v>
+      </c>
+      <c r="J42" s="4">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B43" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H41" s="4">
-        <v>1</v>
-      </c>
-      <c r="I41" s="4" t="str">
+      <c r="H43" s="4">
+        <v>1</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares 1-3 Year Treasury Bond ETF</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4" t="s">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H42" s="4">
-        <v>1</v>
-      </c>
-      <c r="I42" s="4" t="str">
+      <c r="H44" s="4">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares 3-7 Year Treasury Bond ETF</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B45" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4" t="s">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H43" s="4">
-        <v>1</v>
-      </c>
-      <c r="I43" s="4" t="str">
+      <c r="H45" s="4">
+        <v>1</v>
+      </c>
+      <c r="I45" s="4">
+        <v>1</v>
+      </c>
+      <c r="J45" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares 7-10 Year Treasury Bond ETF</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B46" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H44" s="4">
-        <v>1</v>
-      </c>
-      <c r="I44" s="4" t="str">
+      <c r="H46" s="4">
+        <v>1</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>iShares 20+ Year Treasury Bond ETF</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H45" s="4">
-        <v>1</v>
-      </c>
-      <c r="I45" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares TIPS Bond ETF</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4">
-        <v>1</v>
-      </c>
-      <c r="I46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>128</v>
       </c>
@@ -7743,25 +7803,26 @@
         <v>40</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>53</v>
+        <v>135</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="H47" s="4">
-        <v>0</v>
-      </c>
-      <c r="I47" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares MBS ETF</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>iShares TIPS Bond ETF</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>128</v>
       </c>
@@ -7769,25 +7830,19 @@
         <v>40</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>14</v>
+        <v>344</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
-      <c r="F48" t="s">
-        <v>152</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
       <c r="H48" s="4">
-        <v>0</v>
-      </c>
-      <c r="I48" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>Simplify Mortgage Backed Securities ETF</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>128</v>
       </c>
@@ -7795,103 +7850,111 @@
         <v>40</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4" t="str">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>iShares MBS ETF</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" t="s">
+        <v>152</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4" t="str">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>Simplify Mortgage Backed Securities ETF</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H49" s="4">
-        <v>1</v>
-      </c>
-      <c r="I49" s="4" t="str">
+      <c r="H51" s="4">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>AGNC Investment Corp.</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4">
-        <v>1</v>
-      </c>
-      <c r="I50" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4">
-        <v>1</v>
-      </c>
-      <c r="I51" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>97</v>
+        <v>346</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
       <c r="H52" s="4">
         <v>1</v>
       </c>
-      <c r="I52" s="4" t="str">
+      <c r="I52" s="4"/>
+      <c r="J52" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -7900,114 +7963,115 @@
       <c r="H53" s="4">
         <v>1</v>
       </c>
-      <c r="I53" s="4">
+      <c r="I53" s="4"/>
+      <c r="J53" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H54" s="4">
+        <v>1</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4" t="str">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" t="s">
         <v>75</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F56" t="s">
         <v>76</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G56" t="s">
         <v>114</v>
       </c>
-      <c r="H54" s="4">
-        <v>0</v>
-      </c>
-      <c r="I54" s="4" t="str">
+      <c r="H56" s="4">
+        <v>0</v>
+      </c>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>WisdomTree Emerging Markets Local Debt Fund</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H55" s="4">
-        <v>0</v>
-      </c>
-      <c r="I55" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares International Government Bonds ETF</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H56" s="4">
-        <v>1</v>
-      </c>
-      <c r="I56" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>SPDR Gold Shares</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="H57" s="4">
-        <v>1</v>
-      </c>
-      <c r="I57" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares Silver Trust</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>iShares International Government Bonds ETF</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>56</v>
       </c>
@@ -8015,25 +8079,26 @@
         <v>40</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H58" s="4">
         <v>1</v>
       </c>
-      <c r="I58" s="4" t="str">
+      <c r="I58" s="4"/>
+      <c r="J58" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>United States Oil Fund</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>SPDR Gold Shares</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
@@ -8041,96 +8106,154 @@
         <v>40</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H59" s="4">
         <v>1</v>
       </c>
-      <c r="I59" s="4" t="str">
+      <c r="I59" s="4"/>
+      <c r="J59" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>Invesco DB Commodity Index Tracking Fund</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>iShares Silver Trust</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H60" s="4">
         <v>1</v>
       </c>
-      <c r="I60" s="4" t="str">
+      <c r="I60" s="4"/>
+      <c r="J60" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>United States Oil Fund</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H61" s="4">
+        <v>1</v>
+      </c>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4" t="str">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>Invesco DB Commodity Index Tracking Fund</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H62" s="4">
+        <v>1</v>
+      </c>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4" t="str">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="G63" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H61" s="4">
-        <v>1</v>
-      </c>
-      <c r="I61" s="4" t="str">
+      <c r="H63" s="4">
+        <v>1</v>
+      </c>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Invesco CurrencyShares Euro Trust</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>65</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>71</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>72</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F64" t="s">
         <v>73</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G64" t="s">
         <v>113</v>
       </c>
-      <c r="H62" s="4">
-        <v>1</v>
-      </c>
-      <c r="I62" s="4" t="str">
+      <c r="H64" s="4">
+        <v>1</v>
+      </c>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>Invesco CurrencyShares Japanese Yen Trust</v>
       </c>
@@ -8145,10 +8268,1220 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
+  <dimension ref="A1:E56"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="44.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A56">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
+        <v>SPY</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:E56">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:E1,data[#Headers]))</f>
+        <v>Equities</v>
+      </c>
+      <c r="C2" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>S&amp;P 500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>IWM</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C3" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Russell 2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>MDY</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C4" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <v>S&amp;P 400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>QQQ</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C5" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Nasdaq 100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <v>DIA</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C6" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Dow Jones 30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <v>XLK</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C7" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Technology</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <v>XLI</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C8" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Industrials</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <v>XLF</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C9" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Financials</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <v>KRE</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C10" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Regional Banks</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <v>XLC</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C11" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Communications</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <v>XLE</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C12" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Energy</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <v>XLY</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C13" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Discretionary</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <v>XLB</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C14" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Materials</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <v>XLV</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C15" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Health Care</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <v>XLU</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C16" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Utilities</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <v>XLP</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C17" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Staples</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <v>IYR</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C18" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>iShares U.S. Real Estate ETF</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <v>VNQ</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C19" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Vanguard Real Estate ETF</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <v>AIQ</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C20" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="str">
+        <v>AI</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <v>PFF</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C21" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Preferred</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <v>FEZ</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C22" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Eurostoxx 50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <v>EWU</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C23" t="str">
+        <v>GBP</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="str">
+        <v>iShares FTSE United Kingdom ETF</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <v>DAX</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C24" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="str">
+        <v>DAX (Germany)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <v>EWC</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C25" t="str">
+        <v>CAD</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="str">
+        <v>iShares MSCI Canada ETF</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <v>CAC</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C26" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="str">
+        <v>CAC 40 (France)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <v>EWI</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C27" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="str">
+        <v>iShares MSCI Italy ETF</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <v>^N225</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C28" t="str">
+        <v>JPY</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Nikkei 225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <v>TPX</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C29" t="str">
+        <v>JPY</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <v>TOPIX</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <v>FXI</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C30" t="str">
+        <v>CNH</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="str">
+        <v>iShares China Large-Cap ETF</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <v>ASHR</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C31" t="str">
+        <v>CNH</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <v>KWEB</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C32" t="str">
+        <v>CNH</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="str">
+        <v>KraneShares CSI China Internet ETF</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <v>LQD</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C33" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="str">
+        <v>iShares iBoxx $ Investment Grade Corporate Bond ETF</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <v>HYG</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C34" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="str">
+        <v>iShares iBoxx $ High Yield Corporate Bond ETF</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <v>LQDH</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C35" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <v>HYGH</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C36" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <v>AGG</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C37" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <v>MWTIX</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C38" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <v>SHY</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C39" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="str">
+        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <v>IEI</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C40" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="str">
+        <v>iShares 3-7 Year Treasury Bond ETF</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <v>IEF</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C41" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="str">
+        <v>iShares 7-10 Year Treasury Bond ETF</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <v>TLT</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C42" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="str">
+        <v>iShares 20+ Year Treasury Bond ETF</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <v>TIP</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C43" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="str">
+        <v>iShares TIPS Bond ETF</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <v>VTIP</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C44" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <v>AGNC</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C45" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" t="str">
+        <v>AGNC Investment Corp.</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <v>VMBS</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C46" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <v>CMBS</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C47" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <v>EMB</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C48" t="str">
+        <v>EM</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="str">
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <v>EMHY</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C49" t="str">
+        <v>EM</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <v>GLD</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C50" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="str">
+        <v>SPDR Gold Shares</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <v>SLV</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C51" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" t="str">
+        <v>iShares Silver Trust</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <v>USO</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C52" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="str">
+        <v>United States Oil Fund</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <v>DBC</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C53" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Invesco DB Commodity Index Tracking Fund</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <v>UUP</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C54" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <v>FXE</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C55" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Invesco CurrencyShares Euro Trust</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <v>FXY</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C56" t="str">
+        <v>JPY</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Invesco CurrencyShares Japanese Yen Trust</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509EC1D2-D913-4E91-BF4A-1B9A2D2D358E}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="102.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28B96AA-E903-4E49-8EE7-2DF563672EF4}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BECED18-9D5B-4FAE-9BAD-99DBF8245FFA}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:I25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10056,1018 +11389,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
-  <dimension ref="A1:D54"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="44.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A54">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
-        <v>SPY</v>
-      </c>
-      <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:D54">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:D1,data[#Headers]))</f>
-        <v>Equities</v>
-      </c>
-      <c r="C2" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D2" t="str">
-        <v>S&amp;P 500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>IWM</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C3" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Russell 2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>MDY</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C4" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D4" t="str">
-        <v>S&amp;P 400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>QQQ</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C5" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Nasdaq 100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <v>DIA</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C6" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Dow Jones 30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <v>XLK</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C7" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Technology</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <v>XLI</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C8" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Industrials</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <v>XLF</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C9" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Financials</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <v>KRE</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C10" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Regional Banks</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <v>XLC</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C11" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Communications</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <v>XLE</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C12" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Energy</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <v>XLY</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C13" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D13" t="str">
-        <v>Discretionary</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <v>XLB</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C14" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D14" t="str">
-        <v>Materials</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <v>XLV</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C15" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D15" t="str">
-        <v>Health Care</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <v>XLU</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C16" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D16" t="str">
-        <v>Utilities</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <v>XLP</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C17" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D17" t="str">
-        <v>Staples</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <v>IYR</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C18" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D18" t="str">
-        <v>iShares U.S. Real Estate ETF</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <v>VNQ</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C19" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D19" t="str">
-        <v>Vanguard Real Estate ETF</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <v>AIQ</v>
-      </c>
-      <c r="B20" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C20" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D20" t="str">
-        <v>AI</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <v>PFF</v>
-      </c>
-      <c r="B21" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C21" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D21" t="str">
-        <v>Preferred</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <v>FEZ</v>
-      </c>
-      <c r="B22" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C22" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D22" t="str">
-        <v>Eurostoxx 50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <v>EWU</v>
-      </c>
-      <c r="B23" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C23" t="str">
-        <v>GBP</v>
-      </c>
-      <c r="D23" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <v>DAX</v>
-      </c>
-      <c r="B24" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C24" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D24" t="str">
-        <v>DAX (Germany)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <v>EWC</v>
-      </c>
-      <c r="B25" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C25" t="str">
-        <v>CAD</v>
-      </c>
-      <c r="D25" t="str">
-        <v>iShares MSCI Canada ETF</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
-        <v>CAC</v>
-      </c>
-      <c r="B26" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C26" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D26" t="str">
-        <v>CAC 40 (France)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <v>EWI</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C27" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D27" t="str">
-        <v>iShares MSCI Italy ETF</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <v>^N225</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C28" t="str">
-        <v>JPY</v>
-      </c>
-      <c r="D28" t="str">
-        <v>Nikkei 225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <v>TPX</v>
-      </c>
-      <c r="B29" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C29" t="str">
-        <v>JPY</v>
-      </c>
-      <c r="D29" t="str">
-        <v>TOPIX</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <v>FXI</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C30" t="str">
-        <v>CNH</v>
-      </c>
-      <c r="D30" t="str">
-        <v>iShares China Large-Cap ETF</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <v>ASHR</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C31" t="str">
-        <v>CNH</v>
-      </c>
-      <c r="D31" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <v>KWEB</v>
-      </c>
-      <c r="B32" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C32" t="str">
-        <v>CNH</v>
-      </c>
-      <c r="D32" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <v>LQD</v>
-      </c>
-      <c r="B33" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C33" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D33" t="str">
-        <v>iShares iBoxx $ Investment Grade Corporate Bond ETF</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
-        <v>HYG</v>
-      </c>
-      <c r="B34" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C34" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D34" t="str">
-        <v>iShares iBoxx $ High Yield Corporate Bond ETF</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <v>LQDH</v>
-      </c>
-      <c r="B35" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C35" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="str">
-        <v>HYGH</v>
-      </c>
-      <c r="B36" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C36" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="str">
-        <v>SHY</v>
-      </c>
-      <c r="B37" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C37" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D37" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="str">
-        <v>IEI</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C38" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D38" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="str">
-        <v>IEF</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C39" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D39" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="str">
-        <v>TLT</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C40" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D40" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="str">
-        <v>TIP</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C41" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D41" t="str">
-        <v>iShares TIPS Bond ETF</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="str">
-        <v>VTIP</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C42" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="str">
-        <v>AGNC</v>
-      </c>
-      <c r="B43" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C43" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D43" t="str">
-        <v>AGNC Investment Corp.</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="str">
-        <v>VMBS</v>
-      </c>
-      <c r="B44" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C44" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="str">
-        <v>CMBS</v>
-      </c>
-      <c r="B45" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C45" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="str">
-        <v>EMB</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C46" t="str">
-        <v>EM</v>
-      </c>
-      <c r="D46" t="str">
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="str">
-        <v>EMHY</v>
-      </c>
-      <c r="B47" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C47" t="str">
-        <v>EM</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="str">
-        <v>GLD</v>
-      </c>
-      <c r="B48" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C48" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D48" t="str">
-        <v>SPDR Gold Shares</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="str">
-        <v>SLV</v>
-      </c>
-      <c r="B49" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C49" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D49" t="str">
-        <v>iShares Silver Trust</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="str">
-        <v>USO</v>
-      </c>
-      <c r="B50" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C50" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D50" t="str">
-        <v>United States Oil Fund</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="str">
-        <v>DBC</v>
-      </c>
-      <c r="B51" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C51" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D51" t="str">
-        <v>Invesco DB Commodity Index Tracking Fund</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="str">
-        <v>UUP</v>
-      </c>
-      <c r="B52" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C52" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D52" t="str">
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="str">
-        <v>FXE</v>
-      </c>
-      <c r="B53" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C53" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D53" t="str">
-        <v>Invesco CurrencyShares Euro Trust</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="str">
-        <v>FXY</v>
-      </c>
-      <c r="B54" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C54" t="str">
-        <v>JPY</v>
-      </c>
-      <c r="D54" t="str">
-        <v>Invesco CurrencyShares Japanese Yen Trust</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509EC1D2-D913-4E91-BF4A-1B9A2D2D358E}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="102.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28B96AA-E903-4E49-8EE7-2DF563672EF4}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Ensure portfolio factors are in factor set
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAF7574-526E-4857-A029-F28FB009A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D747E5-6DDB-4352-86AE-6D577A474DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="7" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="legacy" sheetId="5" r:id="rId1"/>
-    <sheet name="gpt" sheetId="6" r:id="rId2"/>
-    <sheet name="data_new" sheetId="7" r:id="rId3"/>
-    <sheet name="lior" sheetId="9" r:id="rId4"/>
-    <sheet name="portfolios" sheetId="10" r:id="rId5"/>
-    <sheet name="data" sheetId="3" r:id="rId6"/>
-    <sheet name="read2" sheetId="12" r:id="rId7"/>
-    <sheet name="read" sheetId="4" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId9"/>
-    <sheet name="read_old" sheetId="1" r:id="rId10"/>
-    <sheet name="data_old" sheetId="8" r:id="rId11"/>
+    <sheet name="composites" sheetId="13" r:id="rId1"/>
+    <sheet name="read_composites" sheetId="14" r:id="rId2"/>
+    <sheet name="legacy" sheetId="5" r:id="rId3"/>
+    <sheet name="gpt" sheetId="6" r:id="rId4"/>
+    <sheet name="data_new" sheetId="7" r:id="rId5"/>
+    <sheet name="lior" sheetId="9" r:id="rId6"/>
+    <sheet name="data" sheetId="3" r:id="rId7"/>
+    <sheet name="read" sheetId="12" r:id="rId8"/>
+    <sheet name="read_old2" sheetId="4" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId10"/>
+    <sheet name="read_old" sheetId="1" r:id="rId11"/>
+    <sheet name="data_old" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="450">
   <si>
     <t>SPX</t>
   </si>
@@ -1427,6 +1428,12 @@
   </si>
   <si>
     <t>BSV</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>portfolio_name</t>
   </si>
 </sst>
 </file>
@@ -2080,1412 +2087,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6F81C3-35A2-4C92-A3A4-30A9105A6D5B}">
-  <dimension ref="A1:G81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C34FC6-78FE-492E-BECF-2EB9A04778A9}">
+  <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>283</v>
-      </c>
-    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>430</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
+        <v>433</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>421</v>
+      </c>
+      <c r="G2" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
+        <v>175</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
+        <v>431</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>434</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F4" t="s">
-        <v>284</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" t="s">
-        <v>173</v>
-      </c>
-      <c r="F6" t="s">
-        <v>173</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
+        <v>236</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>321</v>
+        <v>435</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" t="s">
-        <v>174</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
+        <v>238</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
       </c>
       <c r="C8" t="s">
-        <v>321</v>
-      </c>
-      <c r="D8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" t="s">
-        <v>175</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>321</v>
-      </c>
-      <c r="D9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" t="s">
-        <v>176</v>
-      </c>
-      <c r="F9" t="s">
-        <v>176</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>321</v>
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E10" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" t="s">
-        <v>177</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>321</v>
-      </c>
-      <c r="D11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" t="s">
-        <v>342</v>
-      </c>
-      <c r="F11" t="s">
-        <v>342</v>
+        <v>403</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>321</v>
-      </c>
-      <c r="D12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" t="s">
-        <v>178</v>
+        <v>438</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>321</v>
-      </c>
-      <c r="D13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F13" t="s">
-        <v>179</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>321</v>
-      </c>
-      <c r="D14" t="s">
-        <v>167</v>
-      </c>
-      <c r="E14" t="s">
-        <v>180</v>
-      </c>
-      <c r="F14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>321</v>
-      </c>
-      <c r="D15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E15" t="s">
-        <v>181</v>
-      </c>
-      <c r="F15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E16" t="s">
-        <v>182</v>
-      </c>
-      <c r="F16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" t="s">
-        <v>170</v>
-      </c>
-      <c r="E17" t="s">
-        <v>183</v>
-      </c>
-      <c r="F17" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
-      </c>
-      <c r="E18" t="s">
-        <v>184</v>
-      </c>
-      <c r="F18" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" t="s">
-        <v>156</v>
-      </c>
-      <c r="F20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>157</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>158</v>
-      </c>
-      <c r="E22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E23" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" t="s">
-        <v>186</v>
-      </c>
-      <c r="E24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E25" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>188</v>
-      </c>
-      <c r="E26" t="s">
-        <v>288</v>
-      </c>
-      <c r="F26" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" t="s">
-        <v>196</v>
-      </c>
-      <c r="F27" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" t="s">
-        <v>190</v>
-      </c>
-      <c r="E28" t="s">
-        <v>197</v>
-      </c>
-      <c r="F28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" t="s">
-        <v>191</v>
-      </c>
-      <c r="E29" t="s">
-        <v>198</v>
-      </c>
-      <c r="F29" t="s">
-        <v>198</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" t="s">
-        <v>192</v>
-      </c>
-      <c r="E30" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" t="s">
-        <v>193</v>
-      </c>
-      <c r="E32" t="s">
-        <v>199</v>
-      </c>
-      <c r="F32" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" t="s">
-        <v>201</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" t="s">
-        <v>203</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" t="s">
-        <v>204</v>
-      </c>
-      <c r="E37" t="s">
-        <v>205</v>
-      </c>
-      <c r="F37" t="s">
-        <v>293</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" t="s">
-        <v>206</v>
-      </c>
-      <c r="E38" t="s">
-        <v>209</v>
-      </c>
-      <c r="F38" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" t="s">
-        <v>207</v>
-      </c>
-      <c r="E39" t="s">
-        <v>210</v>
-      </c>
-      <c r="F39" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" t="s">
-        <v>208</v>
-      </c>
-      <c r="E40" t="s">
-        <v>211</v>
-      </c>
-      <c r="F40" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>128</v>
-      </c>
-      <c r="B41" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" t="s">
-        <v>212</v>
-      </c>
-      <c r="E41" t="s">
-        <v>218</v>
-      </c>
-      <c r="F41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" t="s">
-        <v>213</v>
-      </c>
-      <c r="E42" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" t="s">
-        <v>214</v>
-      </c>
-      <c r="E43" t="s">
-        <v>131</v>
-      </c>
-      <c r="F43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E44" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" t="s">
-        <v>216</v>
-      </c>
-      <c r="E45" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" t="s">
-        <v>217</v>
-      </c>
-      <c r="E46" t="s">
-        <v>219</v>
-      </c>
-      <c r="F46" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>128</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" t="s">
-        <v>221</v>
-      </c>
-      <c r="E47" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>128</v>
-      </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>222</v>
-      </c>
-      <c r="E48" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" t="s">
-        <v>223</v>
-      </c>
-      <c r="E49" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" t="s">
-        <v>224</v>
-      </c>
-      <c r="E50" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="D51" t="s">
-        <v>225</v>
-      </c>
-      <c r="E51" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>128</v>
-      </c>
-      <c r="B52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" t="s">
-        <v>226</v>
-      </c>
-      <c r="E52" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" t="s">
-        <v>227</v>
-      </c>
-      <c r="E53" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" t="s">
-        <v>228</v>
-      </c>
-      <c r="E54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>128</v>
-      </c>
-      <c r="B55" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" t="s">
-        <v>229</v>
-      </c>
-      <c r="E55" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56" t="s">
-        <v>230</v>
-      </c>
-      <c r="E56" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>128</v>
-      </c>
-      <c r="B57" t="s">
-        <v>220</v>
-      </c>
-      <c r="D57" t="s">
-        <v>231</v>
-      </c>
-      <c r="E57" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" t="s">
-        <v>220</v>
-      </c>
-      <c r="D58" t="s">
-        <v>232</v>
-      </c>
-      <c r="E58" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>128</v>
-      </c>
-      <c r="B59" t="s">
-        <v>220</v>
-      </c>
-      <c r="D59" t="s">
-        <v>233</v>
-      </c>
-      <c r="E59" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>128</v>
-      </c>
-      <c r="B60" t="s">
-        <v>220</v>
-      </c>
-      <c r="D60" t="s">
-        <v>234</v>
-      </c>
-      <c r="E60" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>128</v>
-      </c>
-      <c r="B61" t="s">
-        <v>220</v>
-      </c>
-      <c r="D61" t="s">
-        <v>235</v>
-      </c>
-      <c r="E61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" t="s">
-        <v>318</v>
-      </c>
-      <c r="D62" t="s">
-        <v>147</v>
-      </c>
-      <c r="E62" t="s">
-        <v>68</v>
-      </c>
-      <c r="F62" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" t="s">
-        <v>318</v>
-      </c>
-      <c r="D63" t="s">
-        <v>266</v>
-      </c>
-      <c r="E63" t="s">
-        <v>71</v>
-      </c>
-      <c r="F63" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" t="s">
-        <v>318</v>
-      </c>
-      <c r="D64" t="s">
-        <v>267</v>
-      </c>
-      <c r="E64" t="s">
-        <v>220</v>
-      </c>
-      <c r="F64" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" t="s">
-        <v>251</v>
-      </c>
-      <c r="D65" t="s">
-        <v>268</v>
-      </c>
-      <c r="E65" t="s">
-        <v>251</v>
-      </c>
-      <c r="F65" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>251</v>
-      </c>
-      <c r="D66" t="s">
-        <v>269</v>
-      </c>
-      <c r="E66" t="s">
-        <v>252</v>
-      </c>
-      <c r="F66" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
-        <v>317</v>
-      </c>
-      <c r="D67" t="s">
-        <v>270</v>
-      </c>
-      <c r="E67" t="s">
-        <v>88</v>
-      </c>
-      <c r="F67" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" t="s">
-        <v>317</v>
-      </c>
-      <c r="D68" t="s">
-        <v>271</v>
-      </c>
-      <c r="E68" t="s">
-        <v>253</v>
-      </c>
-      <c r="F68" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" t="s">
-        <v>317</v>
-      </c>
-      <c r="D69" t="s">
-        <v>272</v>
-      </c>
-      <c r="E69" t="s">
-        <v>254</v>
-      </c>
-      <c r="F69" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" t="s">
-        <v>317</v>
-      </c>
-      <c r="D70" t="s">
-        <v>273</v>
-      </c>
-      <c r="E70" t="s">
-        <v>255</v>
-      </c>
-      <c r="F70" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" t="s">
-        <v>319</v>
-      </c>
-      <c r="D71" t="s">
-        <v>274</v>
-      </c>
-      <c r="E71" t="s">
-        <v>79</v>
-      </c>
-      <c r="F71" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" t="s">
-        <v>319</v>
-      </c>
-      <c r="D72" t="s">
-        <v>275</v>
-      </c>
-      <c r="E72" t="s">
-        <v>256</v>
-      </c>
-      <c r="F72" t="s">
-        <v>307</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" t="s">
-        <v>319</v>
-      </c>
-      <c r="D73" t="s">
-        <v>276</v>
-      </c>
-      <c r="E73" t="s">
-        <v>257</v>
-      </c>
-      <c r="F73" t="s">
-        <v>308</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>65</v>
-      </c>
-      <c r="B74" t="s">
-        <v>319</v>
-      </c>
-      <c r="D74" t="s">
-        <v>277</v>
-      </c>
-      <c r="E74" t="s">
-        <v>258</v>
-      </c>
-      <c r="F74" t="s">
-        <v>309</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>65</v>
-      </c>
-      <c r="B75" t="s">
-        <v>74</v>
-      </c>
-      <c r="D75" t="s">
-        <v>278</v>
-      </c>
-      <c r="E75" t="s">
-        <v>259</v>
-      </c>
-      <c r="F75" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>65</v>
-      </c>
-      <c r="B76" t="s">
-        <v>74</v>
-      </c>
-      <c r="D76" t="s">
-        <v>279</v>
-      </c>
-      <c r="E76" t="s">
-        <v>260</v>
-      </c>
-      <c r="F76" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>65</v>
-      </c>
-      <c r="B77" t="s">
-        <v>74</v>
-      </c>
-      <c r="D77" t="s">
-        <v>280</v>
-      </c>
-      <c r="E77" t="s">
-        <v>261</v>
-      </c>
-      <c r="F77" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" t="s">
-        <v>74</v>
-      </c>
-      <c r="D78" t="s">
-        <v>281</v>
-      </c>
-      <c r="E78" t="s">
-        <v>262</v>
-      </c>
-      <c r="F78" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>56</v>
-      </c>
-      <c r="B79" t="s">
-        <v>56</v>
-      </c>
-      <c r="D79" t="s">
-        <v>146</v>
-      </c>
-      <c r="E79" t="s">
-        <v>263</v>
-      </c>
-      <c r="F79" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>56</v>
-      </c>
-      <c r="B80" t="s">
-        <v>56</v>
-      </c>
-      <c r="D80" t="s">
-        <v>282</v>
-      </c>
-      <c r="E80" t="s">
-        <v>264</v>
-      </c>
-      <c r="F80" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>56</v>
-      </c>
-      <c r="B81" t="s">
-        <v>56</v>
-      </c>
-      <c r="D81" t="s">
-        <v>265</v>
-      </c>
-      <c r="E81" t="s">
-        <v>265</v>
-      </c>
-      <c r="F81" t="s">
-        <v>314</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -3494,6 +2231,124 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509EC1D2-D913-4E91-BF4A-1B9A2D2D358E}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="102.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28B96AA-E903-4E49-8EE7-2DF563672EF4}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3613,7 +2468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BECED18-9D5B-4FAE-9BAD-99DBF8245FFA}">
   <dimension ref="A1:M74"/>
   <sheetViews>
@@ -5530,6 +4385,1545 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A5BD3C-985E-4AF9-B99B-18E2DCAB8A90}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>439</v>
+      </c>
+      <c r="B7" t="s">
+        <v>447</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>421</v>
+      </c>
+      <c r="B8" t="s">
+        <v>403</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>421</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6F81C3-35A2-4C92-A3A4-30A9105A6D5B}">
+  <dimension ref="A1:G81"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>321</v>
+      </c>
+      <c r="D9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" t="s">
+        <v>342</v>
+      </c>
+      <c r="F11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>321</v>
+      </c>
+      <c r="D14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>321</v>
+      </c>
+      <c r="D15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" t="s">
+        <v>288</v>
+      </c>
+      <c r="F26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" t="s">
+        <v>196</v>
+      </c>
+      <c r="F27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E28" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" t="s">
+        <v>198</v>
+      </c>
+      <c r="F29" t="s">
+        <v>198</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>193</v>
+      </c>
+      <c r="E32" t="s">
+        <v>199</v>
+      </c>
+      <c r="F32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>202</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>204</v>
+      </c>
+      <c r="E37" t="s">
+        <v>205</v>
+      </c>
+      <c r="F37" t="s">
+        <v>293</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>206</v>
+      </c>
+      <c r="E38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F38" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>207</v>
+      </c>
+      <c r="E39" t="s">
+        <v>210</v>
+      </c>
+      <c r="F39" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" t="s">
+        <v>211</v>
+      </c>
+      <c r="F40" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>212</v>
+      </c>
+      <c r="E41" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>213</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>214</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
+        <v>215</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>217</v>
+      </c>
+      <c r="E46" t="s">
+        <v>219</v>
+      </c>
+      <c r="F46" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" t="s">
+        <v>222</v>
+      </c>
+      <c r="E48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" t="s">
+        <v>223</v>
+      </c>
+      <c r="E49" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" t="s">
+        <v>225</v>
+      </c>
+      <c r="E51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" t="s">
+        <v>226</v>
+      </c>
+      <c r="E52" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>227</v>
+      </c>
+      <c r="E53" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" t="s">
+        <v>228</v>
+      </c>
+      <c r="E54" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" t="s">
+        <v>220</v>
+      </c>
+      <c r="D57" t="s">
+        <v>231</v>
+      </c>
+      <c r="E57" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" t="s">
+        <v>232</v>
+      </c>
+      <c r="E58" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" t="s">
+        <v>220</v>
+      </c>
+      <c r="D59" t="s">
+        <v>233</v>
+      </c>
+      <c r="E59" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" t="s">
+        <v>234</v>
+      </c>
+      <c r="E60" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" t="s">
+        <v>235</v>
+      </c>
+      <c r="E61" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>318</v>
+      </c>
+      <c r="D62" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F62" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>318</v>
+      </c>
+      <c r="D63" t="s">
+        <v>266</v>
+      </c>
+      <c r="E63" t="s">
+        <v>71</v>
+      </c>
+      <c r="F63" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" t="s">
+        <v>318</v>
+      </c>
+      <c r="D64" t="s">
+        <v>267</v>
+      </c>
+      <c r="E64" t="s">
+        <v>220</v>
+      </c>
+      <c r="F64" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>251</v>
+      </c>
+      <c r="D65" t="s">
+        <v>268</v>
+      </c>
+      <c r="E65" t="s">
+        <v>251</v>
+      </c>
+      <c r="F65" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>251</v>
+      </c>
+      <c r="D66" t="s">
+        <v>269</v>
+      </c>
+      <c r="E66" t="s">
+        <v>252</v>
+      </c>
+      <c r="F66" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D67" t="s">
+        <v>270</v>
+      </c>
+      <c r="E67" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>317</v>
+      </c>
+      <c r="D68" t="s">
+        <v>271</v>
+      </c>
+      <c r="E68" t="s">
+        <v>253</v>
+      </c>
+      <c r="F68" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" t="s">
+        <v>317</v>
+      </c>
+      <c r="D69" t="s">
+        <v>272</v>
+      </c>
+      <c r="E69" t="s">
+        <v>254</v>
+      </c>
+      <c r="F69" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>317</v>
+      </c>
+      <c r="D70" t="s">
+        <v>273</v>
+      </c>
+      <c r="E70" t="s">
+        <v>255</v>
+      </c>
+      <c r="F70" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" t="s">
+        <v>319</v>
+      </c>
+      <c r="D71" t="s">
+        <v>274</v>
+      </c>
+      <c r="E71" t="s">
+        <v>79</v>
+      </c>
+      <c r="F71" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s">
+        <v>319</v>
+      </c>
+      <c r="D72" t="s">
+        <v>275</v>
+      </c>
+      <c r="E72" t="s">
+        <v>256</v>
+      </c>
+      <c r="F72" t="s">
+        <v>307</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" t="s">
+        <v>319</v>
+      </c>
+      <c r="D73" t="s">
+        <v>276</v>
+      </c>
+      <c r="E73" t="s">
+        <v>257</v>
+      </c>
+      <c r="F73" t="s">
+        <v>308</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" t="s">
+        <v>319</v>
+      </c>
+      <c r="D74" t="s">
+        <v>277</v>
+      </c>
+      <c r="E74" t="s">
+        <v>258</v>
+      </c>
+      <c r="F74" t="s">
+        <v>309</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" t="s">
+        <v>278</v>
+      </c>
+      <c r="E75" t="s">
+        <v>259</v>
+      </c>
+      <c r="F75" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" t="s">
+        <v>279</v>
+      </c>
+      <c r="E76" t="s">
+        <v>260</v>
+      </c>
+      <c r="F76" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" t="s">
+        <v>280</v>
+      </c>
+      <c r="E77" t="s">
+        <v>261</v>
+      </c>
+      <c r="F77" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" t="s">
+        <v>281</v>
+      </c>
+      <c r="E78" t="s">
+        <v>262</v>
+      </c>
+      <c r="F78" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" t="s">
+        <v>146</v>
+      </c>
+      <c r="E79" t="s">
+        <v>263</v>
+      </c>
+      <c r="F79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>56</v>
+      </c>
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" t="s">
+        <v>282</v>
+      </c>
+      <c r="E80" t="s">
+        <v>264</v>
+      </c>
+      <c r="F80" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" t="s">
+        <v>265</v>
+      </c>
+      <c r="E81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F81" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D44DBA8-A8E6-40E1-8916-CA07A080AF7C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
@@ -6581,7 +6975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8E9F76-5104-49FC-BB43-6F7BA8306F2B}">
   <dimension ref="A5:O65"/>
   <sheetViews>
@@ -8294,7 +8688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB67FE54-23CB-424E-AA4C-48055BA2B8E2}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -8567,159 +8961,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B743FD7B-82CD-4F35-99E1-FCE8FAB32A03}">
-  <dimension ref="A2:G14"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C2" t="s">
-        <v>433</v>
-      </c>
-      <c r="F2" t="s">
-        <v>421</v>
-      </c>
-      <c r="G2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>431</v>
-      </c>
-      <c r="B4">
-        <v>-1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>434</v>
-      </c>
-      <c r="D4" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>-1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D7" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>238</v>
-      </c>
-      <c r="B8">
-        <v>-1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10">
-        <v>-1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>403</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>438</v>
-      </c>
-      <c r="F12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>441</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11015,11 +11261,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12213,7 +12461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
   <dimension ref="A1:E56"/>
   <sheetViews>
@@ -13183,122 +13431,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509EC1D2-D913-4E91-BF4A-1B9A2D2D358E}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="102.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add implied correlation factor
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5C3E90-E733-40C9-8788-8E75DA4C1CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F521ED13-A895-4288-B2C8-C94745B81761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="8" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="6" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="487">
   <si>
     <t>SPX</t>
   </si>
@@ -1540,6 +1540,12 @@
   </si>
   <si>
     <t>^VVIX</t>
+  </si>
+  <si>
+    <t>^COR3M</t>
+  </si>
+  <si>
+    <t>Cboe Implied Correlation Index</t>
   </si>
 </sst>
 </file>
@@ -1880,7 +1886,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:O80" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:O81" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="26"/>
@@ -3663,7 +3669,9 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4686,7 +4694,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4805,7 +4813,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4926,7 +4934,7 @@
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:I25"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10422,13 +10430,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:T80"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10540,7 +10548,7 @@
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" t="b" cm="1">
-        <f t="array" ref="Q2:Q80">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
+        <f t="array" ref="Q2:Q81">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
         <v>1</v>
       </c>
     </row>
@@ -14077,30 +14085,32 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>446</v>
+        <v>476</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>429</v>
+        <v>485</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
+      <c r="F75" s="4" t="s">
+        <v>486</v>
+      </c>
       <c r="G75" s="4"/>
       <c r="H75" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75" s="4">
         <v>0</v>
       </c>
-      <c r="K75" s="4">
+      <c r="K75" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+        <v>Cboe Implied Correlation Index</v>
       </c>
       <c r="L75" s="4" t="s">
         <v>455</v>
@@ -14110,11 +14120,11 @@
       </c>
       <c r="N75" s="4" cm="1">
         <f t="array" ref="N75">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</f>
-        <v>1E-4</v>
+        <v>-1E-4</v>
       </c>
       <c r="O75" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>MWTIX</v>
+        <v>^COR3M</v>
       </c>
       <c r="Q75" t="b">
         <v>0</v>
@@ -14122,13 +14132,13 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -14141,14 +14151,14 @@
         <v>1</v>
       </c>
       <c r="J76" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K76" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>0</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="M76" s="4" t="s">
         <v>454</v>
@@ -14159,9 +14169,8 @@
       </c>
       <c r="O76" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>TRUMP</v>
-      </c>
-      <c r="P76" s="2"/>
+        <v>MWTIX</v>
+      </c>
       <c r="Q76" t="b">
         <v>0</v>
       </c>
@@ -14174,7 +14183,7 @@
         <v>40</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -14205,8 +14214,9 @@
       </c>
       <c r="O77" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>FED</v>
-      </c>
+        <v>TRUMP</v>
+      </c>
+      <c r="P77" s="2"/>
       <c r="Q77" t="b">
         <v>1</v>
       </c>
@@ -14219,7 +14229,7 @@
         <v>40</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -14250,7 +14260,7 @@
       </c>
       <c r="O78" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="Q78" t="b">
         <v>0</v>
@@ -14264,7 +14274,7 @@
         <v>40</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>450</v>
+        <v>421</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -14295,7 +14305,7 @@
       </c>
       <c r="O79" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="Q79" t="b">
         <v>0</v>
@@ -14309,7 +14319,7 @@
         <v>40</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -14340,15 +14350,60 @@
       </c>
       <c r="O80" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
+        <v>GEOPOLITICS</v>
+      </c>
+      <c r="Q80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4">
+        <v>1</v>
+      </c>
+      <c r="I81" s="4">
+        <v>1</v>
+      </c>
+      <c r="J81" s="4">
+        <v>1</v>
+      </c>
+      <c r="K81" s="4">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>0</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="M81" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="N81" s="4" cm="1">
+        <f t="array" ref="N81">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="O81" s="4" t="str">
+        <f>data[[#This Row],[factor_name]]</f>
         <v>2s10s</v>
       </c>
-      <c r="Q80" t="b">
-        <v>1</v>
+      <c r="Q81" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:O80">
+  <conditionalFormatting sqref="A2:O81">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>$Q2</formula>
     </cfRule>
@@ -14536,8 +14591,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add factor master report, improve date management, add MDS date picker
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95AA32E-E77E-4036-8F15-4DF88BE88C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7615A30A-96D3-4F03-9908-EA719A7D088A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="8" activeTab="9" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="6" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="491">
   <si>
     <t>SPX</t>
   </si>
@@ -1555,6 +1555,12 @@
   </si>
   <si>
     <t>TCW</t>
+  </si>
+  <si>
+    <t>Vanguard Short-Term Bond Index Fund ETF</t>
+  </si>
+  <si>
+    <t>Investment-grade short-dated bonds</t>
   </si>
 </sst>
 </file>
@@ -3679,9 +3685,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9123E77-EA56-403E-A728-B01259D22573}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3722,11 +3728,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A59">_xlfn._xlws.FILTER(data[factor_name],(data[Active])*(data[source]="yfinance"))</f>
+        <f t="array" ref="A2:A60">_xlfn._xlws.FILTER(data[factor_name],(data[Active])*(data[source]="yfinance"))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J59">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J60">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -4826,8 +4832,8 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
-        <v>0</v>
+      <c r="F36" t="str">
+        <v>Vanguard Short-Term Bond Index Fund ETF</v>
       </c>
       <c r="G36" t="str">
         <v>yfinance</v>
@@ -4876,7 +4882,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="B38" t="str">
         <v>Credit</v>
@@ -4885,7 +4891,7 @@
         <v>USD</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -4897,7 +4903,7 @@
         <v>yfinance</v>
       </c>
       <c r="H38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="I38" t="str">
         <v>lognormal</v>
@@ -4908,7 +4914,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="B39" t="str">
         <v>Credit</v>
@@ -4929,7 +4935,7 @@
         <v>yfinance</v>
       </c>
       <c r="H39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="I39" t="str">
         <v>lognormal</v>
@@ -4940,10 +4946,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="B40" t="str">
-        <v>Rates</v>
+        <v>Credit</v>
       </c>
       <c r="C40" t="str">
         <v>USD</v>
@@ -4961,18 +4967,18 @@
         <v>yfinance</v>
       </c>
       <c r="H40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="I40" t="str">
-        <v>normal</v>
+        <v>lognormal</v>
       </c>
       <c r="J40">
-        <v>-0.01</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="B41" t="str">
         <v>Rates</v>
@@ -4986,25 +4992,25 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      <c r="F41">
+        <v>0</v>
       </c>
       <c r="G41" t="str">
         <v>yfinance</v>
       </c>
       <c r="H41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="I41" t="str">
-        <v>lognormal</v>
+        <v>normal</v>
       </c>
       <c r="J41">
-        <v>1E-4</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="B42" t="str">
         <v>Rates</v>
@@ -5019,13 +5025,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>iShares 1-3 Year Treasury Bond ETF</v>
       </c>
       <c r="G42" t="str">
         <v>yfinance</v>
       </c>
       <c r="H42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="I42" t="str">
         <v>lognormal</v>
@@ -5036,7 +5042,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="B43" t="str">
         <v>Rates</v>
@@ -5045,19 +5051,19 @@
         <v>USD</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>iShares 3-7 Year Treasury Bond ETF</v>
       </c>
       <c r="G43" t="str">
         <v>yfinance</v>
       </c>
       <c r="H43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="I43" t="str">
         <v>lognormal</v>
@@ -5068,7 +5074,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="B44" t="str">
         <v>Rates</v>
@@ -5077,19 +5083,19 @@
         <v>USD</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>iShares 7-10 Year Treasury Bond ETF</v>
       </c>
       <c r="G44" t="str">
         <v>yfinance</v>
       </c>
       <c r="H44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="I44" t="str">
         <v>lognormal</v>
@@ -5100,7 +5106,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="B45" t="str">
         <v>Rates</v>
@@ -5115,13 +5121,13 @@
         <v>0</v>
       </c>
       <c r="F45" t="str">
-        <v>iShares TIPS Bond ETF</v>
+        <v>iShares 20+ Year Treasury Bond ETF</v>
       </c>
       <c r="G45" t="str">
         <v>yfinance</v>
       </c>
       <c r="H45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="I45" t="str">
         <v>lognormal</v>
@@ -5132,7 +5138,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="B46" t="str">
         <v>Rates</v>
@@ -5146,14 +5152,14 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="str">
+        <v>iShares TIPS Bond ETF</v>
       </c>
       <c r="G46" t="str">
         <v>yfinance</v>
       </c>
       <c r="H46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="I46" t="str">
         <v>lognormal</v>
@@ -5164,7 +5170,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="B47" t="str">
         <v>Rates</v>
@@ -5178,14 +5184,14 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" t="str">
-        <v>AGNC Investment Corp.</v>
+      <c r="F47">
+        <v>0</v>
       </c>
       <c r="G47" t="str">
         <v>yfinance</v>
       </c>
       <c r="H47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="I47" t="str">
         <v>lognormal</v>
@@ -5196,7 +5202,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="B48" t="str">
         <v>Rates</v>
@@ -5210,14 +5216,14 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="str">
+        <v>AGNC Investment Corp.</v>
       </c>
       <c r="G48" t="str">
         <v>yfinance</v>
       </c>
       <c r="H48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="I48" t="str">
         <v>lognormal</v>
@@ -5228,7 +5234,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="B49" t="str">
         <v>Rates</v>
@@ -5249,7 +5255,7 @@
         <v>yfinance</v>
       </c>
       <c r="H49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="I49" t="str">
         <v>lognormal</v>
@@ -5260,13 +5266,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="B50" t="str">
         <v>Rates</v>
       </c>
       <c r="C50" t="str">
-        <v>EM</v>
+        <v>USD</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -5274,14 +5280,14 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50" t="str">
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      <c r="F50">
+        <v>0</v>
       </c>
       <c r="G50" t="str">
         <v>yfinance</v>
       </c>
       <c r="H50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="I50" t="str">
         <v>lognormal</v>
@@ -5292,13 +5298,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="B51" t="str">
-        <v>Commodities</v>
+        <v>Rates</v>
       </c>
       <c r="C51" t="str">
-        <v>USD</v>
+        <v>EM</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -5307,13 +5313,13 @@
         <v>0</v>
       </c>
       <c r="F51" t="str">
-        <v>SPDR Gold Shares</v>
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
       </c>
       <c r="G51" t="str">
         <v>yfinance</v>
       </c>
       <c r="H51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="I51" t="str">
         <v>lognormal</v>
@@ -5324,7 +5330,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="B52" t="str">
         <v>Commodities</v>
@@ -5339,13 +5345,13 @@
         <v>0</v>
       </c>
       <c r="F52" t="str">
-        <v>iShares Silver Trust</v>
+        <v>SPDR Gold Shares</v>
       </c>
       <c r="G52" t="str">
         <v>yfinance</v>
       </c>
       <c r="H52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="I52" t="str">
         <v>lognormal</v>
@@ -5356,7 +5362,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="B53" t="str">
         <v>Commodities</v>
@@ -5371,13 +5377,13 @@
         <v>0</v>
       </c>
       <c r="F53" t="str">
-        <v>United States Oil Fund</v>
+        <v>iShares Silver Trust</v>
       </c>
       <c r="G53" t="str">
         <v>yfinance</v>
       </c>
       <c r="H53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="I53" t="str">
         <v>lognormal</v>
@@ -5388,10 +5394,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="B54" t="str">
-        <v>Currencies</v>
+        <v>Commodities</v>
       </c>
       <c r="C54" t="str">
         <v>USD</v>
@@ -5403,13 +5409,13 @@
         <v>0</v>
       </c>
       <c r="F54" t="str">
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
+        <v>United States Oil Fund</v>
       </c>
       <c r="G54" t="str">
         <v>yfinance</v>
       </c>
       <c r="H54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="I54" t="str">
         <v>lognormal</v>
@@ -5420,13 +5426,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="B55" t="str">
         <v>Currencies</v>
       </c>
       <c r="C55" t="str">
-        <v>EUR</v>
+        <v>USD</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -5435,13 +5441,13 @@
         <v>0</v>
       </c>
       <c r="F55" t="str">
-        <v>Invesco CurrencyShares Euro Trust</v>
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
       </c>
       <c r="G55" t="str">
         <v>yfinance</v>
       </c>
       <c r="H55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="I55" t="str">
         <v>lognormal</v>
@@ -5452,13 +5458,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="B56" t="str">
         <v>Currencies</v>
       </c>
       <c r="C56" t="str">
-        <v>JPY</v>
+        <v>EUR</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -5467,13 +5473,13 @@
         <v>0</v>
       </c>
       <c r="F56" t="str">
-        <v>Invesco CurrencyShares Japanese Yen Trust</v>
+        <v>Invesco CurrencyShares Euro Trust</v>
       </c>
       <c r="G56" t="str">
         <v>yfinance</v>
       </c>
       <c r="H56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="I56" t="str">
         <v>lognormal</v>
@@ -5484,13 +5490,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="B57" t="str">
-        <v>Vol</v>
+        <v>Currencies</v>
       </c>
       <c r="C57" t="str">
-        <v>USD</v>
+        <v>JPY</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -5499,24 +5505,24 @@
         <v>0</v>
       </c>
       <c r="F57" t="str">
-        <v>CBOE Volatility Index</v>
+        <v>Invesco CurrencyShares Japanese Yen Trust</v>
       </c>
       <c r="G57" t="str">
         <v>yfinance</v>
       </c>
       <c r="H57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="I57" t="str">
         <v>lognormal</v>
       </c>
       <c r="J57">
-        <v>-1E-4</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="B58" t="str">
         <v>Vol</v>
@@ -5531,13 +5537,13 @@
         <v>0</v>
       </c>
       <c r="F58" t="str">
-        <v>ICE BofAML MOVE Index</v>
+        <v>CBOE Volatility Index</v>
       </c>
       <c r="G58" t="str">
         <v>yfinance</v>
       </c>
       <c r="H58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="I58" t="str">
         <v>lognormal</v>
@@ -5548,33 +5554,65 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
-        <v>MWTIX</v>
+        <v>^MOVE</v>
       </c>
       <c r="B59" t="str">
-        <v>Portfolio</v>
+        <v>Vol</v>
       </c>
       <c r="C59" t="str">
         <v>USD</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59">
-        <v>0</v>
+      <c r="F59" t="str">
+        <v>ICE BofAML MOVE Index</v>
       </c>
       <c r="G59" t="str">
         <v>yfinance</v>
       </c>
       <c r="H59" t="str">
-        <v>MWTIX</v>
+        <v>^MOVE</v>
       </c>
       <c r="I59" t="str">
         <v>lognormal</v>
       </c>
       <c r="J59">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="str">
+        <v>MWTIX</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Portfolio</v>
+      </c>
+      <c r="C60" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H60" t="str">
+        <v>MWTIX</v>
+      </c>
+      <c r="I60" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J60">
         <v>1E-4</v>
       </c>
     </row>
@@ -5586,7 +5624,7 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5631,11 +5669,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A63">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
+        <f t="array" ref="A2:A64">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J63">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J64">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -6735,8 +6773,8 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
-        <v>0</v>
+      <c r="F36" t="str">
+        <v>Vanguard Short-Term Bond Index Fund ETF</v>
       </c>
       <c r="G36" t="str">
         <v>yfinance</v>
@@ -6785,7 +6823,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="B38" t="str">
         <v>Credit</v>
@@ -6794,7 +6832,7 @@
         <v>USD</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -6806,7 +6844,7 @@
         <v>yfinance</v>
       </c>
       <c r="H38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="I38" t="str">
         <v>lognormal</v>
@@ -6817,7 +6855,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="B39" t="str">
         <v>Credit</v>
@@ -6838,7 +6876,7 @@
         <v>yfinance</v>
       </c>
       <c r="H39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="I39" t="str">
         <v>lognormal</v>
@@ -6849,10 +6887,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="B40" t="str">
-        <v>Rates</v>
+        <v>Credit</v>
       </c>
       <c r="C40" t="str">
         <v>USD</v>
@@ -6870,18 +6908,18 @@
         <v>yfinance</v>
       </c>
       <c r="H40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="I40" t="str">
-        <v>normal</v>
+        <v>lognormal</v>
       </c>
       <c r="J40">
-        <v>-0.01</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="B41" t="str">
         <v>Rates</v>
@@ -6895,25 +6933,25 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      <c r="F41">
+        <v>0</v>
       </c>
       <c r="G41" t="str">
         <v>yfinance</v>
       </c>
       <c r="H41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="I41" t="str">
-        <v>lognormal</v>
+        <v>normal</v>
       </c>
       <c r="J41">
-        <v>1E-4</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="B42" t="str">
         <v>Rates</v>
@@ -6928,13 +6966,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>iShares 1-3 Year Treasury Bond ETF</v>
       </c>
       <c r="G42" t="str">
         <v>yfinance</v>
       </c>
       <c r="H42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="I42" t="str">
         <v>lognormal</v>
@@ -6945,7 +6983,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="B43" t="str">
         <v>Rates</v>
@@ -6954,19 +6992,19 @@
         <v>USD</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>iShares 3-7 Year Treasury Bond ETF</v>
       </c>
       <c r="G43" t="str">
         <v>yfinance</v>
       </c>
       <c r="H43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="I43" t="str">
         <v>lognormal</v>
@@ -6977,7 +7015,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="B44" t="str">
         <v>Rates</v>
@@ -6986,19 +7024,19 @@
         <v>USD</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>iShares 7-10 Year Treasury Bond ETF</v>
       </c>
       <c r="G44" t="str">
         <v>yfinance</v>
       </c>
       <c r="H44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="I44" t="str">
         <v>lognormal</v>
@@ -7009,7 +7047,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="B45" t="str">
         <v>Rates</v>
@@ -7024,13 +7062,13 @@
         <v>0</v>
       </c>
       <c r="F45" t="str">
-        <v>iShares TIPS Bond ETF</v>
+        <v>iShares 20+ Year Treasury Bond ETF</v>
       </c>
       <c r="G45" t="str">
         <v>yfinance</v>
       </c>
       <c r="H45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="I45" t="str">
         <v>lognormal</v>
@@ -7041,7 +7079,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="B46" t="str">
         <v>Rates</v>
@@ -7055,14 +7093,14 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="str">
+        <v>iShares TIPS Bond ETF</v>
       </c>
       <c r="G46" t="str">
         <v>yfinance</v>
       </c>
       <c r="H46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="I46" t="str">
         <v>lognormal</v>
@@ -7073,7 +7111,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="B47" t="str">
         <v>Rates</v>
@@ -7087,14 +7125,14 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" t="str">
-        <v>AGNC Investment Corp.</v>
+      <c r="F47">
+        <v>0</v>
       </c>
       <c r="G47" t="str">
         <v>yfinance</v>
       </c>
       <c r="H47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="I47" t="str">
         <v>lognormal</v>
@@ -7105,7 +7143,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="B48" t="str">
         <v>Rates</v>
@@ -7119,14 +7157,14 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="str">
+        <v>AGNC Investment Corp.</v>
       </c>
       <c r="G48" t="str">
         <v>yfinance</v>
       </c>
       <c r="H48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="I48" t="str">
         <v>lognormal</v>
@@ -7137,7 +7175,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="B49" t="str">
         <v>Rates</v>
@@ -7158,7 +7196,7 @@
         <v>yfinance</v>
       </c>
       <c r="H49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="I49" t="str">
         <v>lognormal</v>
@@ -7169,13 +7207,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="B50" t="str">
         <v>Rates</v>
       </c>
       <c r="C50" t="str">
-        <v>EM</v>
+        <v>USD</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -7183,14 +7221,14 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50" t="str">
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      <c r="F50">
+        <v>0</v>
       </c>
       <c r="G50" t="str">
         <v>yfinance</v>
       </c>
       <c r="H50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="I50" t="str">
         <v>lognormal</v>
@@ -7201,13 +7239,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="B51" t="str">
-        <v>Commodities</v>
+        <v>Rates</v>
       </c>
       <c r="C51" t="str">
-        <v>USD</v>
+        <v>EM</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -7216,13 +7254,13 @@
         <v>0</v>
       </c>
       <c r="F51" t="str">
-        <v>SPDR Gold Shares</v>
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
       </c>
       <c r="G51" t="str">
         <v>yfinance</v>
       </c>
       <c r="H51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="I51" t="str">
         <v>lognormal</v>
@@ -7233,7 +7271,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="B52" t="str">
         <v>Commodities</v>
@@ -7248,13 +7286,13 @@
         <v>0</v>
       </c>
       <c r="F52" t="str">
-        <v>iShares Silver Trust</v>
+        <v>SPDR Gold Shares</v>
       </c>
       <c r="G52" t="str">
         <v>yfinance</v>
       </c>
       <c r="H52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="I52" t="str">
         <v>lognormal</v>
@@ -7265,7 +7303,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="B53" t="str">
         <v>Commodities</v>
@@ -7280,13 +7318,13 @@
         <v>0</v>
       </c>
       <c r="F53" t="str">
-        <v>United States Oil Fund</v>
+        <v>iShares Silver Trust</v>
       </c>
       <c r="G53" t="str">
         <v>yfinance</v>
       </c>
       <c r="H53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="I53" t="str">
         <v>lognormal</v>
@@ -7297,10 +7335,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="B54" t="str">
-        <v>Currencies</v>
+        <v>Commodities</v>
       </c>
       <c r="C54" t="str">
         <v>USD</v>
@@ -7312,13 +7350,13 @@
         <v>0</v>
       </c>
       <c r="F54" t="str">
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
+        <v>United States Oil Fund</v>
       </c>
       <c r="G54" t="str">
         <v>yfinance</v>
       </c>
       <c r="H54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="I54" t="str">
         <v>lognormal</v>
@@ -7329,13 +7367,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="B55" t="str">
         <v>Currencies</v>
       </c>
       <c r="C55" t="str">
-        <v>EUR</v>
+        <v>USD</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -7344,13 +7382,13 @@
         <v>0</v>
       </c>
       <c r="F55" t="str">
-        <v>Invesco CurrencyShares Euro Trust</v>
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
       </c>
       <c r="G55" t="str">
         <v>yfinance</v>
       </c>
       <c r="H55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="I55" t="str">
         <v>lognormal</v>
@@ -7361,13 +7399,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="B56" t="str">
         <v>Currencies</v>
       </c>
       <c r="C56" t="str">
-        <v>JPY</v>
+        <v>EUR</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -7376,13 +7414,13 @@
         <v>0</v>
       </c>
       <c r="F56" t="str">
-        <v>Invesco CurrencyShares Japanese Yen Trust</v>
+        <v>Invesco CurrencyShares Euro Trust</v>
       </c>
       <c r="G56" t="str">
         <v>yfinance</v>
       </c>
       <c r="H56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="I56" t="str">
         <v>lognormal</v>
@@ -7393,13 +7431,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="B57" t="str">
-        <v>Vol</v>
+        <v>Currencies</v>
       </c>
       <c r="C57" t="str">
-        <v>USD</v>
+        <v>JPY</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -7408,24 +7446,24 @@
         <v>0</v>
       </c>
       <c r="F57" t="str">
-        <v>CBOE Volatility Index</v>
+        <v>Invesco CurrencyShares Japanese Yen Trust</v>
       </c>
       <c r="G57" t="str">
         <v>yfinance</v>
       </c>
       <c r="H57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="I57" t="str">
         <v>lognormal</v>
       </c>
       <c r="J57">
-        <v>-1E-4</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="B58" t="str">
         <v>Vol</v>
@@ -7440,13 +7478,13 @@
         <v>0</v>
       </c>
       <c r="F58" t="str">
-        <v>ICE BofAML MOVE Index</v>
+        <v>CBOE Volatility Index</v>
       </c>
       <c r="G58" t="str">
         <v>yfinance</v>
       </c>
       <c r="H58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="I58" t="str">
         <v>lognormal</v>
@@ -7457,39 +7495,39 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
-        <v>TRUMP</v>
+        <v>^MOVE</v>
       </c>
       <c r="B59" t="str">
-        <v>Theme</v>
+        <v>Vol</v>
       </c>
       <c r="C59" t="str">
         <v>USD</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F59" t="str">
+        <v>ICE BofAML MOVE Index</v>
       </c>
       <c r="G59" t="str">
-        <v>composite</v>
+        <v>yfinance</v>
       </c>
       <c r="H59" t="str">
-        <v>TRUMP</v>
+        <v>^MOVE</v>
       </c>
       <c r="I59" t="str">
         <v>lognormal</v>
       </c>
       <c r="J59">
-        <v>1E-4</v>
+        <v>-1E-4</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="B60" t="str">
         <v>Theme</v>
@@ -7510,7 +7548,7 @@
         <v>composite</v>
       </c>
       <c r="H60" t="str">
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="I60" t="str">
         <v>lognormal</v>
@@ -7521,7 +7559,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="B61" t="str">
         <v>Theme</v>
@@ -7542,7 +7580,7 @@
         <v>composite</v>
       </c>
       <c r="H61" t="str">
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="I61" t="str">
         <v>lognormal</v>
@@ -7553,7 +7591,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="B62" t="str">
         <v>Theme</v>
@@ -7574,7 +7612,7 @@
         <v>composite</v>
       </c>
       <c r="H62" t="str">
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="I62" t="str">
         <v>lognormal</v>
@@ -7585,7 +7623,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="B63" t="str">
         <v>Theme</v>
@@ -7606,12 +7644,44 @@
         <v>composite</v>
       </c>
       <c r="H63" t="str">
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="I63" t="str">
         <v>lognormal</v>
       </c>
       <c r="J63">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C64" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H64" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="I64" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J64">
         <v>1E-4</v>
       </c>
     </row>
@@ -7840,7 +7910,7 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -7870,11 +7940,11 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A59">_xlfn._xlws.FILTER(data[factor_name],data[Active]*NOT(data[composite]))</f>
+        <f t="array" ref="A2:A60">_xlfn._xlws.FILTER(data[factor_name],data[Active]*NOT(data[composite]))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:E59">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:E1,data[#Headers]))</f>
+        <f t="array" ref="B2:E60">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:E1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -8461,8 +8531,8 @@
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="E36">
-        <v>0</v>
+      <c r="E36" t="str">
+        <v>Vanguard Short-Term Bond Index Fund ETF</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -8484,7 +8554,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="B38" t="str">
         <v>Credit</v>
@@ -8493,7 +8563,7 @@
         <v>USD</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -8501,7 +8571,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="B39" t="str">
         <v>Credit</v>
@@ -8518,10 +8588,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="B40" t="str">
-        <v>Rates</v>
+        <v>Credit</v>
       </c>
       <c r="C40" t="str">
         <v>USD</v>
@@ -8535,7 +8605,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="B41" t="str">
         <v>Rates</v>
@@ -8546,13 +8616,13 @@
       <c r="D41">
         <v>0</v>
       </c>
-      <c r="E41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      <c r="E41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="B42" t="str">
         <v>Rates</v>
@@ -8564,12 +8634,12 @@
         <v>0</v>
       </c>
       <c r="E42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>iShares 1-3 Year Treasury Bond ETF</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="B43" t="str">
         <v>Rates</v>
@@ -8578,15 +8648,15 @@
         <v>USD</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>iShares 3-7 Year Treasury Bond ETF</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="B44" t="str">
         <v>Rates</v>
@@ -8595,15 +8665,15 @@
         <v>USD</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>iShares 7-10 Year Treasury Bond ETF</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="B45" t="str">
         <v>Rates</v>
@@ -8615,12 +8685,12 @@
         <v>0</v>
       </c>
       <c r="E45" t="str">
-        <v>iShares TIPS Bond ETF</v>
+        <v>iShares 20+ Year Treasury Bond ETF</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="B46" t="str">
         <v>Rates</v>
@@ -8631,13 +8701,13 @@
       <c r="D46">
         <v>0</v>
       </c>
-      <c r="E46">
-        <v>0</v>
+      <c r="E46" t="str">
+        <v>iShares TIPS Bond ETF</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="B47" t="str">
         <v>Rates</v>
@@ -8648,13 +8718,13 @@
       <c r="D47">
         <v>0</v>
       </c>
-      <c r="E47" t="str">
-        <v>AGNC Investment Corp.</v>
+      <c r="E47">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="B48" t="str">
         <v>Rates</v>
@@ -8665,13 +8735,13 @@
       <c r="D48">
         <v>0</v>
       </c>
-      <c r="E48">
-        <v>0</v>
+      <c r="E48" t="str">
+        <v>AGNC Investment Corp.</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="B49" t="str">
         <v>Rates</v>
@@ -8688,41 +8758,41 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="B50" t="str">
         <v>Rates</v>
       </c>
       <c r="C50" t="str">
-        <v>EM</v>
+        <v>USD</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
-      <c r="E50" t="str">
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      <c r="E50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="B51" t="str">
-        <v>Commodities</v>
+        <v>Rates</v>
       </c>
       <c r="C51" t="str">
-        <v>USD</v>
+        <v>EM</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51" t="str">
-        <v>SPDR Gold Shares</v>
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="B52" t="str">
         <v>Commodities</v>
@@ -8734,12 +8804,12 @@
         <v>0</v>
       </c>
       <c r="E52" t="str">
-        <v>iShares Silver Trust</v>
+        <v>SPDR Gold Shares</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="B53" t="str">
         <v>Commodities</v>
@@ -8751,15 +8821,15 @@
         <v>0</v>
       </c>
       <c r="E53" t="str">
-        <v>United States Oil Fund</v>
+        <v>iShares Silver Trust</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="B54" t="str">
-        <v>Currencies</v>
+        <v>Commodities</v>
       </c>
       <c r="C54" t="str">
         <v>USD</v>
@@ -8768,63 +8838,63 @@
         <v>0</v>
       </c>
       <c r="E54" t="str">
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
+        <v>United States Oil Fund</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="B55" t="str">
         <v>Currencies</v>
       </c>
       <c r="C55" t="str">
-        <v>EUR</v>
+        <v>USD</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55" t="str">
-        <v>Invesco CurrencyShares Euro Trust</v>
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="B56" t="str">
         <v>Currencies</v>
       </c>
       <c r="C56" t="str">
-        <v>JPY</v>
+        <v>EUR</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56" t="str">
-        <v>Invesco CurrencyShares Japanese Yen Trust</v>
+        <v>Invesco CurrencyShares Euro Trust</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="B57" t="str">
-        <v>Vol</v>
+        <v>Currencies</v>
       </c>
       <c r="C57" t="str">
-        <v>USD</v>
+        <v>JPY</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57" t="str">
-        <v>CBOE Volatility Index</v>
+        <v>Invesco CurrencyShares Japanese Yen Trust</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="B58" t="str">
         <v>Vol</v>
@@ -8836,23 +8906,40 @@
         <v>0</v>
       </c>
       <c r="E58" t="str">
-        <v>ICE BofAML MOVE Index</v>
+        <v>CBOE Volatility Index</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
-        <v>MWTIX</v>
+        <v>^MOVE</v>
       </c>
       <c r="B59" t="str">
-        <v>Portfolio</v>
+        <v>Vol</v>
       </c>
       <c r="C59" t="str">
         <v>USD</v>
       </c>
       <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="str">
+        <v>ICE BofAML MOVE Index</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="str">
+        <v>MWTIX</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Portfolio</v>
+      </c>
+      <c r="C60" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
         <v>0</v>
       </c>
     </row>
@@ -13870,7 +13957,7 @@
         <v>42</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -14237,7 +14324,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14605,11 +14692,11 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A76" sqref="A76"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16761,8 +16848,12 @@
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>490</v>
+      </c>
       <c r="H41" s="4">
         <v>1</v>
       </c>
@@ -16775,9 +16866,9 @@
       <c r="K41" s="4">
         <v>0</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+        <v>Vanguard Short-Term Bond Index Fund ETF</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>455</v>
@@ -16868,10 +16959,10 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" s="4">
         <v>0</v>
@@ -19002,7 +19093,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A64DEF-E706-4B9C-B282-71F34F86B3DF}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -19047,11 +19138,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A64">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
+        <f t="array" ref="A2:A65">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J64">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J65">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -20151,8 +20242,8 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
-        <v>0</v>
+      <c r="F36" t="str">
+        <v>Vanguard Short-Term Bond Index Fund ETF</v>
       </c>
       <c r="G36" t="str">
         <v>yfinance</v>
@@ -20201,7 +20292,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="B38" t="str">
         <v>Credit</v>
@@ -20210,7 +20301,7 @@
         <v>USD</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -20222,7 +20313,7 @@
         <v>yfinance</v>
       </c>
       <c r="H38" t="str">
-        <v>HYGH</v>
+        <v>LQDH</v>
       </c>
       <c r="I38" t="str">
         <v>lognormal</v>
@@ -20233,7 +20324,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="B39" t="str">
         <v>Credit</v>
@@ -20254,7 +20345,7 @@
         <v>yfinance</v>
       </c>
       <c r="H39" t="str">
-        <v>AGG</v>
+        <v>HYGH</v>
       </c>
       <c r="I39" t="str">
         <v>lognormal</v>
@@ -20265,10 +20356,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="B40" t="str">
-        <v>Rates</v>
+        <v>Credit</v>
       </c>
       <c r="C40" t="str">
         <v>USD</v>
@@ -20286,18 +20377,18 @@
         <v>yfinance</v>
       </c>
       <c r="H40" t="str">
-        <v>^TNX</v>
+        <v>AGG</v>
       </c>
       <c r="I40" t="str">
-        <v>normal</v>
+        <v>lognormal</v>
       </c>
       <c r="J40">
-        <v>-0.01</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="B41" t="str">
         <v>Rates</v>
@@ -20311,25 +20402,25 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      <c r="F41">
+        <v>0</v>
       </c>
       <c r="G41" t="str">
         <v>yfinance</v>
       </c>
       <c r="H41" t="str">
-        <v>SHY</v>
+        <v>^TNX</v>
       </c>
       <c r="I41" t="str">
-        <v>lognormal</v>
+        <v>normal</v>
       </c>
       <c r="J41">
-        <v>1E-4</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="B42" t="str">
         <v>Rates</v>
@@ -20344,13 +20435,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>iShares 1-3 Year Treasury Bond ETF</v>
       </c>
       <c r="G42" t="str">
         <v>yfinance</v>
       </c>
       <c r="H42" t="str">
-        <v>IEI</v>
+        <v>SHY</v>
       </c>
       <c r="I42" t="str">
         <v>lognormal</v>
@@ -20361,7 +20452,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="B43" t="str">
         <v>Rates</v>
@@ -20370,19 +20461,19 @@
         <v>USD</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>iShares 3-7 Year Treasury Bond ETF</v>
       </c>
       <c r="G43" t="str">
         <v>yfinance</v>
       </c>
       <c r="H43" t="str">
-        <v>IEF</v>
+        <v>IEI</v>
       </c>
       <c r="I43" t="str">
         <v>lognormal</v>
@@ -20393,7 +20484,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="B44" t="str">
         <v>Rates</v>
@@ -20402,19 +20493,19 @@
         <v>USD</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>iShares 7-10 Year Treasury Bond ETF</v>
       </c>
       <c r="G44" t="str">
         <v>yfinance</v>
       </c>
       <c r="H44" t="str">
-        <v>TLT</v>
+        <v>IEF</v>
       </c>
       <c r="I44" t="str">
         <v>lognormal</v>
@@ -20425,7 +20516,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="B45" t="str">
         <v>Rates</v>
@@ -20440,13 +20531,13 @@
         <v>0</v>
       </c>
       <c r="F45" t="str">
-        <v>iShares TIPS Bond ETF</v>
+        <v>iShares 20+ Year Treasury Bond ETF</v>
       </c>
       <c r="G45" t="str">
         <v>yfinance</v>
       </c>
       <c r="H45" t="str">
-        <v>TIP</v>
+        <v>TLT</v>
       </c>
       <c r="I45" t="str">
         <v>lognormal</v>
@@ -20457,7 +20548,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="B46" t="str">
         <v>Rates</v>
@@ -20471,14 +20562,14 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="str">
+        <v>iShares TIPS Bond ETF</v>
       </c>
       <c r="G46" t="str">
         <v>yfinance</v>
       </c>
       <c r="H46" t="str">
-        <v>VTIP</v>
+        <v>TIP</v>
       </c>
       <c r="I46" t="str">
         <v>lognormal</v>
@@ -20489,7 +20580,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="B47" t="str">
         <v>Rates</v>
@@ -20503,14 +20594,14 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" t="str">
-        <v>AGNC Investment Corp.</v>
+      <c r="F47">
+        <v>0</v>
       </c>
       <c r="G47" t="str">
         <v>yfinance</v>
       </c>
       <c r="H47" t="str">
-        <v>AGNC</v>
+        <v>VTIP</v>
       </c>
       <c r="I47" t="str">
         <v>lognormal</v>
@@ -20521,7 +20612,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="B48" t="str">
         <v>Rates</v>
@@ -20535,14 +20626,14 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="str">
+        <v>AGNC Investment Corp.</v>
       </c>
       <c r="G48" t="str">
         <v>yfinance</v>
       </c>
       <c r="H48" t="str">
-        <v>VMBS</v>
+        <v>AGNC</v>
       </c>
       <c r="I48" t="str">
         <v>lognormal</v>
@@ -20553,7 +20644,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="B49" t="str">
         <v>Rates</v>
@@ -20574,7 +20665,7 @@
         <v>yfinance</v>
       </c>
       <c r="H49" t="str">
-        <v>CMBS</v>
+        <v>VMBS</v>
       </c>
       <c r="I49" t="str">
         <v>lognormal</v>
@@ -20585,13 +20676,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="B50" t="str">
         <v>Rates</v>
       </c>
       <c r="C50" t="str">
-        <v>EM</v>
+        <v>USD</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -20599,14 +20690,14 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50" t="str">
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      <c r="F50">
+        <v>0</v>
       </c>
       <c r="G50" t="str">
         <v>yfinance</v>
       </c>
       <c r="H50" t="str">
-        <v>EMB</v>
+        <v>CMBS</v>
       </c>
       <c r="I50" t="str">
         <v>lognormal</v>
@@ -20617,13 +20708,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="B51" t="str">
-        <v>Commodities</v>
+        <v>Rates</v>
       </c>
       <c r="C51" t="str">
-        <v>USD</v>
+        <v>EM</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -20632,13 +20723,13 @@
         <v>0</v>
       </c>
       <c r="F51" t="str">
-        <v>SPDR Gold Shares</v>
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
       </c>
       <c r="G51" t="str">
         <v>yfinance</v>
       </c>
       <c r="H51" t="str">
-        <v>GLD</v>
+        <v>EMB</v>
       </c>
       <c r="I51" t="str">
         <v>lognormal</v>
@@ -20649,7 +20740,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="B52" t="str">
         <v>Commodities</v>
@@ -20664,13 +20755,13 @@
         <v>0</v>
       </c>
       <c r="F52" t="str">
-        <v>iShares Silver Trust</v>
+        <v>SPDR Gold Shares</v>
       </c>
       <c r="G52" t="str">
         <v>yfinance</v>
       </c>
       <c r="H52" t="str">
-        <v>SLV</v>
+        <v>GLD</v>
       </c>
       <c r="I52" t="str">
         <v>lognormal</v>
@@ -20681,7 +20772,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="B53" t="str">
         <v>Commodities</v>
@@ -20696,13 +20787,13 @@
         <v>0</v>
       </c>
       <c r="F53" t="str">
-        <v>United States Oil Fund</v>
+        <v>iShares Silver Trust</v>
       </c>
       <c r="G53" t="str">
         <v>yfinance</v>
       </c>
       <c r="H53" t="str">
-        <v>USO</v>
+        <v>SLV</v>
       </c>
       <c r="I53" t="str">
         <v>lognormal</v>
@@ -20713,10 +20804,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="B54" t="str">
-        <v>Currencies</v>
+        <v>Commodities</v>
       </c>
       <c r="C54" t="str">
         <v>USD</v>
@@ -20728,13 +20819,13 @@
         <v>0</v>
       </c>
       <c r="F54" t="str">
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
+        <v>United States Oil Fund</v>
       </c>
       <c r="G54" t="str">
         <v>yfinance</v>
       </c>
       <c r="H54" t="str">
-        <v>UUP</v>
+        <v>USO</v>
       </c>
       <c r="I54" t="str">
         <v>lognormal</v>
@@ -20745,13 +20836,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="B55" t="str">
         <v>Currencies</v>
       </c>
       <c r="C55" t="str">
-        <v>EUR</v>
+        <v>USD</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -20760,13 +20851,13 @@
         <v>0</v>
       </c>
       <c r="F55" t="str">
-        <v>Invesco CurrencyShares Euro Trust</v>
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
       </c>
       <c r="G55" t="str">
         <v>yfinance</v>
       </c>
       <c r="H55" t="str">
-        <v>FXE</v>
+        <v>UUP</v>
       </c>
       <c r="I55" t="str">
         <v>lognormal</v>
@@ -20777,13 +20868,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="B56" t="str">
         <v>Currencies</v>
       </c>
       <c r="C56" t="str">
-        <v>JPY</v>
+        <v>EUR</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -20792,13 +20883,13 @@
         <v>0</v>
       </c>
       <c r="F56" t="str">
-        <v>Invesco CurrencyShares Japanese Yen Trust</v>
+        <v>Invesco CurrencyShares Euro Trust</v>
       </c>
       <c r="G56" t="str">
         <v>yfinance</v>
       </c>
       <c r="H56" t="str">
-        <v>FXY</v>
+        <v>FXE</v>
       </c>
       <c r="I56" t="str">
         <v>lognormal</v>
@@ -20809,13 +20900,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="B57" t="str">
-        <v>Vol</v>
+        <v>Currencies</v>
       </c>
       <c r="C57" t="str">
-        <v>USD</v>
+        <v>JPY</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -20824,24 +20915,24 @@
         <v>0</v>
       </c>
       <c r="F57" t="str">
-        <v>CBOE Volatility Index</v>
+        <v>Invesco CurrencyShares Japanese Yen Trust</v>
       </c>
       <c r="G57" t="str">
         <v>yfinance</v>
       </c>
       <c r="H57" t="str">
-        <v>^VIX</v>
+        <v>FXY</v>
       </c>
       <c r="I57" t="str">
         <v>lognormal</v>
       </c>
       <c r="J57">
-        <v>-1E-4</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="B58" t="str">
         <v>Vol</v>
@@ -20856,13 +20947,13 @@
         <v>0</v>
       </c>
       <c r="F58" t="str">
-        <v>ICE BofAML MOVE Index</v>
+        <v>CBOE Volatility Index</v>
       </c>
       <c r="G58" t="str">
         <v>yfinance</v>
       </c>
       <c r="H58" t="str">
-        <v>^MOVE</v>
+        <v>^VIX</v>
       </c>
       <c r="I58" t="str">
         <v>lognormal</v>
@@ -20873,42 +20964,42 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
-        <v>MWTIX</v>
+        <v>^MOVE</v>
       </c>
       <c r="B59" t="str">
-        <v>Portfolio</v>
+        <v>Vol</v>
       </c>
       <c r="C59" t="str">
         <v>USD</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59">
-        <v>0</v>
+      <c r="F59" t="str">
+        <v>ICE BofAML MOVE Index</v>
       </c>
       <c r="G59" t="str">
         <v>yfinance</v>
       </c>
       <c r="H59" t="str">
-        <v>MWTIX</v>
+        <v>^MOVE</v>
       </c>
       <c r="I59" t="str">
         <v>lognormal</v>
       </c>
       <c r="J59">
-        <v>1E-4</v>
+        <v>-1E-4</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
-        <v>TRUMP</v>
+        <v>MWTIX</v>
       </c>
       <c r="B60" t="str">
-        <v>Theme</v>
+        <v>Portfolio</v>
       </c>
       <c r="C60" t="str">
         <v>USD</v>
@@ -20917,16 +21008,16 @@
         <v>1</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60" t="str">
-        <v>composite</v>
+        <v>yfinance</v>
       </c>
       <c r="H60" t="str">
-        <v>TRUMP</v>
+        <v>MWTIX</v>
       </c>
       <c r="I60" t="str">
         <v>lognormal</v>
@@ -20937,7 +21028,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="B61" t="str">
         <v>Theme</v>
@@ -20958,7 +21049,7 @@
         <v>composite</v>
       </c>
       <c r="H61" t="str">
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="I61" t="str">
         <v>lognormal</v>
@@ -20969,7 +21060,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="B62" t="str">
         <v>Theme</v>
@@ -20990,7 +21081,7 @@
         <v>composite</v>
       </c>
       <c r="H62" t="str">
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="I62" t="str">
         <v>lognormal</v>
@@ -21001,7 +21092,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="B63" t="str">
         <v>Theme</v>
@@ -21022,7 +21113,7 @@
         <v>composite</v>
       </c>
       <c r="H63" t="str">
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="I63" t="str">
         <v>lognormal</v>
@@ -21033,7 +21124,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="B64" t="str">
         <v>Theme</v>
@@ -21054,12 +21145,44 @@
         <v>composite</v>
       </c>
       <c r="H64" t="str">
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="I64" t="str">
         <v>lognormal</v>
       </c>
       <c r="J64">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C65" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H65" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="I65" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J65">
         <v>1E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: Add corelation matrix
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28910"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\risk_lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A550DB0-E25E-4E50-BFD9-FF4AD6658C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D3B27-D900-4CF7-B22E-26D4426CA9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="11" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="6" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="508">
   <si>
     <t>SPX</t>
   </si>
@@ -1609,6 +1609,9 @@
   </si>
   <si>
     <t>TRADEWAR_OLD</t>
+  </si>
+  <si>
+    <t>Staples/Discretionary</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1704,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="43">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
@@ -1938,8 +1959,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{26B58CFA-74FB-41FD-AB02-EC6D3EA4F4A1}">
-      <tableStyleElement type="wholeTable" dxfId="40"/>
-      <tableStyleElement type="headerRow" dxfId="39"/>
+      <tableStyleElement type="wholeTable" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2024,49 +2045,49 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:Q87" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:Q87" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="29"/>
-    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{494805E4-EBB6-47FD-9BC2-8DAD9FB9D3FA}" name="composite" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{608FE572-4016-436E-8625-08926F3A2371}" name="client" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="31"/>
+    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{494805E4-EBB6-47FD-9BC2-8DAD9FB9D3FA}" name="composite" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{608FE572-4016-436E-8625-08926F3A2371}" name="client" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="27">
       <calculatedColumnFormula>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="22">
+    <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="24">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="21">
+    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="23">
       <calculatedColumnFormula>data[[#This Row],[factor_name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:I45" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="11">
       <calculatedColumnFormula>IF(data_old[[#This Row],[description_override]]="",data_old[[#This Row],[Description_GPT]],data_old[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5843,8 +5864,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8014,8 +8035,8 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68">
-        <v>0</v>
+      <c r="F68" t="str">
+        <v>Staples/Discretionary</v>
       </c>
       <c r="G68" t="str">
         <v>composite</v>
@@ -8071,8 +8092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B51E7A-08A5-4042-86E1-7986ED98437B}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14832,7 +14853,7 @@
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15471,22 +15492,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C14 B15 A15:A16 C15:C16 A28:C31">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>$K2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:C17 B18:C20 A18:A22 C21">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$K17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:C23">
-    <cfRule type="expression" dxfId="6" priority="23">
+    <cfRule type="expression" dxfId="8" priority="23">
       <formula>$K16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 B22:C22">
-    <cfRule type="expression" dxfId="5" priority="21">
+    <cfRule type="expression" dxfId="7" priority="21">
       <formula>$K19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15503,11 +15524,11 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G86" sqref="G86"/>
+      <selection pane="bottomRight" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20022,7 +20043,9 @@
         <v>505</v>
       </c>
       <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
+      <c r="E86" s="4" t="s">
+        <v>507</v>
+      </c>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4">
@@ -20037,9 +20060,9 @@
       <c r="K86" s="4">
         <v>0</v>
       </c>
-      <c r="L86" s="4">
+      <c r="L86" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+        <v>Staples/Discretionary</v>
       </c>
       <c r="M86" s="4" t="s">
         <v>445</v>
@@ -20111,29 +20134,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A86:B86 H86:K86 M86:N86">
-    <cfRule type="expression" dxfId="4" priority="24">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:Q65 A68:Q72">
-    <cfRule type="expression" dxfId="3" priority="8">
+  <conditionalFormatting sqref="A2:Q87">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>$S2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66:Q67">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$S65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73:Q74 A76:Q85 A87:B87 H87:K87 M87:N87">
-    <cfRule type="expression" dxfId="1" priority="12">
-      <formula>$S72</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75:Q75">
-    <cfRule type="expression" dxfId="0" priority="14">
-      <formula>$S73</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22519,8 +22522,8 @@
       <c r="E69">
         <v>1</v>
       </c>
-      <c r="F69">
-        <v>0</v>
+      <c r="F69" t="str">
+        <v>Staples/Discretionary</v>
       </c>
       <c r="G69" t="str">
         <v>composite</v>

</xml_diff>

<commit_message>
feature: Build portflios off factor_set returns. Run summary analysis.
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D3B27-D900-4CF7-B22E-26D4426CA9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED47ED5-05FE-41AE-9505-2FE475557D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="6" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="10" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="508">
   <si>
     <t>SPX</t>
   </si>
@@ -1704,61 +1704,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <border>
         <top style="thin">
@@ -1959,8 +1905,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{26B58CFA-74FB-41FD-AB02-EC6D3EA4F4A1}">
-      <tableStyleElement type="wholeTable" dxfId="42"/>
-      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="wholeTable" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2045,49 +1991,49 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:Q87" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:Q88" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="31"/>
-    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{494805E4-EBB6-47FD-9BC2-8DAD9FB9D3FA}" name="composite" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{608FE572-4016-436E-8625-08926F3A2371}" name="client" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="25"/>
+    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{494805E4-EBB6-47FD-9BC2-8DAD9FB9D3FA}" name="composite" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{608FE572-4016-436E-8625-08926F3A2371}" name="client" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="21">
       <calculatedColumnFormula>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="24">
+    <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="18">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="23">
+    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="17">
       <calculatedColumnFormula>data[[#This Row],[factor_name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:I45" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="5">
       <calculatedColumnFormula>IF(data_old[[#This Row],[description_override]]="",data_old[[#This Row],[Description_GPT]],data_old[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5862,10 +5808,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5907,11 +5853,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A69">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
+        <f t="array" ref="A2:A70">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J69">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J70">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -7861,10 +7807,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
-        <v>TRUMP</v>
+        <v>MWTIX</v>
       </c>
       <c r="B63" t="str">
-        <v>Theme</v>
+        <v>Portfolio</v>
       </c>
       <c r="C63" t="str">
         <v>USD</v>
@@ -7873,16 +7819,16 @@
         <v>1</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63" t="str">
-        <v>composite</v>
+        <v>yfinance</v>
       </c>
       <c r="H63" t="str">
-        <v>TRUMP</v>
+        <v>MWTIX</v>
       </c>
       <c r="I63" t="str">
         <v>lognormal</v>
@@ -7893,7 +7839,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="B64" t="str">
         <v>Theme</v>
@@ -7914,7 +7860,7 @@
         <v>composite</v>
       </c>
       <c r="H64" t="str">
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="I64" t="str">
         <v>lognormal</v>
@@ -7925,7 +7871,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="B65" t="str">
         <v>Theme</v>
@@ -7946,7 +7892,7 @@
         <v>composite</v>
       </c>
       <c r="H65" t="str">
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="I65" t="str">
         <v>lognormal</v>
@@ -7957,7 +7903,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="B66" t="str">
         <v>Theme</v>
@@ -7978,7 +7924,7 @@
         <v>composite</v>
       </c>
       <c r="H66" t="str">
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="I66" t="str">
         <v>lognormal</v>
@@ -7989,7 +7935,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="B67" t="str">
         <v>Theme</v>
@@ -8010,7 +7956,7 @@
         <v>composite</v>
       </c>
       <c r="H67" t="str">
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="I67" t="str">
         <v>lognormal</v>
@@ -8021,7 +7967,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
-        <v>XLPXLY</v>
+        <v>2s10s</v>
       </c>
       <c r="B68" t="str">
         <v>Theme</v>
@@ -8035,14 +7981,14 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68" t="str">
-        <v>Staples/Discretionary</v>
+      <c r="F68">
+        <v>0</v>
       </c>
       <c r="G68" t="str">
         <v>composite</v>
       </c>
       <c r="H68" t="str">
-        <v>XLPXLY</v>
+        <v>2s10s</v>
       </c>
       <c r="I68" t="str">
         <v>lognormal</v>
@@ -8053,7 +7999,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
-        <v>TRADEWAR</v>
+        <v>XLPXLY</v>
       </c>
       <c r="B69" t="str">
         <v>Theme</v>
@@ -8067,19 +8013,51 @@
       <c r="E69">
         <v>1</v>
       </c>
-      <c r="F69">
-        <v>0</v>
+      <c r="F69" t="str">
+        <v>Staples/Discretionary</v>
       </c>
       <c r="G69" t="str">
         <v>composite</v>
       </c>
       <c r="H69" t="str">
-        <v>TRADEWAR</v>
+        <v>XLPXLY</v>
       </c>
       <c r="I69" t="str">
         <v>lognormal</v>
       </c>
       <c r="J69">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" t="str">
+        <v>TRADEWAR</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C70" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H70" t="str">
+        <v>TRADEWAR</v>
+      </c>
+      <c r="I70" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J70">
         <v>1E-4</v>
       </c>
     </row>
@@ -14853,7 +14831,7 @@
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15492,22 +15470,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C14 B15 A15:A16 C15:C16 A28:C31">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$K2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:C17 B18:C20 A18:A22 C21">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$K17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:C23">
-    <cfRule type="expression" dxfId="8" priority="23">
+    <cfRule type="expression" dxfId="2" priority="23">
       <formula>$K16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 B22:C22">
-    <cfRule type="expression" dxfId="7" priority="21">
+    <cfRule type="expression" dxfId="1" priority="21">
       <formula>$K19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15522,13 +15500,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:V87"/>
+  <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K86" sqref="K86"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15651,7 +15629,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="2"/>
       <c r="S2" t="b" cm="1">
-        <f t="array" ref="S2:S87">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
+        <f t="array" ref="S2:S88">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
         <v>1</v>
       </c>
     </row>
@@ -19752,7 +19730,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" s="4">
         <v>1</v>
@@ -19789,13 +19767,13 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>444</v>
+        <v>128</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -19805,10 +19783,10 @@
         <v>1</v>
       </c>
       <c r="I81" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K81" s="4">
         <v>0</v>
@@ -19818,7 +19796,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="N81" s="4" t="s">
         <v>454</v>
@@ -19829,9 +19807,10 @@
       </c>
       <c r="P81" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>TRUMP</v>
+        <v>MWTIX</v>
       </c>
       <c r="Q81" s="4"/>
+      <c r="R81" s="2"/>
       <c r="S81" t="b">
         <v>0</v>
       </c>
@@ -19844,7 +19823,7 @@
         <v>40</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -19878,7 +19857,7 @@
       </c>
       <c r="P82" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>FED</v>
+        <v>TRUMP</v>
       </c>
       <c r="Q82" s="4"/>
       <c r="S82" t="b">
@@ -19893,7 +19872,7 @@
         <v>40</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -19927,7 +19906,7 @@
       </c>
       <c r="P83" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>AI</v>
+        <v>FED</v>
       </c>
       <c r="Q83" s="4"/>
       <c r="S83" t="b">
@@ -19942,7 +19921,7 @@
         <v>40</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>450</v>
+        <v>421</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -19976,7 +19955,7 @@
       </c>
       <c r="P84" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>GEOPOLITICS</v>
+        <v>AI</v>
       </c>
       <c r="Q84" s="4"/>
       <c r="S84" t="b">
@@ -19991,7 +19970,7 @@
         <v>40</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -20025,7 +20004,7 @@
       </c>
       <c r="P85" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>2s10s</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="Q85" s="4"/>
       <c r="S85" t="b">
@@ -20040,12 +20019,10 @@
         <v>40</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>505</v>
+        <v>451</v>
       </c>
       <c r="D86" s="4"/>
-      <c r="E86" s="4" t="s">
-        <v>507</v>
-      </c>
+      <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4">
@@ -20060,9 +20037,9 @@
       <c r="K86" s="4">
         <v>0</v>
       </c>
-      <c r="L86" s="4" t="str">
+      <c r="L86" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>Staples/Discretionary</v>
+        <v>0</v>
       </c>
       <c r="M86" s="4" t="s">
         <v>445</v>
@@ -20076,7 +20053,7 @@
       </c>
       <c r="P86" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>XLPXLY</v>
+        <v>2s10s</v>
       </c>
       <c r="Q86" s="4"/>
       <c r="S86" t="b">
@@ -20091,10 +20068,12 @@
         <v>40</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
+      <c r="E87" s="4" t="s">
+        <v>507</v>
+      </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4">
@@ -20109,9 +20088,9 @@
       <c r="K87" s="4">
         <v>0</v>
       </c>
-      <c r="L87" s="4">
+      <c r="L87" s="4" t="str">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+        <v>Staples/Discretionary</v>
       </c>
       <c r="M87" s="4" t="s">
         <v>445</v>
@@ -20125,17 +20104,66 @@
       </c>
       <c r="P87" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>TRADEWAR</v>
+        <v>XLPXLY</v>
       </c>
       <c r="Q87" s="4"/>
       <c r="S87" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4">
+        <v>1</v>
+      </c>
+      <c r="I88" s="4">
+        <v>1</v>
+      </c>
+      <c r="J88" s="4">
+        <v>1</v>
+      </c>
+      <c r="K88" s="4">
+        <v>0</v>
+      </c>
+      <c r="L88" s="4">
+        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+        <v>0</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="O88" s="4" cm="1">
+        <f t="array" ref="O88">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="P88" s="4" t="str">
+        <f>data[[#This Row],[factor_name]]</f>
+        <v>TRADEWAR</v>
+      </c>
+      <c r="Q88" s="4"/>
+      <c r="S88" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:Q87">
-    <cfRule type="expression" dxfId="1" priority="8">
+  <conditionalFormatting sqref="A2:Q88">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$S2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feature: Add chart shading for VIX regimes to dashboard
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D930531-FE02-432C-B6C7-7C1F4D5D5DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09EDC06-1857-4B48-9FBC-1E601EC30C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="9" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="7" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -19,16 +19,17 @@
     <sheet name="lior" sheetId="9" r:id="rId4"/>
     <sheet name="read_composites" sheetId="14" r:id="rId5"/>
     <sheet name="composites" sheetId="13" r:id="rId6"/>
-    <sheet name="data" sheetId="3" r:id="rId7"/>
-    <sheet name="read_new" sheetId="15" r:id="rId8"/>
-    <sheet name="read_tcw" sheetId="17" r:id="rId9"/>
-    <sheet name="read_nocomposite" sheetId="19" r:id="rId10"/>
-    <sheet name="read" sheetId="12" r:id="rId11"/>
-    <sheet name="read_short" sheetId="16" r:id="rId12"/>
-    <sheet name="read_old2" sheetId="4" r:id="rId13"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId14"/>
-    <sheet name="read_old" sheetId="1" r:id="rId15"/>
-    <sheet name="data_old" sheetId="8" r:id="rId16"/>
+    <sheet name="risk_parity" sheetId="20" r:id="rId7"/>
+    <sheet name="data" sheetId="3" r:id="rId8"/>
+    <sheet name="read_new" sheetId="15" r:id="rId9"/>
+    <sheet name="read_tcw" sheetId="17" r:id="rId10"/>
+    <sheet name="read_nocomposite" sheetId="19" r:id="rId11"/>
+    <sheet name="read" sheetId="12" r:id="rId12"/>
+    <sheet name="read_short" sheetId="16" r:id="rId13"/>
+    <sheet name="read_old2" sheetId="4" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId15"/>
+    <sheet name="read_old" sheetId="1" r:id="rId16"/>
+    <sheet name="data_old" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="508">
   <si>
     <t>SPX</t>
   </si>
@@ -3772,11 +3773,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9123E77-EA56-403E-A728-B01259D22573}">
-  <dimension ref="A1:J63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A64DEF-E706-4B9C-B282-71F34F86B3DF}">
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3818,11 +3819,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A63">_xlfn._xlws.FILTER(data[factor_name],(data[Active])*(data[source]="yfinance"))</f>
+        <f t="array" ref="A2:A70">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J63">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J70">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -5799,6 +5800,230 @@
         <v>lognormal</v>
       </c>
       <c r="J63">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" t="str">
+        <v>TRUMP</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C64" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H64" t="str">
+        <v>TRUMP</v>
+      </c>
+      <c r="I64" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J64">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" t="str">
+        <v>FED</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C65" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H65" t="str">
+        <v>FED</v>
+      </c>
+      <c r="I65" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J65">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" t="str">
+        <v>AI</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C66" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H66" t="str">
+        <v>AI</v>
+      </c>
+      <c r="I66" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J66">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" t="str">
+        <v>GEOPOLITICS</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C67" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H67" t="str">
+        <v>GEOPOLITICS</v>
+      </c>
+      <c r="I67" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J67">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C68" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H68" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="I68" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J68">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" t="str">
+        <v>XLPXLY</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C69" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="str">
+        <v>Staples/Discretionary</v>
+      </c>
+      <c r="G69" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H69" t="str">
+        <v>XLPXLY</v>
+      </c>
+      <c r="I69" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J69">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" t="str">
+        <v>TRADEWAR</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Theme</v>
+      </c>
+      <c r="C70" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" t="str">
+        <v>composite</v>
+      </c>
+      <c r="H70" t="str">
+        <v>TRADEWAR</v>
+      </c>
+      <c r="I70" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J70">
         <v>1E-4</v>
       </c>
     </row>
@@ -5808,6 +6033,2042 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9123E77-EA56-403E-A728-B01259D22573}">
+  <dimension ref="A1:J63"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="44.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>466</v>
+      </c>
+      <c r="H1" t="s">
+        <v>465</v>
+      </c>
+      <c r="I1" t="s">
+        <v>464</v>
+      </c>
+      <c r="J1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A63">_xlfn._xlws.FILTER(data[factor_name],(data[Active])*(data[source]="yfinance"))</f>
+        <v>SPY</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:J63">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <v>Equities</v>
+      </c>
+      <c r="C2" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <v>S&amp;P 500</v>
+      </c>
+      <c r="G2" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H2" t="str">
+        <v>SPY</v>
+      </c>
+      <c r="I2" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>IWM</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C3" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Russell 2000</v>
+      </c>
+      <c r="G3" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H3" t="str">
+        <v>IWM</v>
+      </c>
+      <c r="I3" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>MDY</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C4" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="str">
+        <v>S&amp;P 400</v>
+      </c>
+      <c r="G4" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H4" t="str">
+        <v>MDY</v>
+      </c>
+      <c r="I4" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J4">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>RSP</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C5" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <v>S&amp;P 500 EW</v>
+      </c>
+      <c r="G5" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H5" t="str">
+        <v>RSP</v>
+      </c>
+      <c r="I5" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J5">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <v>QQQ</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C6" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Nasdaq 100</v>
+      </c>
+      <c r="G6" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H6" t="str">
+        <v>QQQ</v>
+      </c>
+      <c r="I6" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J6">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <v>DIA</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C7" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Dow Jones 30</v>
+      </c>
+      <c r="G7" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H7" t="str">
+        <v>DIA</v>
+      </c>
+      <c r="I7" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J7">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <v>XLK</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C8" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Technology</v>
+      </c>
+      <c r="G8" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H8" t="str">
+        <v>XLK</v>
+      </c>
+      <c r="I8" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J8">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <v>XLI</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C9" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Industrials</v>
+      </c>
+      <c r="G9" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H9" t="str">
+        <v>XLI</v>
+      </c>
+      <c r="I9" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J9">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <v>XLF</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C10" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Financials</v>
+      </c>
+      <c r="G10" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H10" t="str">
+        <v>XLF</v>
+      </c>
+      <c r="I10" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J10">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <v>KRE</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C11" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Regional Banks</v>
+      </c>
+      <c r="G11" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H11" t="str">
+        <v>KRE</v>
+      </c>
+      <c r="I11" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J11">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <v>XLC</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C12" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Communications</v>
+      </c>
+      <c r="G12" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H12" t="str">
+        <v>XLC</v>
+      </c>
+      <c r="I12" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J12">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <v>XLE</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C13" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Energy</v>
+      </c>
+      <c r="G13" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H13" t="str">
+        <v>XLE</v>
+      </c>
+      <c r="I13" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J13">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <v>XLY</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C14" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Discretionary</v>
+      </c>
+      <c r="G14" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H14" t="str">
+        <v>XLY</v>
+      </c>
+      <c r="I14" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J14">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <v>XLB</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C15" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Materials</v>
+      </c>
+      <c r="G15" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H15" t="str">
+        <v>XLB</v>
+      </c>
+      <c r="I15" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J15">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <v>XLV</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C16" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Health Care</v>
+      </c>
+      <c r="G16" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H16" t="str">
+        <v>XLV</v>
+      </c>
+      <c r="I16" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <v>XLU</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C17" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Utilities</v>
+      </c>
+      <c r="G17" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H17" t="str">
+        <v>XLU</v>
+      </c>
+      <c r="I17" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J17">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <v>XLP</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Sector</v>
+      </c>
+      <c r="C18" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Staples</v>
+      </c>
+      <c r="G18" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H18" t="str">
+        <v>XLP</v>
+      </c>
+      <c r="I18" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J18">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <v>IYR</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C19" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="str">
+        <v>iShares U.S. Real Estate ETF</v>
+      </c>
+      <c r="G19" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H19" t="str">
+        <v>IYR</v>
+      </c>
+      <c r="I19" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J19">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <v>VNQ</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C20" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Vanguard Real Estate ETF</v>
+      </c>
+      <c r="G20" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H20" t="str">
+        <v>VNQ</v>
+      </c>
+      <c r="I20" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J20">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <v>AIQ</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C21" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="str">
+        <v>AI</v>
+      </c>
+      <c r="G21" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H21" t="str">
+        <v>AIQ</v>
+      </c>
+      <c r="I21" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J21">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <v>ICLN</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C22" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Clean Energy</v>
+      </c>
+      <c r="G22" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H22" t="str">
+        <v>ICLN</v>
+      </c>
+      <c r="I22" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J22">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <v>PFF</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C23" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Preferred</v>
+      </c>
+      <c r="G23" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H23" t="str">
+        <v>PFF</v>
+      </c>
+      <c r="I23" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J23">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <v>FEZ</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C24" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="str">
+        <v>Eurostoxx 50</v>
+      </c>
+      <c r="G24" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H24" t="str">
+        <v>FEZ</v>
+      </c>
+      <c r="I24" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J24">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <v>EWU</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C25" t="str">
+        <v>GBP</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <v>iShares FTSE United Kingdom ETF</v>
+      </c>
+      <c r="G25" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H25" t="str">
+        <v>EWU</v>
+      </c>
+      <c r="I25" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <v>DAX</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C26" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="str">
+        <v>DAX (Germany)</v>
+      </c>
+      <c r="G26" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H26" t="str">
+        <v>DAX</v>
+      </c>
+      <c r="I26" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J26">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <v>EWC</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C27" t="str">
+        <v>CAD</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
+        <v>iShares MSCI Canada ETF</v>
+      </c>
+      <c r="G27" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H27" t="str">
+        <v>EWC</v>
+      </c>
+      <c r="I27" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J27">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <v>EWI</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C28" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="str">
+        <v>iShares MSCI Italy ETF</v>
+      </c>
+      <c r="G28" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H28" t="str">
+        <v>EWI</v>
+      </c>
+      <c r="I28" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J28">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <v>^N225</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C29" t="str">
+        <v>JPY</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="str">
+        <v>Nikkei 225</v>
+      </c>
+      <c r="G29" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H29" t="str">
+        <v>^N225</v>
+      </c>
+      <c r="I29" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J29">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <v>FXI</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C30" t="str">
+        <v>CNH</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
+        <v>iShares China Large-Cap ETF</v>
+      </c>
+      <c r="G30" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H30" t="str">
+        <v>FXI</v>
+      </c>
+      <c r="I30" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J30">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <v>ASHR</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C31" t="str">
+        <v>CNH</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="str">
+        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+      </c>
+      <c r="G31" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H31" t="str">
+        <v>ASHR</v>
+      </c>
+      <c r="I31" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J31">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <v>KWEB</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C32" t="str">
+        <v>CNH</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <v>KraneShares CSI China Internet ETF</v>
+      </c>
+      <c r="G32" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H32" t="str">
+        <v>KWEB</v>
+      </c>
+      <c r="I32" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J32">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <v>EEM</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Equities</v>
+      </c>
+      <c r="C33" t="str">
+        <v>EM</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H33" t="str">
+        <v>EEM</v>
+      </c>
+      <c r="I33" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J33">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <v>LQD</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C34" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="str">
+        <v>iShares iBoxx $ Investment Grade Corporate Bond ETF</v>
+      </c>
+      <c r="G34" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H34" t="str">
+        <v>LQD</v>
+      </c>
+      <c r="I34" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J34">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <v>BSV</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C35" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="str">
+        <v>Vanguard Short-Term Bond Index Fund ETF</v>
+      </c>
+      <c r="G35" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H35" t="str">
+        <v>BSV</v>
+      </c>
+      <c r="I35" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J35">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <v>HYG</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C36" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="str">
+        <v>iShares iBoxx $ High Yield Corporate Bond ETF</v>
+      </c>
+      <c r="G36" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H36" t="str">
+        <v>HYG</v>
+      </c>
+      <c r="I36" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J36">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <v>LQDH</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C37" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H37" t="str">
+        <v>LQDH</v>
+      </c>
+      <c r="I37" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J37">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <v>HYGH</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C38" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H38" t="str">
+        <v>HYGH</v>
+      </c>
+      <c r="I38" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J38">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <v>AGG</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Credit</v>
+      </c>
+      <c r="C39" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H39" t="str">
+        <v>AGG</v>
+      </c>
+      <c r="I39" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J39">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <v>^TNX</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C40" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H40" t="str">
+        <v>^TNX</v>
+      </c>
+      <c r="I40" t="str">
+        <v>normal</v>
+      </c>
+      <c r="J40">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <v>SHY</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C41" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="str">
+        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      </c>
+      <c r="G41" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H41" t="str">
+        <v>SHY</v>
+      </c>
+      <c r="I41" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J41">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <v>IEI</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C42" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="str">
+        <v>iShares 3-7 Year Treasury Bond ETF</v>
+      </c>
+      <c r="G42" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H42" t="str">
+        <v>IEI</v>
+      </c>
+      <c r="I42" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J42">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <v>IEF</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C43" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="str">
+        <v>iShares 7-10 Year Treasury Bond ETF</v>
+      </c>
+      <c r="G43" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H43" t="str">
+        <v>IEF</v>
+      </c>
+      <c r="I43" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J43">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <v>TLT</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C44" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="str">
+        <v>iShares 20+ Year Treasury Bond ETF</v>
+      </c>
+      <c r="G44" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H44" t="str">
+        <v>TLT</v>
+      </c>
+      <c r="I44" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J44">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <v>TIP</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C45" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="str">
+        <v>iShares TIPS Bond ETF</v>
+      </c>
+      <c r="G45" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H45" t="str">
+        <v>TIP</v>
+      </c>
+      <c r="I45" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J45">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <v>VTIP</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C46" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H46" t="str">
+        <v>VTIP</v>
+      </c>
+      <c r="I46" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J46">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <v>AGNC</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C47" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="str">
+        <v>AGNC Investment Corp.</v>
+      </c>
+      <c r="G47" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H47" t="str">
+        <v>AGNC</v>
+      </c>
+      <c r="I47" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J47">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <v>VMBS</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C48" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H48" t="str">
+        <v>VMBS</v>
+      </c>
+      <c r="I48" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J48">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <v>CMBS</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C49" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H49" t="str">
+        <v>CMBS</v>
+      </c>
+      <c r="I49" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J49">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <v>EMB</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Rates</v>
+      </c>
+      <c r="C50" t="str">
+        <v>EM</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="str">
+        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
+      </c>
+      <c r="G50" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H50" t="str">
+        <v>EMB</v>
+      </c>
+      <c r="I50" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J50">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <v>GLD</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C51" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="str">
+        <v>SPDR Gold Shares</v>
+      </c>
+      <c r="G51" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H51" t="str">
+        <v>GLD</v>
+      </c>
+      <c r="I51" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J51">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <v>SLV</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C52" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="str">
+        <v>iShares Silver Trust</v>
+      </c>
+      <c r="G52" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H52" t="str">
+        <v>SLV</v>
+      </c>
+      <c r="I52" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J52">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <v>USO</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Commodities</v>
+      </c>
+      <c r="C53" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="str">
+        <v>United States Oil Fund</v>
+      </c>
+      <c r="G53" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H53" t="str">
+        <v>USO</v>
+      </c>
+      <c r="I53" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J53">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <v>UUP</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C54" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Invesco DB US Dollar Index Bullish Fund</v>
+      </c>
+      <c r="G54" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H54" t="str">
+        <v>UUP</v>
+      </c>
+      <c r="I54" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J54">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <v>DX-Y.NYB</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C55" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H55" t="str">
+        <v>DX-Y.NYB</v>
+      </c>
+      <c r="I55" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J55">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <v>FXE</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C56" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Invesco CurrencyShares Euro Trust</v>
+      </c>
+      <c r="G56" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H56" t="str">
+        <v>FXE</v>
+      </c>
+      <c r="I56" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J56">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="str">
+        <v>FXY</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C57" t="str">
+        <v>JPY</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Invesco CurrencyShares Japanese Yen Trust</v>
+      </c>
+      <c r="G57" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H57" t="str">
+        <v>FXY</v>
+      </c>
+      <c r="I57" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J57">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" t="str">
+        <v>FXF</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C58" t="str">
+        <v>JPY</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="str">
+        <v>Invesco CurrencyShares Swiss Franc Trust</v>
+      </c>
+      <c r="G58" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H58" t="str">
+        <v>FXF</v>
+      </c>
+      <c r="I58" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J58">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" t="str">
+        <v>^VIX</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C59" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="str">
+        <v>CBOE Volatility Index</v>
+      </c>
+      <c r="G59" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H59" t="str">
+        <v>^VIX</v>
+      </c>
+      <c r="I59" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J59">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="str">
+        <v>VXX</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C60" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="str">
+        <v>VIX Short-Term Futures ETN</v>
+      </c>
+      <c r="G60" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H60" t="str">
+        <v>VXX</v>
+      </c>
+      <c r="I60" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J60">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="str">
+        <v>^VIX3M</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C61" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="str">
+        <v>CBOE S&amp;P 500 3-Month Volatility</v>
+      </c>
+      <c r="G61" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H61" t="str">
+        <v>^VIX3M</v>
+      </c>
+      <c r="I61" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J61">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" t="str">
+        <v>^MOVE</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C62" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" t="str">
+        <v>ICE BofAML MOVE Index</v>
+      </c>
+      <c r="G62" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H62" t="str">
+        <v>^MOVE</v>
+      </c>
+      <c r="I62" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J62">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" t="str">
+        <v>MWTIX</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Portfolio</v>
+      </c>
+      <c r="C63" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63" t="str">
+        <v>yfinance</v>
+      </c>
+      <c r="H63" t="str">
+        <v>MWTIX</v>
+      </c>
+      <c r="I63" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J63">
+        <v>1E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:J70"/>
@@ -8068,7 +10329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B51E7A-08A5-4042-86E1-7986ED98437B}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -8279,7 +10540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E63"/>
@@ -9371,7 +11632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509EC1D2-D913-4E91-BF4A-1B9A2D2D358E}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C9"/>
@@ -9490,7 +11751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28B96AA-E903-4E49-8EE7-2DF563672EF4}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D9"/>
@@ -9611,7 +11872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BECED18-9D5B-4FAE-9BAD-99DBF8245FFA}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:M74"/>
@@ -15500,15 +17761,197 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C05AAC-62F4-4536-9109-8789088E3F23}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:B22">_xlfn.XLOOKUP(_xlfn._TRO_ALL(A:A),data[factor_name],data[asset_class],"")</f>
+        <v>Equities</v>
+      </c>
+      <c r="F1" t="str">
+        <f>"['"&amp;_xlfn.TEXTJOIN("', '",,_xlfn._TRO_ALL(A:A))&amp;"']"</f>
+        <v>['SPY', 'FEZ', '^N225', 'LQDH', 'HYGH', 'EMB', 'IEI', 'IEF', 'TLT', 'FXE', 'FXY', 'FXF', 'TIP', 'VMBS', 'CMBS', 'GLD', 'USO']</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Equities</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Equities</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Credit</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Credit</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Currencies</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Currencies</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Currencies</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>346</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Rates</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Commodities</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Commodities</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15766,9 +18209,7 @@
       <c r="E5" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>362</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4">
         <v>1</v>
@@ -20176,7 +22617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BE1690-4C72-4E94-925C-89FAF286C7F8}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -20343,2264 +22784,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A64DEF-E706-4B9C-B282-71F34F86B3DF}">
-  <dimension ref="A1:J70"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="44.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D1" t="s">
-        <v>428</v>
-      </c>
-      <c r="E1" t="s">
-        <v>445</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>466</v>
-      </c>
-      <c r="H1" t="s">
-        <v>465</v>
-      </c>
-      <c r="I1" t="s">
-        <v>464</v>
-      </c>
-      <c r="J1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A70">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
-        <v>SPY</v>
-      </c>
-      <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J70">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
-        <v>Equities</v>
-      </c>
-      <c r="C2" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="str">
-        <v>S&amp;P 500</v>
-      </c>
-      <c r="G2" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H2" t="str">
-        <v>SPY</v>
-      </c>
-      <c r="I2" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J2">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>IWM</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C3" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Russell 2000</v>
-      </c>
-      <c r="G3" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H3" t="str">
-        <v>IWM</v>
-      </c>
-      <c r="I3" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J3">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>MDY</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C4" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="str">
-        <v>S&amp;P 400</v>
-      </c>
-      <c r="G4" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H4" t="str">
-        <v>MDY</v>
-      </c>
-      <c r="I4" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J4">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>RSP</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C5" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <v>S&amp;P 500 EW</v>
-      </c>
-      <c r="G5" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H5" t="str">
-        <v>RSP</v>
-      </c>
-      <c r="I5" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J5">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <v>QQQ</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C6" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Nasdaq 100</v>
-      </c>
-      <c r="G6" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H6" t="str">
-        <v>QQQ</v>
-      </c>
-      <c r="I6" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J6">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <v>DIA</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C7" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Dow Jones 30</v>
-      </c>
-      <c r="G7" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H7" t="str">
-        <v>DIA</v>
-      </c>
-      <c r="I7" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J7">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <v>XLK</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C8" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Technology</v>
-      </c>
-      <c r="G8" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H8" t="str">
-        <v>XLK</v>
-      </c>
-      <c r="I8" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J8">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <v>XLI</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C9" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="str">
-        <v>Industrials</v>
-      </c>
-      <c r="G9" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H9" t="str">
-        <v>XLI</v>
-      </c>
-      <c r="I9" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J9">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <v>XLF</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C10" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Financials</v>
-      </c>
-      <c r="G10" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H10" t="str">
-        <v>XLF</v>
-      </c>
-      <c r="I10" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J10">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <v>KRE</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C11" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Regional Banks</v>
-      </c>
-      <c r="G11" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H11" t="str">
-        <v>KRE</v>
-      </c>
-      <c r="I11" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J11">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <v>XLC</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C12" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Communications</v>
-      </c>
-      <c r="G12" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H12" t="str">
-        <v>XLC</v>
-      </c>
-      <c r="I12" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J12">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <v>XLE</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C13" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="str">
-        <v>Energy</v>
-      </c>
-      <c r="G13" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H13" t="str">
-        <v>XLE</v>
-      </c>
-      <c r="I13" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J13">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <v>XLY</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C14" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="str">
-        <v>Discretionary</v>
-      </c>
-      <c r="G14" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H14" t="str">
-        <v>XLY</v>
-      </c>
-      <c r="I14" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J14">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <v>XLB</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C15" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="str">
-        <v>Materials</v>
-      </c>
-      <c r="G15" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H15" t="str">
-        <v>XLB</v>
-      </c>
-      <c r="I15" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J15">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <v>XLV</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C16" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="str">
-        <v>Health Care</v>
-      </c>
-      <c r="G16" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H16" t="str">
-        <v>XLV</v>
-      </c>
-      <c r="I16" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J16">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <v>XLU</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C17" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="str">
-        <v>Utilities</v>
-      </c>
-      <c r="G17" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H17" t="str">
-        <v>XLU</v>
-      </c>
-      <c r="I17" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J17">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <v>XLP</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Sector</v>
-      </c>
-      <c r="C18" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="str">
-        <v>Staples</v>
-      </c>
-      <c r="G18" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H18" t="str">
-        <v>XLP</v>
-      </c>
-      <c r="I18" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J18">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <v>IYR</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C19" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="str">
-        <v>iShares U.S. Real Estate ETF</v>
-      </c>
-      <c r="G19" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H19" t="str">
-        <v>IYR</v>
-      </c>
-      <c r="I19" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J19">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <v>VNQ</v>
-      </c>
-      <c r="B20" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C20" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="str">
-        <v>Vanguard Real Estate ETF</v>
-      </c>
-      <c r="G20" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H20" t="str">
-        <v>VNQ</v>
-      </c>
-      <c r="I20" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J20">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <v>AIQ</v>
-      </c>
-      <c r="B21" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C21" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="str">
-        <v>AI</v>
-      </c>
-      <c r="G21" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H21" t="str">
-        <v>AIQ</v>
-      </c>
-      <c r="I21" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J21">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <v>ICLN</v>
-      </c>
-      <c r="B22" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C22" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="str">
-        <v>Clean Energy</v>
-      </c>
-      <c r="G22" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H22" t="str">
-        <v>ICLN</v>
-      </c>
-      <c r="I22" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J22">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <v>PFF</v>
-      </c>
-      <c r="B23" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C23" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="str">
-        <v>Preferred</v>
-      </c>
-      <c r="G23" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H23" t="str">
-        <v>PFF</v>
-      </c>
-      <c r="I23" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J23">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <v>FEZ</v>
-      </c>
-      <c r="B24" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C24" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="str">
-        <v>Eurostoxx 50</v>
-      </c>
-      <c r="G24" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H24" t="str">
-        <v>FEZ</v>
-      </c>
-      <c r="I24" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J24">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <v>EWU</v>
-      </c>
-      <c r="B25" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C25" t="str">
-        <v>GBP</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
-      </c>
-      <c r="G25" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H25" t="str">
-        <v>EWU</v>
-      </c>
-      <c r="I25" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J25">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
-        <v>DAX</v>
-      </c>
-      <c r="B26" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C26" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="str">
-        <v>DAX (Germany)</v>
-      </c>
-      <c r="G26" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H26" t="str">
-        <v>DAX</v>
-      </c>
-      <c r="I26" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J26">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <v>EWC</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C27" t="str">
-        <v>CAD</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="str">
-        <v>iShares MSCI Canada ETF</v>
-      </c>
-      <c r="G27" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H27" t="str">
-        <v>EWC</v>
-      </c>
-      <c r="I27" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J27">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <v>EWI</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C28" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="str">
-        <v>iShares MSCI Italy ETF</v>
-      </c>
-      <c r="G28" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H28" t="str">
-        <v>EWI</v>
-      </c>
-      <c r="I28" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J28">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <v>^N225</v>
-      </c>
-      <c r="B29" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C29" t="str">
-        <v>JPY</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="str">
-        <v>Nikkei 225</v>
-      </c>
-      <c r="G29" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H29" t="str">
-        <v>^N225</v>
-      </c>
-      <c r="I29" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J29">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <v>FXI</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C30" t="str">
-        <v>CNH</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="str">
-        <v>iShares China Large-Cap ETF</v>
-      </c>
-      <c r="G30" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H30" t="str">
-        <v>FXI</v>
-      </c>
-      <c r="I30" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J30">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <v>ASHR</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C31" t="str">
-        <v>CNH</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
-      </c>
-      <c r="G31" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H31" t="str">
-        <v>ASHR</v>
-      </c>
-      <c r="I31" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J31">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <v>KWEB</v>
-      </c>
-      <c r="B32" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C32" t="str">
-        <v>CNH</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
-      </c>
-      <c r="G32" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H32" t="str">
-        <v>KWEB</v>
-      </c>
-      <c r="I32" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J32">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <v>EEM</v>
-      </c>
-      <c r="B33" t="str">
-        <v>Equities</v>
-      </c>
-      <c r="C33" t="str">
-        <v>EM</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H33" t="str">
-        <v>EEM</v>
-      </c>
-      <c r="I33" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J33">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
-        <v>LQD</v>
-      </c>
-      <c r="B34" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C34" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" t="str">
-        <v>iShares iBoxx $ Investment Grade Corporate Bond ETF</v>
-      </c>
-      <c r="G34" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H34" t="str">
-        <v>LQD</v>
-      </c>
-      <c r="I34" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J34">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <v>BSV</v>
-      </c>
-      <c r="B35" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C35" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="str">
-        <v>Vanguard Short-Term Bond Index Fund ETF</v>
-      </c>
-      <c r="G35" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H35" t="str">
-        <v>BSV</v>
-      </c>
-      <c r="I35" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J35">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="str">
-        <v>HYG</v>
-      </c>
-      <c r="B36" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C36" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="str">
-        <v>iShares iBoxx $ High Yield Corporate Bond ETF</v>
-      </c>
-      <c r="G36" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H36" t="str">
-        <v>HYG</v>
-      </c>
-      <c r="I36" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J36">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" t="str">
-        <v>LQDH</v>
-      </c>
-      <c r="B37" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C37" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H37" t="str">
-        <v>LQDH</v>
-      </c>
-      <c r="I37" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J37">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" t="str">
-        <v>HYGH</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C38" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H38" t="str">
-        <v>HYGH</v>
-      </c>
-      <c r="I38" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J38">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" t="str">
-        <v>AGG</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Credit</v>
-      </c>
-      <c r="C39" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H39" t="str">
-        <v>AGG</v>
-      </c>
-      <c r="I39" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J39">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" t="str">
-        <v>^TNX</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C40" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H40" t="str">
-        <v>^TNX</v>
-      </c>
-      <c r="I40" t="str">
-        <v>normal</v>
-      </c>
-      <c r="J40">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="str">
-        <v>SHY</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C41" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
-      </c>
-      <c r="G41" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H41" t="str">
-        <v>SHY</v>
-      </c>
-      <c r="I41" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J41">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="str">
-        <v>IEI</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C42" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
-      </c>
-      <c r="G42" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H42" t="str">
-        <v>IEI</v>
-      </c>
-      <c r="I42" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J42">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="str">
-        <v>IEF</v>
-      </c>
-      <c r="B43" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C43" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
-      </c>
-      <c r="G43" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H43" t="str">
-        <v>IEF</v>
-      </c>
-      <c r="I43" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J43">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" t="str">
-        <v>TLT</v>
-      </c>
-      <c r="B44" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C44" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
-      </c>
-      <c r="G44" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H44" t="str">
-        <v>TLT</v>
-      </c>
-      <c r="I44" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J44">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" t="str">
-        <v>TIP</v>
-      </c>
-      <c r="B45" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C45" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45" t="str">
-        <v>iShares TIPS Bond ETF</v>
-      </c>
-      <c r="G45" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H45" t="str">
-        <v>TIP</v>
-      </c>
-      <c r="I45" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J45">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" t="str">
-        <v>VTIP</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C46" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H46" t="str">
-        <v>VTIP</v>
-      </c>
-      <c r="I46" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J46">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" t="str">
-        <v>AGNC</v>
-      </c>
-      <c r="B47" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C47" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" t="str">
-        <v>AGNC Investment Corp.</v>
-      </c>
-      <c r="G47" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H47" t="str">
-        <v>AGNC</v>
-      </c>
-      <c r="I47" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J47">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" t="str">
-        <v>VMBS</v>
-      </c>
-      <c r="B48" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C48" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H48" t="str">
-        <v>VMBS</v>
-      </c>
-      <c r="I48" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J48">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" t="str">
-        <v>CMBS</v>
-      </c>
-      <c r="B49" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C49" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H49" t="str">
-        <v>CMBS</v>
-      </c>
-      <c r="I49" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J49">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" t="str">
-        <v>EMB</v>
-      </c>
-      <c r="B50" t="str">
-        <v>Rates</v>
-      </c>
-      <c r="C50" t="str">
-        <v>EM</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50" t="str">
-        <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
-      </c>
-      <c r="G50" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H50" t="str">
-        <v>EMB</v>
-      </c>
-      <c r="I50" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J50">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" t="str">
-        <v>GLD</v>
-      </c>
-      <c r="B51" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C51" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51" t="str">
-        <v>SPDR Gold Shares</v>
-      </c>
-      <c r="G51" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H51" t="str">
-        <v>GLD</v>
-      </c>
-      <c r="I51" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J51">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" t="str">
-        <v>SLV</v>
-      </c>
-      <c r="B52" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C52" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52" t="str">
-        <v>iShares Silver Trust</v>
-      </c>
-      <c r="G52" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H52" t="str">
-        <v>SLV</v>
-      </c>
-      <c r="I52" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J52">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" t="str">
-        <v>USO</v>
-      </c>
-      <c r="B53" t="str">
-        <v>Commodities</v>
-      </c>
-      <c r="C53" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" t="str">
-        <v>United States Oil Fund</v>
-      </c>
-      <c r="G53" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H53" t="str">
-        <v>USO</v>
-      </c>
-      <c r="I53" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J53">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" t="str">
-        <v>UUP</v>
-      </c>
-      <c r="B54" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C54" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54" t="str">
-        <v>Invesco DB US Dollar Index Bullish Fund</v>
-      </c>
-      <c r="G54" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H54" t="str">
-        <v>UUP</v>
-      </c>
-      <c r="I54" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J54">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" t="str">
-        <v>DX-Y.NYB</v>
-      </c>
-      <c r="B55" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C55" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H55" t="str">
-        <v>DX-Y.NYB</v>
-      </c>
-      <c r="I55" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J55">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" t="str">
-        <v>FXE</v>
-      </c>
-      <c r="B56" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C56" t="str">
-        <v>EUR</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56" t="str">
-        <v>Invesco CurrencyShares Euro Trust</v>
-      </c>
-      <c r="G56" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H56" t="str">
-        <v>FXE</v>
-      </c>
-      <c r="I56" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J56">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" t="str">
-        <v>FXY</v>
-      </c>
-      <c r="B57" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C57" t="str">
-        <v>JPY</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57" t="str">
-        <v>Invesco CurrencyShares Japanese Yen Trust</v>
-      </c>
-      <c r="G57" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H57" t="str">
-        <v>FXY</v>
-      </c>
-      <c r="I57" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J57">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" t="str">
-        <v>FXF</v>
-      </c>
-      <c r="B58" t="str">
-        <v>Currencies</v>
-      </c>
-      <c r="C58" t="str">
-        <v>JPY</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58" t="str">
-        <v>Invesco CurrencyShares Swiss Franc Trust</v>
-      </c>
-      <c r="G58" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H58" t="str">
-        <v>FXF</v>
-      </c>
-      <c r="I58" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J58">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" t="str">
-        <v>^VIX</v>
-      </c>
-      <c r="B59" t="str">
-        <v>Vol</v>
-      </c>
-      <c r="C59" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59" t="str">
-        <v>CBOE Volatility Index</v>
-      </c>
-      <c r="G59" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H59" t="str">
-        <v>^VIX</v>
-      </c>
-      <c r="I59" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J59">
-        <v>-1E-4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" t="str">
-        <v>VXX</v>
-      </c>
-      <c r="B60" t="str">
-        <v>Vol</v>
-      </c>
-      <c r="C60" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60" t="str">
-        <v>VIX Short-Term Futures ETN</v>
-      </c>
-      <c r="G60" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H60" t="str">
-        <v>VXX</v>
-      </c>
-      <c r="I60" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J60">
-        <v>-1E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" t="str">
-        <v>^VIX3M</v>
-      </c>
-      <c r="B61" t="str">
-        <v>Vol</v>
-      </c>
-      <c r="C61" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61" t="str">
-        <v>CBOE S&amp;P 500 3-Month Volatility</v>
-      </c>
-      <c r="G61" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H61" t="str">
-        <v>^VIX3M</v>
-      </c>
-      <c r="I61" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J61">
-        <v>-1E-4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" t="str">
-        <v>^MOVE</v>
-      </c>
-      <c r="B62" t="str">
-        <v>Vol</v>
-      </c>
-      <c r="C62" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62" t="str">
-        <v>ICE BofAML MOVE Index</v>
-      </c>
-      <c r="G62" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H62" t="str">
-        <v>^MOVE</v>
-      </c>
-      <c r="I62" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J62">
-        <v>-1E-4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" t="str">
-        <v>MWTIX</v>
-      </c>
-      <c r="B63" t="str">
-        <v>Portfolio</v>
-      </c>
-      <c r="C63" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63" t="str">
-        <v>yfinance</v>
-      </c>
-      <c r="H63" t="str">
-        <v>MWTIX</v>
-      </c>
-      <c r="I63" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J63">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" t="str">
-        <v>TRUMP</v>
-      </c>
-      <c r="B64" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C64" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H64" t="str">
-        <v>TRUMP</v>
-      </c>
-      <c r="I64" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J64">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" t="str">
-        <v>FED</v>
-      </c>
-      <c r="B65" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C65" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H65" t="str">
-        <v>FED</v>
-      </c>
-      <c r="I65" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J65">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" t="str">
-        <v>AI</v>
-      </c>
-      <c r="B66" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C66" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H66" t="str">
-        <v>AI</v>
-      </c>
-      <c r="I66" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J66">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" t="str">
-        <v>GEOPOLITICS</v>
-      </c>
-      <c r="B67" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C67" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H67" t="str">
-        <v>GEOPOLITICS</v>
-      </c>
-      <c r="I67" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J67">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" t="str">
-        <v>2s10s</v>
-      </c>
-      <c r="B68" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C68" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H68" t="str">
-        <v>2s10s</v>
-      </c>
-      <c r="I68" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J68">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" t="str">
-        <v>XLPXLY</v>
-      </c>
-      <c r="B69" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C69" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="F69" t="str">
-        <v>Staples/Discretionary</v>
-      </c>
-      <c r="G69" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H69" t="str">
-        <v>XLPXLY</v>
-      </c>
-      <c r="I69" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J69">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" t="str">
-        <v>TRADEWAR</v>
-      </c>
-      <c r="B70" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C70" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H70" t="str">
-        <v>TRADEWAR</v>
-      </c>
-      <c r="I70" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J70">
-        <v>1E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
config: Create tracking portfolio test (and update docs)
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09EDC06-1857-4B48-9FBC-1E601EC30C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57776251-29A2-4988-912A-5D06C5D51C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="7" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
@@ -20,16 +20,17 @@
     <sheet name="read_composites" sheetId="14" r:id="rId5"/>
     <sheet name="composites" sheetId="13" r:id="rId6"/>
     <sheet name="risk_parity" sheetId="20" r:id="rId7"/>
-    <sheet name="data" sheetId="3" r:id="rId8"/>
-    <sheet name="read_new" sheetId="15" r:id="rId9"/>
-    <sheet name="read_tcw" sheetId="17" r:id="rId10"/>
-    <sheet name="read_nocomposite" sheetId="19" r:id="rId11"/>
-    <sheet name="read" sheetId="12" r:id="rId12"/>
-    <sheet name="read_short" sheetId="16" r:id="rId13"/>
-    <sheet name="read_old2" sheetId="4" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId15"/>
-    <sheet name="read_old" sheetId="1" r:id="rId16"/>
-    <sheet name="data_old" sheetId="8" r:id="rId17"/>
+    <sheet name="tracking" sheetId="21" r:id="rId8"/>
+    <sheet name="data" sheetId="3" r:id="rId9"/>
+    <sheet name="read_new" sheetId="15" r:id="rId10"/>
+    <sheet name="read_tcw" sheetId="17" r:id="rId11"/>
+    <sheet name="read_nocomposite" sheetId="19" r:id="rId12"/>
+    <sheet name="read" sheetId="12" r:id="rId13"/>
+    <sheet name="read_short" sheetId="16" r:id="rId14"/>
+    <sheet name="read_old2" sheetId="4" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId16"/>
+    <sheet name="read_old" sheetId="1" r:id="rId17"/>
+    <sheet name="data_old" sheetId="8" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="509">
   <si>
     <t>SPX</t>
   </si>
@@ -1613,6 +1614,9 @@
   </si>
   <si>
     <t>Staples/Discretionary</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -1680,7 +1684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1701,6 +1705,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3773,6 +3778,175 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BE1690-4C72-4E94-925C-89FAF286C7F8}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E1" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G1" t="s">
+        <v>463</v>
+      </c>
+      <c r="H1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G2" t="s">
+        <v>457</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>454</v>
+      </c>
+      <c r="G3" t="s">
+        <v>457</v>
+      </c>
+      <c r="H3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>455</v>
+      </c>
+      <c r="E4" t="s">
+        <v>459</v>
+      </c>
+      <c r="F4" t="s">
+        <v>454</v>
+      </c>
+      <c r="G4" t="s">
+        <v>457</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>455</v>
+      </c>
+      <c r="E5" t="s">
+        <v>458</v>
+      </c>
+      <c r="F5" t="s">
+        <v>467</v>
+      </c>
+      <c r="G5" t="s">
+        <v>457</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>455</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" t="s">
+        <v>454</v>
+      </c>
+      <c r="G6" t="s">
+        <v>453</v>
+      </c>
+      <c r="H6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A64DEF-E706-4B9C-B282-71F34F86B3DF}">
   <dimension ref="A1:J70"/>
   <sheetViews>
@@ -6032,7 +6206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9123E77-EA56-403E-A728-B01259D22573}">
   <dimension ref="A1:J63"/>
   <sheetViews>
@@ -8068,7 +8242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:J70"/>
@@ -10329,7 +10503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B51E7A-08A5-4042-86E1-7986ED98437B}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -10540,7 +10714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E63"/>
@@ -11632,7 +11806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509EC1D2-D913-4E91-BF4A-1B9A2D2D358E}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C9"/>
@@ -11751,7 +11925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28B96AA-E903-4E49-8EE7-2DF563672EF4}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D9"/>
@@ -11872,7 +12046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BECED18-9D5B-4FAE-9BAD-99DBF8245FFA}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:M74"/>
@@ -17943,15 +18117,183 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC776AF-E8A8-4661-B4BA-DFE8D3F65EBD}">
+  <dimension ref="A1:R13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" t="s">
+        <v>499</v>
+      </c>
+      <c r="N1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O1" t="s">
+        <v>346</v>
+      </c>
+      <c r="P1" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" cm="1">
+        <f t="array" ref="A2:A13">DATE(_xlfn.SEQUENCE(12,,2025,-1),1,1)</f>
+        <v>45658</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>45292</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>44927</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>44562</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>44197</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>43831</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>43101</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>42370</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>42005</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>41640</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F77" sqref="F77"/>
+      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22615,173 +22957,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BE1690-4C72-4E94-925C-89FAF286C7F8}">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D1" t="s">
-        <v>466</v>
-      </c>
-      <c r="E1" t="s">
-        <v>465</v>
-      </c>
-      <c r="F1" t="s">
-        <v>464</v>
-      </c>
-      <c r="G1" t="s">
-        <v>463</v>
-      </c>
-      <c r="H1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>455</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>454</v>
-      </c>
-      <c r="G2" t="s">
-        <v>457</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>461</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>455</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>454</v>
-      </c>
-      <c r="G3" t="s">
-        <v>457</v>
-      </c>
-      <c r="H3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>455</v>
-      </c>
-      <c r="E4" t="s">
-        <v>459</v>
-      </c>
-      <c r="F4" t="s">
-        <v>454</v>
-      </c>
-      <c r="G4" t="s">
-        <v>457</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>455</v>
-      </c>
-      <c r="E5" t="s">
-        <v>458</v>
-      </c>
-      <c r="F5" t="s">
-        <v>467</v>
-      </c>
-      <c r="G5" t="s">
-        <v>457</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>456</v>
-      </c>
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>455</v>
-      </c>
-      <c r="E6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" t="s">
-        <v>454</v>
-      </c>
-      <c r="G6" t="s">
-        <v>453</v>
-      </c>
-      <c r="H6" t="s">
-        <v>452</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: Reassign asset classes for composite factors; rename variables and clean docstrings
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B75F17B-266F-4FB6-B889-310300EF2E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B051C999-C8A7-49F4-A826-5F4E97BD5A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="5" activeTab="8" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="10" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -1766,10 +1766,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1814,6 +1810,10 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2020,31 +2020,31 @@
     </tableColumn>
     <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="20"/>
     <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="18">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="18">
+    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="17">
       <calculatedColumnFormula>data[[#This Row],[factor_name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:I45" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="5">
       <calculatedColumnFormula>IF(data_old[[#This Row],[description_override]]="",data_old[[#This Row],[Description_GPT]],data_old[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3955,11 +3955,11 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q15" sqref="Q15"/>
+      <selection pane="bottomRight" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8464,7 +8464,7 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>444</v>
+        <v>128</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>40</v>
@@ -8513,7 +8513,7 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>444</v>
+        <v>39</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>40</v>
@@ -10960,7 +10960,7 @@
         <v>2s10s</v>
       </c>
       <c r="B68" t="str">
-        <v>Theme</v>
+        <v>Rates</v>
       </c>
       <c r="C68" t="str">
         <v>USD</v>
@@ -10992,7 +10992,7 @@
         <v>XLPXLY</v>
       </c>
       <c r="B69" t="str">
-        <v>Theme</v>
+        <v>Equities</v>
       </c>
       <c r="C69" t="str">
         <v>USD</v>
@@ -13097,8 +13097,11 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15257,7 +15260,7 @@
         <v>2s10s</v>
       </c>
       <c r="B68" t="str">
-        <v>Theme</v>
+        <v>Rates</v>
       </c>
       <c r="C68" t="str">
         <v>USD</v>
@@ -15289,7 +15292,7 @@
         <v>XLPXLY</v>
       </c>
       <c r="B69" t="str">
-        <v>Theme</v>
+        <v>Equities</v>
       </c>
       <c r="C69" t="str">
         <v>USD</v>
@@ -15570,7 +15573,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22980,7 +22983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6EE184-8219-4FAC-8CFD-91717B8EFB99}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -23015,7 +23018,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <f ca="1">TODAY()-1</f>
-        <v>45804</v>
+        <v>45809</v>
       </c>
       <c r="B2">
         <v>0.20547945205479451</v>

</xml_diff>

<commit_message>
chore: Clean interface, trim portfolio returns, clean comments and todos
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B051C999-C8A7-49F4-A826-5F4E97BD5A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780C28FC-4A06-46E2-85C7-B7C3FC0CC5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="10" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="10" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="528">
   <si>
     <t>SPX</t>
   </si>
@@ -1498,9 +1498,6 @@
     <t>normal</t>
   </si>
   <si>
-    <t>CBOE Interest Rate 10 Year T No (^TNX)</t>
-  </si>
-  <si>
     <t>multiplier</t>
   </si>
   <si>
@@ -1622,6 +1619,63 @@
   </si>
   <si>
     <t>ELECTION</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>FTSE 100</t>
+  </si>
+  <si>
+    <t>MSCI Canada</t>
+  </si>
+  <si>
+    <t>MSCI Italy</t>
+  </si>
+  <si>
+    <t>MSCI Spain</t>
+  </si>
+  <si>
+    <t>China Large-Cap</t>
+  </si>
+  <si>
+    <t>CSI China Internet</t>
+  </si>
+  <si>
+    <t>iShares MSCI Emerging Markets ETF</t>
+  </si>
+  <si>
+    <t>iShares Core US Aggregate Bond ETF</t>
+  </si>
+  <si>
+    <t>US Agg</t>
+  </si>
+  <si>
+    <t>CBOE Interest Rate 10 Year</t>
+  </si>
+  <si>
+    <t>Short-Term Inflation-Protected Securities ETF</t>
+  </si>
+  <si>
+    <t>Mortgage-Backed Securities ETF</t>
+  </si>
+  <si>
+    <t>iShares JP Morgan EM High Yield Bond ETF</t>
+  </si>
+  <si>
+    <t>TCW MetWest Total Return Bd I</t>
+  </si>
+  <si>
+    <t>JPYUSD</t>
+  </si>
+  <si>
+    <t>CHFUSD</t>
+  </si>
+  <si>
+    <t>Hedged HYG</t>
+  </si>
+  <si>
+    <t>Hedged LQD</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1711,11 +1765,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="39">
     <dxf>
       <border>
         <top style="thin">
@@ -1760,6 +1817,28 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1827,10 +1906,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1916,8 +1991,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{26B58CFA-74FB-41FD-AB02-EC6D3EA4F4A1}">
-      <tableStyleElement type="wholeTable" dxfId="36"/>
-      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="wholeTable" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="37"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2002,49 +2077,49 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:Q88" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:Q87" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="25"/>
-    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{494805E4-EBB6-47FD-9BC2-8DAD9FB9D3FA}" name="composite" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{608FE572-4016-436E-8625-08926F3A2371}" name="client" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="21">
-      <calculatedColumnFormula>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{0E50B2E3-0362-41DB-ACC2-478CC6F618A4}" name="factor_name" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{02943B27-7FCB-4450-B8E0-CF0DB6CF5CCA}" name="factor_name_new" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{D181BF84-863F-4FD0-B518-14EA5B0FB18E}" name="description_override" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{1C40DF9B-2910-4DE6-A188-563938E39797}" name="Description_GPT" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{1806E074-6CB5-47AB-8FA3-EF0F6E429062}" name="Underlying" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{21539C17-C1CC-4FA9-A0E1-A2F8FF8AB52C}" name="Active" dataDxfId="27"/>
+    <tableColumn id="37" xr3:uid="{DE50B7AE-5F67-471C-BE48-8BFA5076EDB0}" name="hyper_factor" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{494805E4-EBB6-47FD-9BC2-8DAD9FB9D3FA}" name="composite" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{608FE572-4016-436E-8625-08926F3A2371}" name="client" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{5A601067-D384-419C-A711-AD3034F77E28}" name="description" dataDxfId="7">
+      <calculatedColumnFormula array="1">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="18">
+    <tableColumn id="11" xr3:uid="{C400A641-F032-4829-A2CD-62831D657B37}" name="source" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{BC682952-ADA8-4869-A16F-B9E7BC86E430}" name="diffusion_type" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{A99CC35E-FB67-451C-BF9C-DA8D933B1B0C}" name="multiplier" dataDxfId="21">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="17">
+    <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="20">
       <calculatedColumnFormula>data[[#This Row],[factor_name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:I45" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="8">
       <calculatedColumnFormula>IF(data_old[[#This Row],[description_override]]="",data_old[[#This Row],[Description_GPT]],data_old[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3794,7 +3869,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3830,7 +3905,7 @@
         <v>72</v>
       </c>
       <c r="M1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N1" t="s">
         <v>135</v>
@@ -3953,13 +4028,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:V87"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F67" sqref="F67"/>
+      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4006,7 +4081,7 @@
         <v>445</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>19</v>
@@ -4018,13 +4093,13 @@
         <v>464</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>465</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -4061,8 +4136,8 @@
       <c r="K2" s="4">
         <v>0</v>
       </c>
-      <c r="L2" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L2" s="4" t="str" cm="1">
+        <f t="array" ref="L2">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>S&amp;P 500</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -4082,7 +4157,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="2"/>
       <c r="S2" t="b" cm="1">
-        <f t="array" ref="S2:S88">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
+        <f t="array" ref="S2:S87">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
         <v>1</v>
       </c>
     </row>
@@ -4120,8 +4195,8 @@
       <c r="K3" s="4">
         <v>0</v>
       </c>
-      <c r="L3" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L3" s="4" t="str" cm="1">
+        <f t="array" ref="L3">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Russell 2000</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -4143,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
@@ -4180,8 +4255,8 @@
       <c r="K4" s="4">
         <v>0</v>
       </c>
-      <c r="L4" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L4" s="4" t="str" cm="1">
+        <f t="array" ref="L4">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>S&amp;P 400</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -4231,8 +4306,8 @@
       <c r="K5" s="4">
         <v>0</v>
       </c>
-      <c r="L5" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L5" s="4" t="str" cm="1">
+        <f t="array" ref="L5">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>S&amp;P 500 EW</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -4254,7 +4329,7 @@
         <v>1</v>
       </c>
       <c r="V5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -4291,8 +4366,8 @@
       <c r="K6" s="4">
         <v>0</v>
       </c>
-      <c r="L6" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L6" s="4" t="str" cm="1">
+        <f t="array" ref="L6">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Nasdaq 100</v>
       </c>
       <c r="M6" s="4" t="s">
@@ -4348,8 +4423,8 @@
       <c r="K7" s="4">
         <v>0</v>
       </c>
-      <c r="L7" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L7" s="4" t="str" cm="1">
+        <f t="array" ref="L7">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Dow Jones 30</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -4401,8 +4476,8 @@
       <c r="K8" s="4">
         <v>0</v>
       </c>
-      <c r="L8" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L8" s="4" t="str" cm="1">
+        <f t="array" ref="L8">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Technology</v>
       </c>
       <c r="M8" s="4" t="s">
@@ -4454,8 +4529,8 @@
       <c r="K9" s="4">
         <v>0</v>
       </c>
-      <c r="L9" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L9" s="4" t="str" cm="1">
+        <f t="array" ref="L9">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Industrials</v>
       </c>
       <c r="M9" s="4" t="s">
@@ -4507,8 +4582,8 @@
       <c r="K10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L10" s="4" t="str" cm="1">
+        <f t="array" ref="L10">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Financials</v>
       </c>
       <c r="M10" s="4" t="s">
@@ -4560,8 +4635,8 @@
       <c r="K11" s="4">
         <v>0</v>
       </c>
-      <c r="L11" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L11" s="4" t="str" cm="1">
+        <f t="array" ref="L11">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Regional Banks</v>
       </c>
       <c r="M11" s="4" t="s">
@@ -4613,8 +4688,8 @@
       <c r="K12" s="4">
         <v>0</v>
       </c>
-      <c r="L12" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L12" s="4" t="str" cm="1">
+        <f t="array" ref="L12">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Communications</v>
       </c>
       <c r="M12" s="4" t="s">
@@ -4666,8 +4741,8 @@
       <c r="K13" s="4">
         <v>0</v>
       </c>
-      <c r="L13" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L13" s="4" t="str" cm="1">
+        <f t="array" ref="L13">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Energy</v>
       </c>
       <c r="M13" s="4" t="s">
@@ -4719,8 +4794,8 @@
       <c r="K14" s="4">
         <v>0</v>
       </c>
-      <c r="L14" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L14" s="4" t="str" cm="1">
+        <f t="array" ref="L14">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Discretionary</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -4772,8 +4847,8 @@
       <c r="K15" s="4">
         <v>0</v>
       </c>
-      <c r="L15" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L15" s="4" t="str" cm="1">
+        <f t="array" ref="L15">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Materials</v>
       </c>
       <c r="M15" s="4" t="s">
@@ -4825,8 +4900,8 @@
       <c r="K16" s="4">
         <v>0</v>
       </c>
-      <c r="L16" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L16" s="4" t="str" cm="1">
+        <f t="array" ref="L16">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Health Care</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -4878,8 +4953,8 @@
       <c r="K17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L17" s="4" t="str" cm="1">
+        <f t="array" ref="L17">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Utilities</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -4931,8 +5006,8 @@
       <c r="K18" s="4">
         <v>0</v>
       </c>
-      <c r="L18" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L18" s="4" t="str" cm="1">
+        <f t="array" ref="L18">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Staples</v>
       </c>
       <c r="M18" s="4" t="s">
@@ -4982,8 +5057,8 @@
       <c r="K19" s="4">
         <v>0</v>
       </c>
-      <c r="L19" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L19" s="4" t="str" cm="1">
+        <f t="array" ref="L19">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares U.S. Real Estate ETF</v>
       </c>
       <c r="M19" s="4" t="s">
@@ -5033,8 +5108,8 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
-      <c r="L20" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L20" s="4" t="str" cm="1">
+        <f t="array" ref="L20">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Vanguard Real Estate ETF</v>
       </c>
       <c r="M20" s="4" t="s">
@@ -5068,7 +5143,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>421</v>
+        <v>509</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>404</v>
@@ -5086,9 +5161,9 @@
       <c r="K21" s="4">
         <v>0</v>
       </c>
-      <c r="L21" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>AI</v>
+      <c r="L21" s="4" t="str" cm="1">
+        <f t="array" ref="L21">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>455</v>
@@ -5137,8 +5212,8 @@
       <c r="K22" s="4">
         <v>0</v>
       </c>
-      <c r="L22" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L22" s="4" t="str" cm="1">
+        <f t="array" ref="L22">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Clean Energy</v>
       </c>
       <c r="M22" s="4" t="s">
@@ -5190,8 +5265,8 @@
       <c r="K23" s="4">
         <v>0</v>
       </c>
-      <c r="L23" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L23" s="4" t="str" cm="1">
+        <f t="array" ref="L23">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Preferred</v>
       </c>
       <c r="M23" s="4" t="s">
@@ -5247,8 +5322,8 @@
       <c r="K24" s="4">
         <v>0</v>
       </c>
-      <c r="L24" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L24" s="4" t="str" cm="1">
+        <f t="array" ref="L24">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Eurostoxx 50</v>
       </c>
       <c r="M24" s="4" t="s">
@@ -5300,8 +5375,8 @@
       <c r="K25" s="4">
         <v>0</v>
       </c>
-      <c r="L25" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L25" s="4" t="str" cm="1">
+        <f t="array" ref="L25">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Eurostoxx Banks</v>
       </c>
       <c r="M25" s="4" t="s">
@@ -5334,7 +5409,9 @@
         <v>86</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>510</v>
+      </c>
       <c r="F26" s="4" t="s">
         <v>87</v>
       </c>
@@ -5353,9 +5430,9 @@
       <c r="K26" s="4">
         <v>0</v>
       </c>
-      <c r="L26" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares FTSE United Kingdom ETF</v>
+      <c r="L26" s="4" t="str" cm="1">
+        <f t="array" ref="L26">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>FTSE 100</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>455</v>
@@ -5410,8 +5487,8 @@
       <c r="K27" s="4">
         <v>0</v>
       </c>
-      <c r="L27" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L27" s="4" t="str" cm="1">
+        <f t="array" ref="L27">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>DAX (Germany)</v>
       </c>
       <c r="M27" s="4" t="s">
@@ -5444,7 +5521,9 @@
         <v>89</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>511</v>
+      </c>
       <c r="F28" s="4" t="s">
         <v>90</v>
       </c>
@@ -5463,9 +5542,9 @@
       <c r="K28" s="4">
         <v>0</v>
       </c>
-      <c r="L28" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares MSCI Canada ETF</v>
+      <c r="L28" s="4" t="str" cm="1">
+        <f t="array" ref="L28">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>MSCI Canada</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>455</v>
@@ -5516,8 +5595,8 @@
       <c r="K29" s="4">
         <v>0</v>
       </c>
-      <c r="L29" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L29" s="4" t="str" cm="1">
+        <f t="array" ref="L29">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>FTSE MIB (Italy)</v>
       </c>
       <c r="M29" s="4" t="s">
@@ -5573,8 +5652,8 @@
       <c r="K30" s="4">
         <v>0</v>
       </c>
-      <c r="L30" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L30" s="4" t="str" cm="1">
+        <f t="array" ref="L30">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CAC 40 (France)</v>
       </c>
       <c r="M30" s="4" t="s">
@@ -5607,7 +5686,9 @@
         <v>93</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>512</v>
+      </c>
       <c r="F31" s="4" t="s">
         <v>94</v>
       </c>
@@ -5626,9 +5707,9 @@
       <c r="K31" s="4">
         <v>0</v>
       </c>
-      <c r="L31" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares MSCI Italy ETF</v>
+      <c r="L31" s="4" t="str" cm="1">
+        <f t="array" ref="L31">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>MSCI Italy</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>455</v>
@@ -5665,9 +5746,7 @@
       <c r="E32" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
         <v>121</v>
       </c>
@@ -5683,8 +5762,8 @@
       <c r="K32" s="4">
         <v>0</v>
       </c>
-      <c r="L32" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L32" s="4" t="str" cm="1">
+        <f t="array" ref="L32">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>IBEX 35 (Spain)</v>
       </c>
       <c r="M32" s="4" t="s">
@@ -5717,7 +5796,9 @@
         <v>91</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>513</v>
+      </c>
       <c r="F33" s="4" t="s">
         <v>92</v>
       </c>
@@ -5736,9 +5817,9 @@
       <c r="K33" s="4">
         <v>0</v>
       </c>
-      <c r="L33" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares MSCI Spain ETF</v>
+      <c r="L33" s="4" t="str" cm="1">
+        <f t="array" ref="L33">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>MSCI Spain</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>455</v>
@@ -5793,8 +5874,8 @@
       <c r="K34" s="4">
         <v>0</v>
       </c>
-      <c r="L34" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L34" s="4" t="str" cm="1">
+        <f t="array" ref="L34">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Nikkei 225</v>
       </c>
       <c r="M34" s="4" t="s">
@@ -5850,8 +5931,8 @@
       <c r="K35" s="4">
         <v>0</v>
       </c>
-      <c r="L35" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L35" s="4" t="str" cm="1">
+        <f t="array" ref="L35">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>TOPIX</v>
       </c>
       <c r="M35" s="4" t="s">
@@ -5869,7 +5950,7 @@
         <v>TPX</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="S35" t="b">
         <v>1</v>
@@ -5888,7 +5969,9 @@
       <c r="D36" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>514</v>
+      </c>
       <c r="F36" s="4" t="s">
         <v>81</v>
       </c>
@@ -5907,9 +5990,9 @@
       <c r="K36" s="4">
         <v>0</v>
       </c>
-      <c r="L36" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares China Large-Cap ETF</v>
+      <c r="L36" s="4" t="str" cm="1">
+        <f t="array" ref="L36">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>China Large-Cap</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>455</v>
@@ -5943,7 +6026,9 @@
       <c r="D37" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="F37" s="4" t="s">
         <v>83</v>
       </c>
@@ -5962,9 +6047,9 @@
       <c r="K37" s="4">
         <v>0</v>
       </c>
-      <c r="L37" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+      <c r="L37" s="4" t="str" cm="1">
+        <f t="array" ref="L37">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>CSI 300 (China)</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>455</v>
@@ -5998,7 +6083,9 @@
       <c r="D38" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>515</v>
+      </c>
       <c r="F38" s="4" t="s">
         <v>401</v>
       </c>
@@ -6015,9 +6102,9 @@
       <c r="K38" s="4">
         <v>0</v>
       </c>
-      <c r="L38" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>KraneShares CSI China Internet ETF</v>
+      <c r="L38" s="4" t="str" cm="1">
+        <f t="array" ref="L38">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>CSI China Internet</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>455</v>
@@ -6049,9 +6136,13 @@
         <v>199</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>516</v>
+      </c>
       <c r="H39" s="4">
         <v>1</v>
       </c>
@@ -6064,9 +6155,9 @@
       <c r="K39" s="4">
         <v>0</v>
       </c>
-      <c r="L39" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L39" s="4" t="str" cm="1">
+        <f t="array" ref="L39">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>MSCI EM</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>455</v>
@@ -6119,8 +6210,8 @@
       <c r="K40" s="4">
         <v>0</v>
       </c>
-      <c r="L40" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L40" s="4" t="str" cm="1">
+        <f t="array" ref="L40">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares iBoxx $ Investment Grade Corporate Bond ETF</v>
       </c>
       <c r="M40" s="4" t="s">
@@ -6155,11 +6246,11 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>490</v>
-      </c>
       <c r="H41" s="4">
         <v>1</v>
       </c>
@@ -6172,8 +6263,8 @@
       <c r="K41" s="4">
         <v>0</v>
       </c>
-      <c r="L41" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L41" s="4" t="str" cm="1">
+        <f t="array" ref="L41">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Vanguard Short-Term Bond Index Fund ETF</v>
       </c>
       <c r="M41" s="4" t="s">
@@ -6227,8 +6318,8 @@
       <c r="K42" s="4">
         <v>0</v>
       </c>
-      <c r="L42" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L42" s="4" t="str" cm="1">
+        <f t="array" ref="L42">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares iBoxx $ High Yield Corporate Bond ETF</v>
       </c>
       <c r="M42" s="4" t="s">
@@ -6263,9 +6354,13 @@
       <c r="D43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>527</v>
+      </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="4" t="s">
+        <v>406</v>
+      </c>
       <c r="H43" s="4">
         <v>1</v>
       </c>
@@ -6278,9 +6373,9 @@
       <c r="K43" s="4">
         <v>0</v>
       </c>
-      <c r="L43" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L43" s="4" t="str" cm="1">
+        <f t="array" ref="L43">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>Hedged LQD</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>455</v>
@@ -6314,9 +6409,13 @@
       <c r="D44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>526</v>
+      </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>408</v>
+      </c>
       <c r="H44" s="4">
         <v>1</v>
       </c>
@@ -6329,9 +6428,9 @@
       <c r="K44" s="4">
         <v>0</v>
       </c>
-      <c r="L44" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L44" s="4" t="str" cm="1">
+        <f t="array" ref="L44">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>Hedged HYG</v>
       </c>
       <c r="M44" s="4" t="s">
         <v>455</v>
@@ -6363,9 +6462,13 @@
         <v>218</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>518</v>
+      </c>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>517</v>
+      </c>
       <c r="H45" s="4">
         <v>1</v>
       </c>
@@ -6378,9 +6481,9 @@
       <c r="K45" s="4">
         <v>0</v>
       </c>
-      <c r="L45" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L45" s="4" t="str" cm="1">
+        <f t="array" ref="L45">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>US Agg</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>455</v>
@@ -6415,7 +6518,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>468</v>
+        <v>519</v>
       </c>
       <c r="H46" s="4">
         <v>1</v>
@@ -6429,9 +6532,9 @@
       <c r="K46" s="4">
         <v>0</v>
       </c>
-      <c r="L46" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L46" s="4" t="str" cm="1">
+        <f t="array" ref="L46">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>CBOE Interest Rate 10 Year</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>455</v>
@@ -6465,7 +6568,10 @@
       <c r="D47" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="str">
+        <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(data[[#This Row],[Description_GPT]],"iShares ")," Bond")</f>
+        <v>1-3 Year Treasury</v>
+      </c>
       <c r="F47" s="4" t="s">
         <v>52</v>
       </c>
@@ -6484,9 +6590,9 @@
       <c r="K47" s="4">
         <v>0</v>
       </c>
-      <c r="L47" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+      <c r="L47" s="4" t="str" cm="1">
+        <f t="array" ref="L47">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>1-3 Year Treasury</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>455</v>
@@ -6520,7 +6626,10 @@
       <c r="D48" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4" t="str">
+        <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(data[[#This Row],[Description_GPT]],"iShares ")," Bond")</f>
+        <v>3-7 Year Treasury</v>
+      </c>
       <c r="F48" s="4" t="s">
         <v>127</v>
       </c>
@@ -6539,9 +6648,9 @@
       <c r="K48" s="4">
         <v>0</v>
       </c>
-      <c r="L48" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+      <c r="L48" s="4" t="str" cm="1">
+        <f t="array" ref="L48">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>3-7 Year Treasury</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>455</v>
@@ -6575,7 +6684,10 @@
       <c r="D49" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4" t="str">
+        <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(data[[#This Row],[Description_GPT]],"iShares ")," Bond")</f>
+        <v>7-10 Year Treasury</v>
+      </c>
       <c r="F49" s="4" t="s">
         <v>132</v>
       </c>
@@ -6594,9 +6706,9 @@
       <c r="K49" s="4">
         <v>0</v>
       </c>
-      <c r="L49" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+      <c r="L49" s="4" t="str" cm="1">
+        <f t="array" ref="L49">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>7-10 Year Treasury</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>455</v>
@@ -6630,7 +6742,10 @@
       <c r="D50" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4" t="str">
+        <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(data[[#This Row],[Description_GPT]],"iShares ")," Bond")</f>
+        <v>20+ Year Treasury</v>
+      </c>
       <c r="F50" s="4" t="s">
         <v>50</v>
       </c>
@@ -6649,9 +6764,9 @@
       <c r="K50" s="4">
         <v>0</v>
       </c>
-      <c r="L50" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+      <c r="L50" s="4" t="str" cm="1">
+        <f t="array" ref="L50">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>20+ Year Treasury</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>455</v>
@@ -6702,8 +6817,8 @@
       <c r="K51" s="4">
         <v>0</v>
       </c>
-      <c r="L51" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L51" s="4" t="str" cm="1">
+        <f t="array" ref="L51">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares TIPS Bond ETF</v>
       </c>
       <c r="M51" s="4" t="s">
@@ -6738,7 +6853,9 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="G52" s="4" t="s">
+        <v>520</v>
+      </c>
       <c r="H52" s="4">
         <v>1</v>
       </c>
@@ -6751,7 +6868,10 @@
       <c r="K52" s="4">
         <v>0</v>
       </c>
-      <c r="L52" s="4"/>
+      <c r="L52" s="4" t="str" cm="1">
+        <f t="array" ref="L52">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>Short-Term Inflation-Protected Securities ETF</v>
+      </c>
       <c r="M52" s="4" t="s">
         <v>455</v>
       </c>
@@ -6801,8 +6921,8 @@
       <c r="K53" s="4">
         <v>0</v>
       </c>
-      <c r="L53" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L53" s="4" t="str" cm="1">
+        <f t="array" ref="L53">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares MBS ETF</v>
       </c>
       <c r="M53" s="4" t="s">
@@ -6854,8 +6974,8 @@
       <c r="K54" s="4">
         <v>0</v>
       </c>
-      <c r="L54" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L54" s="4" t="str" cm="1">
+        <f t="array" ref="L54">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Simplify Mortgage Backed Securities ETF</v>
       </c>
       <c r="M54" s="4" t="s">
@@ -6907,8 +7027,8 @@
       <c r="K55" s="4">
         <v>0</v>
       </c>
-      <c r="L55" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L55" s="4" t="str" cm="1">
+        <f t="array" ref="L55">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>AGNC Investment Corp.</v>
       </c>
       <c r="M55" s="4" t="s">
@@ -6943,7 +7063,9 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
+      <c r="G56" s="4" t="s">
+        <v>521</v>
+      </c>
       <c r="H56" s="4">
         <v>1</v>
       </c>
@@ -6956,9 +7078,9 @@
       <c r="K56" s="4">
         <v>0</v>
       </c>
-      <c r="L56" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L56" s="4" t="str" cm="1">
+        <f t="array" ref="L56">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>Mortgage-Backed Securities ETF</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>455</v>
@@ -6992,7 +7114,9 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>417</v>
+      </c>
       <c r="H57" s="4">
         <v>1</v>
       </c>
@@ -7005,9 +7129,9 @@
       <c r="K57" s="4">
         <v>0</v>
       </c>
-      <c r="L57" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L57" s="4" t="str" cm="1">
+        <f t="array" ref="L57">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>iShares CMBS ETF</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>455</v>
@@ -7058,8 +7182,8 @@
       <c r="K58" s="4">
         <v>0</v>
       </c>
-      <c r="L58" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L58" s="4" t="str" cm="1">
+        <f t="array" ref="L58">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares J.P. Morgan USD Emerging Markets Bond ETF</v>
       </c>
       <c r="M58" s="4" t="s">
@@ -7094,7 +7218,9 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>522</v>
+      </c>
       <c r="H59" s="4">
         <v>0</v>
       </c>
@@ -7107,9 +7233,9 @@
       <c r="K59" s="4">
         <v>0</v>
       </c>
-      <c r="L59" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L59" s="4" t="str" cm="1">
+        <f t="array" ref="L59">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>iShares JP Morgan EM High Yield Bond ETF</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>455</v>
@@ -7158,8 +7284,8 @@
       <c r="K60" s="4">
         <v>0</v>
       </c>
-      <c r="L60" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L60" s="4" t="str" cm="1">
+        <f t="array" ref="L60">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>WisdomTree Emerging Markets Local Debt Fund</v>
       </c>
       <c r="M60" s="4" t="s">
@@ -7211,8 +7337,8 @@
       <c r="K61" s="4">
         <v>0</v>
       </c>
-      <c r="L61" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L61" s="4" t="str" cm="1">
+        <f t="array" ref="L61">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares International Government Bonds ETF</v>
       </c>
       <c r="M61" s="4" t="s">
@@ -7264,8 +7390,8 @@
       <c r="K62" s="4">
         <v>0</v>
       </c>
-      <c r="L62" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L62" s="4" t="str" cm="1">
+        <f t="array" ref="L62">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>SPDR Gold Shares</v>
       </c>
       <c r="M62" s="4" t="s">
@@ -7317,8 +7443,8 @@
       <c r="K63" s="4">
         <v>0</v>
       </c>
-      <c r="L63" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L63" s="4" t="str" cm="1">
+        <f t="array" ref="L63">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>iShares Silver Trust</v>
       </c>
       <c r="M63" s="4" t="s">
@@ -7370,8 +7496,8 @@
       <c r="K64" s="4">
         <v>0</v>
       </c>
-      <c r="L64" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L64" s="4" t="str" cm="1">
+        <f t="array" ref="L64">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>United States Oil Fund</v>
       </c>
       <c r="M64" s="4" t="s">
@@ -7423,8 +7549,8 @@
       <c r="K65" s="4">
         <v>0</v>
       </c>
-      <c r="L65" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L65" s="4" t="str" cm="1">
+        <f t="array" ref="L65">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Invesco DB Commodity Index Tracking Fund</v>
       </c>
       <c r="M65" s="4" t="s">
@@ -7476,8 +7602,8 @@
       <c r="K66" s="4">
         <v>0</v>
       </c>
-      <c r="L66" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L66" s="4" t="str" cm="1">
+        <f t="array" ref="L66">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Invesco DB US Dollar Index Bullish Fund</v>
       </c>
       <c r="M66" s="4" t="s">
@@ -7507,10 +7633,10 @@
         <v>40</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>493</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>494</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -7529,9 +7655,9 @@
       <c r="K67" s="4">
         <v>0</v>
       </c>
-      <c r="L67" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L67" s="4" t="str" cm="1">
+        <f t="array" ref="L67">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>U.S. Dollar Index</v>
       </c>
       <c r="M67" s="4" t="s">
         <v>455</v>
@@ -7562,7 +7688,9 @@
       <c r="C68" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4" t="s">
         <v>70</v>
@@ -7582,8 +7710,8 @@
       <c r="K68" s="4">
         <v>0</v>
       </c>
-      <c r="L68" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L68" s="4" t="str" cm="1">
+        <f t="array" ref="L68">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Invesco CurrencyShares Euro Trust</v>
       </c>
       <c r="M68" s="4" t="s">
@@ -7615,6 +7743,9 @@
       <c r="C69" t="s">
         <v>72</v>
       </c>
+      <c r="D69" t="s">
+        <v>524</v>
+      </c>
       <c r="F69" t="s">
         <v>73</v>
       </c>
@@ -7633,8 +7764,8 @@
       <c r="K69" s="4">
         <v>0</v>
       </c>
-      <c r="L69" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L69" s="4" t="str" cm="1">
+        <f t="array" ref="L69">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Invesco CurrencyShares Japanese Yen Trust</v>
       </c>
       <c r="M69" s="4" t="s">
@@ -7664,14 +7795,17 @@
         <v>71</v>
       </c>
       <c r="C70" t="s">
+        <v>498</v>
+      </c>
+      <c r="D70" t="s">
+        <v>525</v>
+      </c>
+      <c r="F70" t="s">
         <v>499</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>500</v>
       </c>
-      <c r="G70" t="s">
-        <v>501</v>
-      </c>
       <c r="H70" s="4">
         <v>1</v>
       </c>
@@ -7684,8 +7818,8 @@
       <c r="K70" s="4">
         <v>0</v>
       </c>
-      <c r="L70" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L70" s="4" t="str" cm="1">
+        <f t="array" ref="L70">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Invesco CurrencyShares Swiss Franc Trust</v>
       </c>
       <c r="M70" s="4" t="s">
@@ -7709,18 +7843,18 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4">
@@ -7735,8 +7869,8 @@
       <c r="K71" s="4">
         <v>0</v>
       </c>
-      <c r="L71" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L71" s="4" t="str" cm="1">
+        <f t="array" ref="L71">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CBOE Volatility Index</v>
       </c>
       <c r="M71" s="4" t="s">
@@ -7760,18 +7894,18 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4">
@@ -7786,8 +7920,8 @@
       <c r="K72" s="4">
         <v>0</v>
       </c>
-      <c r="L72" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L72" s="4" t="str" cm="1">
+        <f t="array" ref="L72">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>VIX Short-Term Futures ETN</v>
       </c>
       <c r="M72" s="4" t="s">
@@ -7811,18 +7945,18 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4">
@@ -7837,8 +7971,8 @@
       <c r="K73" s="4">
         <v>0</v>
       </c>
-      <c r="L73" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L73" s="4" t="str" cm="1">
+        <f t="array" ref="L73">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CBOE S&amp;P 500 3-Month Volatility</v>
       </c>
       <c r="M73" s="4" t="s">
@@ -7862,18 +7996,18 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4">
@@ -7888,8 +8022,8 @@
       <c r="K74" s="4">
         <v>0</v>
       </c>
-      <c r="L74" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L74" s="4" t="str" cm="1">
+        <f t="array" ref="L74">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CBOE VIX VOLATILITY INDEX</v>
       </c>
       <c r="M74" s="4" t="s">
@@ -7913,18 +8047,18 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="4">
@@ -7939,8 +8073,8 @@
       <c r="K75" s="4">
         <v>0</v>
       </c>
-      <c r="L75" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L75" s="4" t="str" cm="1">
+        <f t="array" ref="L75">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>ICE BofAML MOVE Index</v>
       </c>
       <c r="M75" s="4" t="s">
@@ -7964,18 +8098,18 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4">
@@ -7990,8 +8124,8 @@
       <c r="K76" s="4">
         <v>0</v>
       </c>
-      <c r="L76" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L76" s="4" t="str" cm="1">
+        <f t="array" ref="L76">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CBOE Crude Oil Volatility Index</v>
       </c>
       <c r="M76" s="4" t="s">
@@ -8015,18 +8149,18 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="4">
@@ -8041,8 +8175,8 @@
       <c r="K77" s="4">
         <v>0</v>
       </c>
-      <c r="L77" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L77" s="4" t="str" cm="1">
+        <f t="array" ref="L77">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CBOE Euro currency Volatility I</v>
       </c>
       <c r="M77" s="4" t="s">
@@ -8066,18 +8200,18 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4">
@@ -8092,8 +8226,8 @@
       <c r="K78" s="4">
         <v>0</v>
       </c>
-      <c r="L78" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L78" s="4" t="str" cm="1">
+        <f t="array" ref="L78">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>CBOE Gold Volatility Index</v>
       </c>
       <c r="M78" s="4" t="s">
@@ -8117,18 +8251,18 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4">
@@ -8143,8 +8277,8 @@
       <c r="K79" s="4">
         <v>0</v>
       </c>
-      <c r="L79" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
+      <c r="L79" s="4" t="str" cm="1">
+        <f t="array" ref="L79">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
         <v>Cboe Implied Correlation Index</v>
       </c>
       <c r="M79" s="4" t="s">
@@ -8179,9 +8313,11 @@
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
+      <c r="G80" s="4" t="s">
+        <v>523</v>
+      </c>
       <c r="H80" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80" s="4">
         <v>1</v>
@@ -8190,11 +8326,11 @@
         <v>0</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="L80" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+        <v>487</v>
+      </c>
+      <c r="L80" s="4" t="str" cm="1">
+        <f t="array" ref="L80">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>TCW MetWest Total Return Bd I</v>
       </c>
       <c r="M80" s="4" t="s">
         <v>455</v>
@@ -8216,38 +8352,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>128</v>
+        <v>444</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>429</v>
+        <v>508</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
+      <c r="G81" s="4" t="str" cm="1">
+        <f t="array" ref="G81">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>XLF 1.5, ICLN -1, IWM 1.5, FEZ -1</v>
+      </c>
       <c r="H81" s="4">
         <v>1</v>
       </c>
       <c r="I81" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K81" s="4">
         <v>0</v>
       </c>
-      <c r="L81" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L81" s="4" t="str" cm="1">
+        <f t="array" ref="L81">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>XLF 1.5, ICLN -1, IWM 1.5, FEZ -1</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="N81" s="4" t="s">
         <v>454</v>
@@ -8258,15 +8397,18 @@
       </c>
       <c r="P81" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>MWTIX</v>
+        <v>ELECTION</v>
       </c>
       <c r="Q81" s="4"/>
-      <c r="R81" s="2"/>
       <c r="S81" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U81" s="11" cm="1">
+        <f t="array" ref="U81:U84">_xlfn._xlws.FILTER(composities[weight],composities[portfolio_name]=data[[#This Row],[factor_name]])</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>444</v>
       </c>
@@ -8274,12 +8416,15 @@
         <v>40</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>509</v>
+        <v>439</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
+      <c r="G82" s="4" t="str" cm="1">
+        <f t="array" ref="G82">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>SHY 1, BSV 1</v>
+      </c>
       <c r="H82" s="4">
         <v>1</v>
       </c>
@@ -8292,9 +8437,9 @@
       <c r="K82" s="4">
         <v>0</v>
       </c>
-      <c r="L82" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L82" s="4" t="str" cm="1">
+        <f t="array" ref="L82">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>SHY 1, BSV 1</v>
       </c>
       <c r="M82" s="4" t="s">
         <v>445</v>
@@ -8308,14 +8453,17 @@
       </c>
       <c r="P82" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>ELECTION</v>
+        <v>FED</v>
       </c>
       <c r="Q82" s="4"/>
       <c r="S82" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U82">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>444</v>
       </c>
@@ -8323,12 +8471,15 @@
         <v>40</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
+      <c r="G83" s="4" t="str" cm="1">
+        <f t="array" ref="G83">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>AIQ 1, QQQ 0.25, IWM -0.25</v>
+      </c>
       <c r="H83" s="4">
         <v>1</v>
       </c>
@@ -8341,9 +8492,9 @@
       <c r="K83" s="4">
         <v>0</v>
       </c>
-      <c r="L83" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L83" s="4" t="str" cm="1">
+        <f t="array" ref="L83">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>AIQ 1, QQQ 0.25, IWM -0.25</v>
       </c>
       <c r="M83" s="4" t="s">
         <v>445</v>
@@ -8357,14 +8508,17 @@
       </c>
       <c r="P83" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>FED</v>
+        <v>AI</v>
       </c>
       <c r="Q83" s="4"/>
       <c r="S83" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U83">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>444</v>
       </c>
@@ -8372,12 +8526,15 @@
         <v>40</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>421</v>
+        <v>450</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
+      <c r="G84" s="4" t="str" cm="1">
+        <f t="array" ref="G84">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>GLD 0.75, USO 0.25</v>
+      </c>
       <c r="H84" s="4">
         <v>1</v>
       </c>
@@ -8390,9 +8547,9 @@
       <c r="K84" s="4">
         <v>0</v>
       </c>
-      <c r="L84" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L84" s="4" t="str" cm="1">
+        <f t="array" ref="L84">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>GLD 0.75, USO 0.25</v>
       </c>
       <c r="M84" s="4" t="s">
         <v>445</v>
@@ -8406,27 +8563,33 @@
       </c>
       <c r="P84" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>AI</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="Q84" s="4"/>
       <c r="S84" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U84">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>444</v>
+        <v>128</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
+      <c r="G85" s="4" t="str" cm="1">
+        <f t="array" ref="G85">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>SHY -3.86, IEF 1</v>
+      </c>
       <c r="H85" s="4">
         <v>1</v>
       </c>
@@ -8439,9 +8602,9 @@
       <c r="K85" s="4">
         <v>0</v>
       </c>
-      <c r="L85" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L85" s="4" t="str" cm="1">
+        <f t="array" ref="L85">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>SHY -3.86, IEF 1</v>
       </c>
       <c r="M85" s="4" t="s">
         <v>445</v>
@@ -8455,27 +8618,32 @@
       </c>
       <c r="P85" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>GEOPOLITICS</v>
+        <v>2s10s</v>
       </c>
       <c r="Q85" s="4"/>
       <c r="S85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>451</v>
+        <v>504</v>
       </c>
       <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
+      <c r="E86" s="4" t="s">
+        <v>506</v>
+      </c>
       <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
+      <c r="G86" s="4" t="str" cm="1">
+        <f t="array" ref="G86">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>XLP 1, XLY -1</v>
+      </c>
       <c r="H86" s="4">
         <v>1</v>
       </c>
@@ -8488,9 +8656,9 @@
       <c r="K86" s="4">
         <v>0</v>
       </c>
-      <c r="L86" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
+      <c r="L86" s="4" t="str" cm="1">
+        <f t="array" ref="L86">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>Staples/Discretionary</v>
       </c>
       <c r="M86" s="4" t="s">
         <v>445</v>
@@ -8504,29 +8672,30 @@
       </c>
       <c r="P86" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>2s10s</v>
+        <v>XLPXLY</v>
       </c>
       <c r="Q86" s="4"/>
       <c r="S86" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>39</v>
+        <v>444</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D87" s="4"/>
-      <c r="E87" s="4" t="s">
-        <v>507</v>
-      </c>
+      <c r="E87" s="4"/>
       <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4" t="str" cm="1">
+        <f t="array" ref="G87">_xlfn.XLOOKUP(data[[#This Row],[factor_name]],_xlfn.ANCHORARRAY(composites!$F$2),_xlfn.ANCHORARRAY(composites!$G$2))</f>
+        <v>GLD 0.21, FXY 0.30, FXF 0.37, ^VIX3M -0.04, XLP 0.15, XLY -0.15</v>
+      </c>
       <c r="H87" s="4">
         <v>1</v>
       </c>
@@ -8539,9 +8708,9 @@
       <c r="K87" s="4">
         <v>0</v>
       </c>
-      <c r="L87" s="4" t="str">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>Staples/Discretionary</v>
+      <c r="L87" s="4" t="str" cm="1">
+        <f t="array" ref="L87">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>GLD 0.21, FXY 0.30, FXF 0.37, ^VIX3M -0.04, XLP 0.15, XLY -0.15</v>
       </c>
       <c r="M87" s="4" t="s">
         <v>445</v>
@@ -8555,65 +8724,16 @@
       </c>
       <c r="P87" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
-        <v>XLPXLY</v>
+        <v>TRADEWAR</v>
       </c>
       <c r="Q87" s="4"/>
       <c r="S87" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4">
-        <v>1</v>
-      </c>
-      <c r="I88" s="4">
-        <v>1</v>
-      </c>
-      <c r="J88" s="4">
-        <v>1</v>
-      </c>
-      <c r="K88" s="4">
-        <v>0</v>
-      </c>
-      <c r="L88" s="4">
-        <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
-        <v>0</v>
-      </c>
-      <c r="M88" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="N88" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="O88" s="4" cm="1">
-        <f t="array" ref="O88">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",1,1)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="P88" s="4" t="str">
-        <f>data[[#This Row],[factor_name]]</f>
-        <v>TRADEWAR</v>
-      </c>
-      <c r="Q88" s="4"/>
-      <c r="S88" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:Q88">
+  <conditionalFormatting sqref="A82:Q87 A81:F81 H81:Q81 U81 A2:Q80">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>$S2</formula>
     </cfRule>
@@ -8801,7 +8921,10 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8838,7 +8961,7 @@
         <v>464</v>
       </c>
       <c r="J1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -9468,7 +9591,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>AI</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="G21" t="str">
         <v>yfinance</v>
@@ -9596,7 +9719,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
+        <v>FTSE 100</v>
       </c>
       <c r="G25" t="str">
         <v>yfinance</v>
@@ -9660,7 +9783,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="str">
-        <v>iShares MSCI Canada ETF</v>
+        <v>MSCI Canada</v>
       </c>
       <c r="G27" t="str">
         <v>yfinance</v>
@@ -9692,7 +9815,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="str">
-        <v>iShares MSCI Italy ETF</v>
+        <v>MSCI Italy</v>
       </c>
       <c r="G28" t="str">
         <v>yfinance</v>
@@ -9756,7 +9879,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="str">
-        <v>iShares China Large-Cap ETF</v>
+        <v>China Large-Cap</v>
       </c>
       <c r="G30" t="str">
         <v>yfinance</v>
@@ -9788,7 +9911,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+        <v>CSI 300 (China)</v>
       </c>
       <c r="G31" t="str">
         <v>yfinance</v>
@@ -9820,7 +9943,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
+        <v>CSI China Internet</v>
       </c>
       <c r="G32" t="str">
         <v>yfinance</v>
@@ -9851,8 +9974,8 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>0</v>
+      <c r="F33" t="str">
+        <v>MSCI EM</v>
       </c>
       <c r="G33" t="str">
         <v>yfinance</v>
@@ -9979,8 +10102,8 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="str">
+        <v>Hedged LQD</v>
       </c>
       <c r="G37" t="str">
         <v>yfinance</v>
@@ -10011,8 +10134,8 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>0</v>
+      <c r="F38" t="str">
+        <v>Hedged HYG</v>
       </c>
       <c r="G38" t="str">
         <v>yfinance</v>
@@ -10043,8 +10166,8 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" t="str">
+        <v>US Agg</v>
       </c>
       <c r="G39" t="str">
         <v>yfinance</v>
@@ -10075,8 +10198,8 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>0</v>
+      <c r="F40" t="str">
+        <v>CBOE Interest Rate 10 Year</v>
       </c>
       <c r="G40" t="str">
         <v>yfinance</v>
@@ -10108,7 +10231,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+        <v>1-3 Year Treasury</v>
       </c>
       <c r="G41" t="str">
         <v>yfinance</v>
@@ -10140,7 +10263,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>3-7 Year Treasury</v>
       </c>
       <c r="G42" t="str">
         <v>yfinance</v>
@@ -10172,7 +10295,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>7-10 Year Treasury</v>
       </c>
       <c r="G43" t="str">
         <v>yfinance</v>
@@ -10204,7 +10327,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>20+ Year Treasury</v>
       </c>
       <c r="G44" t="str">
         <v>yfinance</v>
@@ -10267,8 +10390,8 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="str">
+        <v>Short-Term Inflation-Protected Securities ETF</v>
       </c>
       <c r="G46" t="str">
         <v>yfinance</v>
@@ -10331,8 +10454,8 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="str">
+        <v>Mortgage-Backed Securities ETF</v>
       </c>
       <c r="G48" t="str">
         <v>yfinance</v>
@@ -10363,8 +10486,8 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
-        <v>0</v>
+      <c r="F49" t="str">
+        <v>iShares CMBS ETF</v>
       </c>
       <c r="G49" t="str">
         <v>yfinance</v>
@@ -10555,8 +10678,8 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
-        <v>0</v>
+      <c r="F55" t="str">
+        <v>U.S. Dollar Index</v>
       </c>
       <c r="G55" t="str">
         <v>yfinance</v>
@@ -10811,8 +10934,8 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
-        <v>0</v>
+      <c r="F63" t="str">
+        <v>TCW MetWest Total Return Bd I</v>
       </c>
       <c r="G63" t="str">
         <v>yfinance</v>
@@ -10843,8 +10966,8 @@
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="F64">
-        <v>0</v>
+      <c r="F64" t="str">
+        <v>XLF 1.5, ICLN -1, IWM 1.5, FEZ -1</v>
       </c>
       <c r="G64" t="str">
         <v>composite</v>
@@ -10875,8 +10998,8 @@
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65">
-        <v>0</v>
+      <c r="F65" t="str">
+        <v>SHY 1, BSV 1</v>
       </c>
       <c r="G65" t="str">
         <v>composite</v>
@@ -10907,8 +11030,8 @@
       <c r="E66">
         <v>1</v>
       </c>
-      <c r="F66">
-        <v>0</v>
+      <c r="F66" t="str">
+        <v>AIQ 1, QQQ 0.25, IWM -0.25</v>
       </c>
       <c r="G66" t="str">
         <v>composite</v>
@@ -10939,8 +11062,8 @@
       <c r="E67">
         <v>1</v>
       </c>
-      <c r="F67">
-        <v>0</v>
+      <c r="F67" t="str">
+        <v>GLD 0.75, USO 0.25</v>
       </c>
       <c r="G67" t="str">
         <v>composite</v>
@@ -10971,8 +11094,8 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68">
-        <v>0</v>
+      <c r="F68" t="str">
+        <v>SHY -3.86, IEF 1</v>
       </c>
       <c r="G68" t="str">
         <v>composite</v>
@@ -11035,8 +11158,8 @@
       <c r="E70">
         <v>1</v>
       </c>
-      <c r="F70">
-        <v>0</v>
+      <c r="F70" t="str">
+        <v>GLD 0.21, FXY 0.30, FXF 0.37, ^VIX3M -0.04, XLP 0.15, XLY -0.15</v>
       </c>
       <c r="G70" t="str">
         <v>composite</v>
@@ -11098,7 +11221,7 @@
         <v>464</v>
       </c>
       <c r="J1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -11728,7 +11851,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>AI</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="G21" t="str">
         <v>yfinance</v>
@@ -11856,7 +11979,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
+        <v>FTSE 100</v>
       </c>
       <c r="G25" t="str">
         <v>yfinance</v>
@@ -11920,7 +12043,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="str">
-        <v>iShares MSCI Canada ETF</v>
+        <v>MSCI Canada</v>
       </c>
       <c r="G27" t="str">
         <v>yfinance</v>
@@ -11952,7 +12075,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="str">
-        <v>iShares MSCI Italy ETF</v>
+        <v>MSCI Italy</v>
       </c>
       <c r="G28" t="str">
         <v>yfinance</v>
@@ -12016,7 +12139,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="str">
-        <v>iShares China Large-Cap ETF</v>
+        <v>China Large-Cap</v>
       </c>
       <c r="G30" t="str">
         <v>yfinance</v>
@@ -12048,7 +12171,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+        <v>CSI 300 (China)</v>
       </c>
       <c r="G31" t="str">
         <v>yfinance</v>
@@ -12080,7 +12203,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
+        <v>CSI China Internet</v>
       </c>
       <c r="G32" t="str">
         <v>yfinance</v>
@@ -12111,8 +12234,8 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>0</v>
+      <c r="F33" t="str">
+        <v>MSCI EM</v>
       </c>
       <c r="G33" t="str">
         <v>yfinance</v>
@@ -12239,8 +12362,8 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="str">
+        <v>Hedged LQD</v>
       </c>
       <c r="G37" t="str">
         <v>yfinance</v>
@@ -12271,8 +12394,8 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>0</v>
+      <c r="F38" t="str">
+        <v>Hedged HYG</v>
       </c>
       <c r="G38" t="str">
         <v>yfinance</v>
@@ -12303,8 +12426,8 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" t="str">
+        <v>US Agg</v>
       </c>
       <c r="G39" t="str">
         <v>yfinance</v>
@@ -12335,8 +12458,8 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>0</v>
+      <c r="F40" t="str">
+        <v>CBOE Interest Rate 10 Year</v>
       </c>
       <c r="G40" t="str">
         <v>yfinance</v>
@@ -12368,7 +12491,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+        <v>1-3 Year Treasury</v>
       </c>
       <c r="G41" t="str">
         <v>yfinance</v>
@@ -12400,7 +12523,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>3-7 Year Treasury</v>
       </c>
       <c r="G42" t="str">
         <v>yfinance</v>
@@ -12432,7 +12555,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>7-10 Year Treasury</v>
       </c>
       <c r="G43" t="str">
         <v>yfinance</v>
@@ -12464,7 +12587,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>20+ Year Treasury</v>
       </c>
       <c r="G44" t="str">
         <v>yfinance</v>
@@ -12527,8 +12650,8 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="str">
+        <v>Short-Term Inflation-Protected Securities ETF</v>
       </c>
       <c r="G46" t="str">
         <v>yfinance</v>
@@ -12591,8 +12714,8 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="str">
+        <v>Mortgage-Backed Securities ETF</v>
       </c>
       <c r="G48" t="str">
         <v>yfinance</v>
@@ -12623,8 +12746,8 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
-        <v>0</v>
+      <c r="F49" t="str">
+        <v>iShares CMBS ETF</v>
       </c>
       <c r="G49" t="str">
         <v>yfinance</v>
@@ -12815,8 +12938,8 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
-        <v>0</v>
+      <c r="F55" t="str">
+        <v>U.S. Dollar Index</v>
       </c>
       <c r="G55" t="str">
         <v>yfinance</v>
@@ -13071,8 +13194,8 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
-        <v>0</v>
+      <c r="F63" t="str">
+        <v>TCW MetWest Total Return Bd I</v>
       </c>
       <c r="G63" t="str">
         <v>yfinance</v>
@@ -13095,13 +13218,13 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G69" sqref="G69"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13138,16 +13261,16 @@
         <v>464</v>
       </c>
       <c r="J1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A70">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
+        <f t="array" ref="A2:A69">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J70">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J69">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -13768,7 +13891,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>AI</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="G21" t="str">
         <v>yfinance</v>
@@ -13896,7 +14019,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
+        <v>FTSE 100</v>
       </c>
       <c r="G25" t="str">
         <v>yfinance</v>
@@ -13960,7 +14083,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="str">
-        <v>iShares MSCI Canada ETF</v>
+        <v>MSCI Canada</v>
       </c>
       <c r="G27" t="str">
         <v>yfinance</v>
@@ -13992,7 +14115,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="str">
-        <v>iShares MSCI Italy ETF</v>
+        <v>MSCI Italy</v>
       </c>
       <c r="G28" t="str">
         <v>yfinance</v>
@@ -14056,7 +14179,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="str">
-        <v>iShares China Large-Cap ETF</v>
+        <v>China Large-Cap</v>
       </c>
       <c r="G30" t="str">
         <v>yfinance</v>
@@ -14088,7 +14211,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+        <v>CSI 300 (China)</v>
       </c>
       <c r="G31" t="str">
         <v>yfinance</v>
@@ -14120,7 +14243,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
+        <v>CSI China Internet</v>
       </c>
       <c r="G32" t="str">
         <v>yfinance</v>
@@ -14151,8 +14274,8 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>0</v>
+      <c r="F33" t="str">
+        <v>MSCI EM</v>
       </c>
       <c r="G33" t="str">
         <v>yfinance</v>
@@ -14279,8 +14402,8 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="str">
+        <v>Hedged LQD</v>
       </c>
       <c r="G37" t="str">
         <v>yfinance</v>
@@ -14311,8 +14434,8 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>0</v>
+      <c r="F38" t="str">
+        <v>Hedged HYG</v>
       </c>
       <c r="G38" t="str">
         <v>yfinance</v>
@@ -14343,8 +14466,8 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" t="str">
+        <v>US Agg</v>
       </c>
       <c r="G39" t="str">
         <v>yfinance</v>
@@ -14375,8 +14498,8 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>0</v>
+      <c r="F40" t="str">
+        <v>CBOE Interest Rate 10 Year</v>
       </c>
       <c r="G40" t="str">
         <v>yfinance</v>
@@ -14408,7 +14531,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+        <v>1-3 Year Treasury</v>
       </c>
       <c r="G41" t="str">
         <v>yfinance</v>
@@ -14440,7 +14563,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>3-7 Year Treasury</v>
       </c>
       <c r="G42" t="str">
         <v>yfinance</v>
@@ -14472,7 +14595,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>7-10 Year Treasury</v>
       </c>
       <c r="G43" t="str">
         <v>yfinance</v>
@@ -14504,7 +14627,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>20+ Year Treasury</v>
       </c>
       <c r="G44" t="str">
         <v>yfinance</v>
@@ -14567,8 +14690,8 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="F46" t="str">
+        <v>Short-Term Inflation-Protected Securities ETF</v>
       </c>
       <c r="G46" t="str">
         <v>yfinance</v>
@@ -14631,8 +14754,8 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="str">
+        <v>Mortgage-Backed Securities ETF</v>
       </c>
       <c r="G48" t="str">
         <v>yfinance</v>
@@ -14663,8 +14786,8 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
-        <v>0</v>
+      <c r="F49" t="str">
+        <v>iShares CMBS ETF</v>
       </c>
       <c r="G49" t="str">
         <v>yfinance</v>
@@ -14855,8 +14978,8 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
-        <v>0</v>
+      <c r="F55" t="str">
+        <v>U.S. Dollar Index</v>
       </c>
       <c r="G55" t="str">
         <v>yfinance</v>
@@ -15097,10 +15220,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
-        <v>MWTIX</v>
+        <v>ELECTION</v>
       </c>
       <c r="B63" t="str">
-        <v>Portfolio</v>
+        <v>Theme</v>
       </c>
       <c r="C63" t="str">
         <v>USD</v>
@@ -15109,16 +15232,16 @@
         <v>1</v>
       </c>
       <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F63" t="str">
+        <v>XLF 1.5, ICLN -1, IWM 1.5, FEZ -1</v>
       </c>
       <c r="G63" t="str">
-        <v>yfinance</v>
+        <v>composite</v>
       </c>
       <c r="H63" t="str">
-        <v>MWTIX</v>
+        <v>ELECTION</v>
       </c>
       <c r="I63" t="str">
         <v>lognormal</v>
@@ -15129,7 +15252,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
-        <v>ELECTION</v>
+        <v>FED</v>
       </c>
       <c r="B64" t="str">
         <v>Theme</v>
@@ -15143,14 +15266,14 @@
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="F64">
-        <v>0</v>
+      <c r="F64" t="str">
+        <v>SHY 1, BSV 1</v>
       </c>
       <c r="G64" t="str">
         <v>composite</v>
       </c>
       <c r="H64" t="str">
-        <v>ELECTION</v>
+        <v>FED</v>
       </c>
       <c r="I64" t="str">
         <v>lognormal</v>
@@ -15161,7 +15284,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
-        <v>FED</v>
+        <v>AI</v>
       </c>
       <c r="B65" t="str">
         <v>Theme</v>
@@ -15175,14 +15298,14 @@
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65">
-        <v>0</v>
+      <c r="F65" t="str">
+        <v>AIQ 1, QQQ 0.25, IWM -0.25</v>
       </c>
       <c r="G65" t="str">
         <v>composite</v>
       </c>
       <c r="H65" t="str">
-        <v>FED</v>
+        <v>AI</v>
       </c>
       <c r="I65" t="str">
         <v>lognormal</v>
@@ -15193,7 +15316,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
-        <v>AI</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="B66" t="str">
         <v>Theme</v>
@@ -15207,14 +15330,14 @@
       <c r="E66">
         <v>1</v>
       </c>
-      <c r="F66">
-        <v>0</v>
+      <c r="F66" t="str">
+        <v>GLD 0.75, USO 0.25</v>
       </c>
       <c r="G66" t="str">
         <v>composite</v>
       </c>
       <c r="H66" t="str">
-        <v>AI</v>
+        <v>GEOPOLITICS</v>
       </c>
       <c r="I66" t="str">
         <v>lognormal</v>
@@ -15225,10 +15348,10 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
-        <v>GEOPOLITICS</v>
+        <v>2s10s</v>
       </c>
       <c r="B67" t="str">
-        <v>Theme</v>
+        <v>Rates</v>
       </c>
       <c r="C67" t="str">
         <v>USD</v>
@@ -15239,14 +15362,14 @@
       <c r="E67">
         <v>1</v>
       </c>
-      <c r="F67">
-        <v>0</v>
+      <c r="F67" t="str">
+        <v>SHY -3.86, IEF 1</v>
       </c>
       <c r="G67" t="str">
         <v>composite</v>
       </c>
       <c r="H67" t="str">
-        <v>GEOPOLITICS</v>
+        <v>2s10s</v>
       </c>
       <c r="I67" t="str">
         <v>lognormal</v>
@@ -15257,10 +15380,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
-        <v>2s10s</v>
+        <v>XLPXLY</v>
       </c>
       <c r="B68" t="str">
-        <v>Rates</v>
+        <v>Equities</v>
       </c>
       <c r="C68" t="str">
         <v>USD</v>
@@ -15271,14 +15394,14 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68">
-        <v>0</v>
+      <c r="F68" t="str">
+        <v>Staples/Discretionary</v>
       </c>
       <c r="G68" t="str">
         <v>composite</v>
       </c>
       <c r="H68" t="str">
-        <v>2s10s</v>
+        <v>XLPXLY</v>
       </c>
       <c r="I68" t="str">
         <v>lognormal</v>
@@ -15289,10 +15412,10 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
-        <v>XLPXLY</v>
+        <v>TRADEWAR</v>
       </c>
       <c r="B69" t="str">
-        <v>Equities</v>
+        <v>Theme</v>
       </c>
       <c r="C69" t="str">
         <v>USD</v>
@@ -15304,50 +15427,18 @@
         <v>1</v>
       </c>
       <c r="F69" t="str">
-        <v>Staples/Discretionary</v>
+        <v>GLD 0.21, FXY 0.30, FXF 0.37, ^VIX3M -0.04, XLP 0.15, XLY -0.15</v>
       </c>
       <c r="G69" t="str">
         <v>composite</v>
       </c>
       <c r="H69" t="str">
-        <v>XLPXLY</v>
+        <v>TRADEWAR</v>
       </c>
       <c r="I69" t="str">
         <v>lognormal</v>
       </c>
       <c r="J69">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" t="str">
-        <v>TRADEWAR</v>
-      </c>
-      <c r="B70" t="str">
-        <v>Theme</v>
-      </c>
-      <c r="C70" t="str">
-        <v>USD</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70" t="str">
-        <v>composite</v>
-      </c>
-      <c r="H70" t="str">
-        <v>TRADEWAR</v>
-      </c>
-      <c r="I70" t="str">
-        <v>lognormal</v>
-      </c>
-      <c r="J70">
         <v>1E-4</v>
       </c>
     </row>
@@ -15937,7 +16028,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="str">
-        <v>AI</v>
+        <v>Artificial Intelligence</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -16005,7 +16096,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
+        <v>FTSE 100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -16039,7 +16130,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="str">
-        <v>iShares MSCI Canada ETF</v>
+        <v>MSCI Canada</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -16056,7 +16147,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="str">
-        <v>iShares MSCI Italy ETF</v>
+        <v>MSCI Italy</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -16090,7 +16181,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="str">
-        <v>iShares China Large-Cap ETF</v>
+        <v>China Large-Cap</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -16107,7 +16198,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+        <v>CSI 300 (China)</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -16124,7 +16215,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
+        <v>CSI China Internet</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -16140,8 +16231,8 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="E33">
-        <v>0</v>
+      <c r="E33" t="str">
+        <v>MSCI EM</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -16208,8 +16299,8 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37">
-        <v>0</v>
+      <c r="E37" t="str">
+        <v>Hedged LQD</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -16225,8 +16316,8 @@
       <c r="D38">
         <v>0</v>
       </c>
-      <c r="E38">
-        <v>0</v>
+      <c r="E38" t="str">
+        <v>Hedged HYG</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -16242,8 +16333,8 @@
       <c r="D39">
         <v>0</v>
       </c>
-      <c r="E39">
-        <v>0</v>
+      <c r="E39" t="str">
+        <v>US Agg</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -16259,8 +16350,8 @@
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="E40">
-        <v>0</v>
+      <c r="E40" t="str">
+        <v>CBOE Interest Rate 10 Year</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -16277,7 +16368,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+        <v>1-3 Year Treasury</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -16294,7 +16385,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>3-7 Year Treasury</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -16311,7 +16402,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>7-10 Year Treasury</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -16328,7 +16419,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>20+ Year Treasury</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -16361,8 +16452,8 @@
       <c r="D46">
         <v>0</v>
       </c>
-      <c r="E46">
-        <v>0</v>
+      <c r="E46" t="str">
+        <v>Short-Term Inflation-Protected Securities ETF</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -16395,8 +16486,8 @@
       <c r="D48">
         <v>0</v>
       </c>
-      <c r="E48">
-        <v>0</v>
+      <c r="E48" t="str">
+        <v>Mortgage-Backed Securities ETF</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -16412,8 +16503,8 @@
       <c r="D49">
         <v>0</v>
       </c>
-      <c r="E49">
-        <v>0</v>
+      <c r="E49" t="str">
+        <v>iShares CMBS ETF</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -16514,8 +16605,8 @@
       <c r="D55">
         <v>0</v>
       </c>
-      <c r="E55">
-        <v>0</v>
+      <c r="E55" t="str">
+        <v>U.S. Dollar Index</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -16650,8 +16741,8 @@
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63">
-        <v>0</v>
+      <c r="E63" t="str">
+        <v>TCW MetWest Total Return Bd I</v>
       </c>
     </row>
   </sheetData>
@@ -20531,7 +20622,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="str">
-        <v>iShares FTSE United Kingdom ETF</v>
+        <v>FTSE 100</v>
       </c>
       <c r="E27" t="str">
         <v>iShares FTSE United Kingdom ETF</v>
@@ -20585,7 +20676,7 @@
         <v>89</v>
       </c>
       <c r="D29" t="str">
-        <v>iShares MSCI Canada ETF</v>
+        <v>MSCI Canada</v>
       </c>
       <c r="E29" t="str">
         <v>iShares MSCI Canada ETF</v>
@@ -20666,7 +20757,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="str">
-        <v>iShares MSCI Italy ETF</v>
+        <v>MSCI Italy</v>
       </c>
       <c r="E32" t="str">
         <v>iShares MSCI Italy ETF</v>
@@ -20696,17 +20787,17 @@
         <v>IBEX 35 (Spain)</v>
       </c>
       <c r="E33" t="str">
-        <v>iShares MSCI Spain ETF</v>
+        <v>IBEX 35 ETF</v>
       </c>
       <c r="F33" t="e">
         <v>#N/A</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="M33" t="b">
-        <v>1</v>
-      </c>
-      <c r="N33" t="str">
-        <v>iShares MSCI Spain ETF</v>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33" t="e">
+        <v>#N/A</v>
       </c>
       <c r="O33" t="str">
         <v>IBEX 35 ETF</v>
@@ -20720,7 +20811,7 @@
         <v>91</v>
       </c>
       <c r="D34" t="str">
-        <v>iShares MSCI Spain ETF</v>
+        <v>MSCI Spain</v>
       </c>
       <c r="E34" t="str">
         <v>iShares MSCI Spain ETF</v>
@@ -20801,7 +20892,7 @@
         <v>80</v>
       </c>
       <c r="D37" t="str">
-        <v>iShares China Large-Cap ETF</v>
+        <v>China Large-Cap</v>
       </c>
       <c r="E37" t="str">
         <v>iShares China Large-Cap ETF</v>
@@ -20828,7 +20919,7 @@
         <v>82</v>
       </c>
       <c r="D38" t="str">
-        <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
+        <v>CSI 300 (China)</v>
       </c>
       <c r="E38" t="str">
         <v>Xtrackers Harvest CSI 300 China A-Shares ETF</v>
@@ -20855,7 +20946,7 @@
         <v>400</v>
       </c>
       <c r="D39" t="str">
-        <v>KraneShares CSI China Internet ETF</v>
+        <v>CSI China Internet</v>
       </c>
       <c r="E39" t="str">
         <v>KraneShares CSI China Internet ETF</v>
@@ -20935,8 +21026,8 @@
       <c r="C42" t="s">
         <v>347</v>
       </c>
-      <c r="D42">
-        <v>0</v>
+      <c r="D42" t="str">
+        <v>Hedged LQD</v>
       </c>
       <c r="E42" t="str">
         <v>iShares Interest Rate Hedged Corporate Bond ETF</v>
@@ -20962,8 +21053,8 @@
       <c r="C43" t="s">
         <v>348</v>
       </c>
-      <c r="D43">
-        <v>0</v>
+      <c r="D43" t="str">
+        <v>Hedged HYG</v>
       </c>
       <c r="E43" t="str">
         <v>iShares Interest Rate Hedged High Yield Bond ETF</v>
@@ -20990,7 +21081,7 @@
         <v>51</v>
       </c>
       <c r="D44" t="str">
-        <v>iShares 1-3 Year Treasury Bond ETF</v>
+        <v>1-3 Year Treasury</v>
       </c>
       <c r="E44" t="str">
         <v>iShares 1-3 Year Treasury Bond ETF</v>
@@ -21017,7 +21108,7 @@
         <v>126</v>
       </c>
       <c r="D45" t="str">
-        <v>iShares 3-7 Year Treasury Bond ETF</v>
+        <v>3-7 Year Treasury</v>
       </c>
       <c r="E45" t="str">
         <v>iShares 3-7 Year Treasury Bond ETF</v>
@@ -21044,7 +21135,7 @@
         <v>131</v>
       </c>
       <c r="D46" t="str">
-        <v>iShares 7-10 Year Treasury Bond ETF</v>
+        <v>7-10 Year Treasury</v>
       </c>
       <c r="E46" t="str">
         <v>iShares 7-10 Year Treasury Bond ETF</v>
@@ -21071,7 +21162,7 @@
         <v>49</v>
       </c>
       <c r="D47" t="str">
-        <v>iShares 20+ Year Treasury Bond ETF</v>
+        <v>20+ Year Treasury</v>
       </c>
       <c r="E47" t="str">
         <v>iShares 20+ Year Treasury Bond ETF</v>
@@ -21124,8 +21215,8 @@
       <c r="C49" t="s">
         <v>344</v>
       </c>
-      <c r="D49">
-        <v>0</v>
+      <c r="D49" t="str">
+        <v>Short-Term Inflation-Protected Securities ETF</v>
       </c>
       <c r="E49" t="str">
         <v>Vanguard Short-Term Inflation-Protected Securities ETF</v>
@@ -21232,8 +21323,8 @@
       <c r="C53" t="s">
         <v>346</v>
       </c>
-      <c r="D53">
-        <v>0</v>
+      <c r="D53" t="str">
+        <v>Mortgage-Backed Securities ETF</v>
       </c>
       <c r="E53" t="str">
         <v>Vanguard Mortgage-Backed Securities ETF</v>
@@ -21315,8 +21406,8 @@
       <c r="C56" t="s">
         <v>349</v>
       </c>
-      <c r="D56">
-        <v>0</v>
+      <c r="D56" t="str">
+        <v>iShares JP Morgan EM High Yield Bond ETF</v>
       </c>
       <c r="E56" t="str">
         <v>iShares Emerging Markets High Yield Bond ETF</v>
@@ -21862,7 +21953,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -22118,10 +22211,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C34FC6-78FE-492E-BECF-2EB9A04778A9}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:W31"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="A17:C22"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22129,9 +22222,11 @@
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="12" customWidth="1"/>
+    <col min="19" max="19" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -22141,16 +22236,16 @@
       <c r="C1" t="s">
         <v>448</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>435</v>
       </c>
-      <c r="E1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B2" t="s">
         <v>175</v>
@@ -22158,26 +22253,38 @@
       <c r="C2">
         <v>1.5</v>
       </c>
-      <c r="K2" t="b" cm="1">
-        <f t="array" aca="1" ref="K2:K22" ca="1">composities[portfolio_name]&lt;&gt;OFFSET(composities[portfolio_name],-1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="E2" t="str" cm="1">
+        <f t="array" ref="E2:E22">TEXT(composities[weight],IF(INT(composities[weight]*100)/100=composities[weight],"General","0.00"))</f>
+        <v>1.5</v>
+      </c>
+      <c r="F2" t="str" cm="1">
+        <f t="array" ref="F2:F8">_xlfn.UNIQUE(composities[portfolio_name])</f>
+        <v>ELECTION</v>
+      </c>
+      <c r="G2" t="str" cm="1">
+        <f t="array" ref="G2:G8">_xlfn.BYROW(_xlfn.ANCHORARRAY(F2),_xlfn.LAMBDA(_xlpm.portfolio,_xlfn.TEXTJOIN(", ",,_xlfn.BYROW(_xlfn._xlws.FILTER(_xlfn.HSTACK(composities[factor_name],_xlfn.ANCHORARRAY($E$2)),composities[portfolio_name]=_xlpm.portfolio),_xlfn.LAMBDA(_xlpm.factor,_xlfn.TEXTJOIN(" ",,_xlpm.factor))))))</f>
+        <v>XLF 1.5, ICLN -1, IWM 1.5, FEZ -1</v>
+      </c>
+      <c r="U2" t="b" cm="1">
+        <f t="array" aca="1" ref="U2:U22" ca="1">composities[portfolio_name]&lt;&gt;OFFSET(composities[portfolio_name],-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB2" t="s">
         <v>430</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AC2" t="s">
         <v>433</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AF2" t="s">
         <v>421</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AG2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B3" t="s">
         <v>431</v>
@@ -22185,23 +22292,32 @@
       <c r="C3">
         <v>-1</v>
       </c>
-      <c r="K3" t="b">
+      <c r="E3" t="str">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>FED</v>
+      </c>
+      <c r="G3" t="str">
+        <v>SHY 1, BSV 1</v>
+      </c>
+      <c r="U3" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="AA3" t="s">
         <v>175</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -22209,26 +22325,35 @@
       <c r="C4">
         <v>1.5</v>
       </c>
-      <c r="K4" t="b">
+      <c r="E4" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="F4" t="str">
+        <v>AI</v>
+      </c>
+      <c r="G4" t="str">
+        <v>AIQ 1, QQQ 0.25, IWM -0.25</v>
+      </c>
+      <c r="U4" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AA4" t="s">
         <v>431</v>
       </c>
-      <c r="R4">
+      <c r="AB4">
         <v>-1</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AC4" t="s">
         <v>434</v>
       </c>
-      <c r="T4" t="s">
+      <c r="AD4" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -22236,21 +22361,30 @@
       <c r="C5">
         <v>-1</v>
       </c>
-      <c r="K5" t="b">
+      <c r="E5" t="str">
+        <v>-1</v>
+      </c>
+      <c r="F5" t="str">
+        <v>GEOPOLITICS</v>
+      </c>
+      <c r="G5" t="str">
+        <v>GLD 0.75, USO 0.25</v>
+      </c>
+      <c r="U5" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="AA5" t="s">
         <v>5</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>439</v>
       </c>
@@ -22260,21 +22394,30 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="K6" t="b">
+      <c r="E6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2s10s</v>
+      </c>
+      <c r="G6" t="str">
+        <v>SHY -3.86, IEF 1</v>
+      </c>
+      <c r="U6" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="AA6" t="s">
         <v>8</v>
       </c>
-      <c r="R6">
+      <c r="AB6">
         <v>-1</v>
       </c>
-      <c r="S6" t="s">
+      <c r="AC6" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>439</v>
       </c>
@@ -22284,24 +22427,33 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="K7" t="b">
+      <c r="E7" t="str">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <v>XLPXLY</v>
+      </c>
+      <c r="G7" t="str">
+        <v>XLP 1, XLY -1</v>
+      </c>
+      <c r="U7" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="AA7" t="s">
         <v>236</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="s">
         <v>435</v>
       </c>
-      <c r="T7" t="s">
+      <c r="AD7" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>421</v>
       </c>
@@ -22311,27 +22463,36 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="K8" t="b">
+      <c r="E8" t="str">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <v>TRADEWAR</v>
+      </c>
+      <c r="G8" t="str">
+        <v>GLD 0.21, FXY 0.30, FXF 0.37, ^VIX3M -0.04, XLP 0.15, XLY -0.15</v>
+      </c>
+      <c r="U8" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="N8" t="s">
+      <c r="X8" t="s">
         <v>403</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="s">
         <v>238</v>
       </c>
-      <c r="R8">
+      <c r="AB8">
         <v>-1</v>
       </c>
-      <c r="S8" t="s">
+      <c r="AC8" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>421</v>
       </c>
@@ -22341,24 +22502,27 @@
       <c r="C9">
         <v>0.25</v>
       </c>
-      <c r="K9" t="b">
+      <c r="E9" t="str">
+        <v>0.25</v>
+      </c>
+      <c r="U9" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="N9" t="s">
+      <c r="X9" t="s">
         <v>7</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="s">
         <v>135</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>421</v>
       </c>
@@ -22368,27 +22532,30 @@
       <c r="C10">
         <v>-0.25</v>
       </c>
-      <c r="K10" t="b">
+      <c r="E10" t="str">
+        <v>-0.25</v>
+      </c>
+      <c r="U10" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="N10" t="s">
+      <c r="X10" t="s">
         <v>5</v>
       </c>
-      <c r="O10">
+      <c r="Y10">
         <v>-1</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="AA10" t="s">
         <v>49</v>
       </c>
-      <c r="R10">
+      <c r="AB10">
         <v>-1</v>
       </c>
-      <c r="T10" t="s">
+      <c r="AD10" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>450</v>
       </c>
@@ -22398,18 +22565,21 @@
       <c r="C11">
         <v>0.75</v>
       </c>
-      <c r="K11" t="b">
+      <c r="E11" t="str">
+        <v>0.75</v>
+      </c>
+      <c r="U11" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="AA11" t="s">
         <v>403</v>
       </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AF11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>450</v>
       </c>
@@ -22419,18 +22589,21 @@
       <c r="C12">
         <v>0.25</v>
       </c>
-      <c r="K12" t="b">
+      <c r="E12" t="str">
+        <v>0.25</v>
+      </c>
+      <c r="U12" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="AA12" t="s">
         <v>438</v>
       </c>
-      <c r="V12">
+      <c r="AF12">
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>451</v>
       </c>
@@ -22438,21 +22611,24 @@
         <v>51</v>
       </c>
       <c r="C13">
-        <f>-C14*L14/L13</f>
+        <f>-C14*V14/V13</f>
         <v>-3.8633879781420766</v>
       </c>
-      <c r="K13" t="b">
+      <c r="E13" t="str">
+        <v>-3.86</v>
+      </c>
+      <c r="U13" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="L13">
+      <c r="V13">
         <v>1.83</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="AA13" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>451</v>
       </c>
@@ -22462,24 +22638,27 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="K14" t="b">
+      <c r="E14" t="str">
+        <v>1</v>
+      </c>
+      <c r="U14" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="L14">
+      <c r="V14">
         <v>7.07</v>
       </c>
-      <c r="M14">
-        <f>L14/L13</f>
+      <c r="W14">
+        <f>V14/V13</f>
         <v>3.8633879781420766</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="AA14" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B15" t="s">
         <v>182</v>
@@ -22487,23 +22666,32 @@
       <c r="C15" s="8">
         <v>1</v>
       </c>
-      <c r="E15">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="L15">
         <v>3</v>
       </c>
-      <c r="G15" t="s">
-        <v>505</v>
-      </c>
-      <c r="H15">
+      <c r="N15" t="s">
+        <v>504</v>
+      </c>
+      <c r="O15">
         <v>22</v>
       </c>
-      <c r="K15" t="b">
+      <c r="U15" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B16" t="s">
         <v>178</v>
@@ -22511,147 +22699,201 @@
       <c r="C16" s="8">
         <v>-1</v>
       </c>
-      <c r="H16">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8" t="str">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="O16">
         <v>16</v>
       </c>
-      <c r="K16" t="b">
+      <c r="U16" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B17" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="8" cm="1">
-        <f t="array" ref="C17">E17/D17*$F$17/SUM(ABS(($E$17:$E$21)))</f>
+        <f t="array" ref="C17">L17/K17*$M$17/SUM(ABS(($L$17:$L$21)))</f>
         <v>0.20547945205479451</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8" t="str">
+        <v>0.21</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17">
         <v>14.6</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" s="9">
         <v>15</v>
       </c>
-      <c r="J17" cm="1">
-        <f t="array" ref="J17:J20">C17:C20*D17:D20</f>
+      <c r="T17" cm="1">
+        <f t="array" ref="T17:T20">C17:C20*K17:K20</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="K17" t="b">
+      <c r="U17" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="8">
-        <f>E18/D18*$F$17/COUNT($E$17:$E$21)</f>
+        <f>L18/K18*$M$17/COUNT($L$17:$L$21)</f>
         <v>0.29702970297029702</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8" t="str">
+        <v>0.30</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18">
         <v>10.1</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="J18">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="T18">
         <v>2.9999999999999996</v>
       </c>
-      <c r="K18" t="b">
+      <c r="U18" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>501</v>
+      </c>
+      <c r="B19" t="s">
+        <v>498</v>
+      </c>
+      <c r="C19" s="8">
+        <f>L19/K19*$M$17/COUNT($L$17:$L$21)</f>
+        <v>0.36585365853658536</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8" t="str">
+        <v>0.37</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="U19" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
         <v>502</v>
       </c>
-      <c r="B19" t="s">
-        <v>499</v>
-      </c>
-      <c r="C19" s="8">
-        <f>E19/D19*$F$17/COUNT($E$17:$E$21)</f>
-        <v>0.36585365853658536</v>
-      </c>
-      <c r="D19">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>2.9999999999999996</v>
-      </c>
-      <c r="K19" t="b">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>501</v>
+      </c>
+      <c r="B20" t="s">
+        <v>496</v>
+      </c>
+      <c r="C20" s="8">
+        <f>L20/K20*$M$17/COUNT($L$17:$L$21)</f>
+        <v>-3.7499999999999999E-2</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="str">
+        <v>-0.04</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20">
+        <v>80</v>
+      </c>
+      <c r="L20">
+        <v>-1</v>
+      </c>
+      <c r="T20">
+        <v>-3</v>
+      </c>
+      <c r="U20" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="M19" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>502</v>
-      </c>
-      <c r="B20" t="s">
-        <v>497</v>
-      </c>
-      <c r="C20" s="8">
-        <f>E20/D20*$F$17/COUNT($E$17:$E$21)</f>
-        <v>-3.7499999999999999E-2</v>
-      </c>
-      <c r="D20">
-        <v>80</v>
-      </c>
-      <c r="E20">
-        <v>-1</v>
-      </c>
-      <c r="J20">
-        <v>-3</v>
-      </c>
-      <c r="K20" t="b">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" ref="B21:B22" si="0">B15</f>
         <v>XLP</v>
       </c>
       <c r="C21" s="8">
-        <f>E21/D21*$F$17/COUNT($E$17:$E$21)</f>
+        <f>L21/K21*$M$17/COUNT($L$17:$L$21)</f>
         <v>0.15</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="8"/>
+      <c r="E21" s="8" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21">
         <v>20</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="U21" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -22661,122 +22903,199 @@
         <f>-C21</f>
         <v>-0.15</v>
       </c>
-      <c r="K22" t="b">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="str">
+        <v>-0.15</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="U22" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C23" s="8"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N26" t="str">
+        <f>_xlfn.TEXTJOIN(", ",,_xlfn.ANCHORARRAY(N28))</f>
+        <v>XLF, 1.5, ICLN, -1, IWM, 1.5, FEZ, -1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B28" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8">
-        <f>E28/D28</f>
+        <f>L28/K28</f>
         <v>0.20547945205479454</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28">
         <v>14.6</v>
       </c>
-      <c r="E28">
+      <c r="L28">
         <v>3</v>
       </c>
-      <c r="J28" cm="1">
-        <f t="array" ref="J28:J31">C28:C31*D28:D31</f>
+      <c r="N28" t="str" cm="1">
+        <f t="array" ref="N28:O31">_xlfn._xlws.FILTER(composities[[factor_name]:[weight]],composities[portfolio_name]="ELECTION")</f>
+        <v>XLF</v>
+      </c>
+      <c r="O28">
+        <v>1.5</v>
+      </c>
+      <c r="Q28" t="str" cm="1">
+        <f t="array" ref="Q28:R29">_xlfn._xlws.FILTER(composities[[factor_name]:[weight]],composities[portfolio_name]="2s10s")</f>
+        <v>SHY</v>
+      </c>
+      <c r="R28">
+        <v>-3.8633879781420766</v>
+      </c>
+      <c r="S28" t="str" cm="1">
+        <f t="array" ref="S28">_xlfn.LET(_xlpm.f,_xlfn._xlws.FILTER(composities[[factor_name]:[weight]],composities[portfolio_name]="ELECTION"),_xlfn.TEXTJOIN("; ",,_xlfn.BYROW(_xlpm.f,_xlfn.LAMBDA(_xlpm.row,_xlfn.TEXTJOIN(" ",,_xlpm.row)))))</f>
+        <v>XLF 1.5; ICLN -1; IWM 1.5; FEZ -1</v>
+      </c>
+      <c r="T28" cm="1">
+        <f t="array" ref="T28:T31">C28:C31*K28:K31</f>
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
       </c>
       <c r="C29" s="8">
-        <f>E29/D29</f>
+        <f>L29/K29</f>
         <v>0.29702970297029702</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29">
         <v>10.1</v>
       </c>
-      <c r="E29">
+      <c r="L29">
         <v>3</v>
       </c>
-      <c r="J29">
+      <c r="N29" t="str">
+        <v>ICLN</v>
+      </c>
+      <c r="O29">
+        <v>-1</v>
+      </c>
+      <c r="Q29" t="str">
+        <v>IEF</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="T29">
         <v>2.9999999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C30" s="8">
-        <f>E30/D30</f>
+        <f>L30/K30</f>
         <v>0.36585365853658541</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E30">
+      <c r="L30">
         <v>3</v>
       </c>
-      <c r="J30">
+      <c r="N30" t="str">
+        <v>IWM</v>
+      </c>
+      <c r="O30">
+        <v>1.5</v>
+      </c>
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="M30" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="W30" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C31" s="8">
-        <f>E31/D31</f>
+        <f>L31/K31</f>
         <v>-0.1125</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31">
         <v>80</v>
       </c>
-      <c r="E31">
-        <f>-SUM(E28:E30)</f>
+      <c r="L31">
+        <f>-SUM(L28:L30)</f>
         <v>-9</v>
       </c>
-      <c r="J31">
+      <c r="N31" t="str">
+        <v>FEZ</v>
+      </c>
+      <c r="O31">
+        <v>-1</v>
+      </c>
+      <c r="T31">
         <v>-9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:C14 B15 A15:A16 C15:C16 A28:C31">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>$K2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:C17 B18:C20 A18:A22 C21">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$K17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:C23">
-    <cfRule type="expression" dxfId="2" priority="23">
-      <formula>$K16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21 B22:C22">
-    <cfRule type="expression" dxfId="1" priority="21">
-      <formula>$K19</formula>
+  <conditionalFormatting sqref="A2:C22">
+    <cfRule type="expression" dxfId="1" priority="38">
+      <formula>$Q1048571</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22905,7 +23224,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B15" t="str">
         <v>Currencies</v>

</xml_diff>

<commit_message>
feature: Add LMXL data from excel file for BTC and BTC_vol factors
</commit_message>
<xml_diff>
--- a/factor_master.xlsx
+++ b/factor_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29024"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EF3926-DEF9-4F30-9E78-DE92A1211D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944A3071-975D-4798-8D4E-B0E54098CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="10" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="10" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="688">
   <si>
     <t>SPX</t>
   </si>
@@ -2141,6 +2141,21 @@
   </si>
   <si>
     <t>^EVZ,92169,0</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>BTC_vol</t>
+  </si>
+  <si>
+    <t>BTC1_price</t>
+  </si>
+  <si>
+    <t>BTC1_atm</t>
+  </si>
+  <si>
+    <t>lmxl</t>
   </si>
 </sst>
 </file>
@@ -2208,7 +2223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2231,6 +2246,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2273,18 +2291,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2335,6 +2341,18 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2541,7 +2559,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:T88" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}" name="data" displayName="data" ref="A1:T90" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{740DC173-AAC9-4239-A44E-C43F8517304D}" name="asset_class" dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{A3BC3BB8-0420-458E-AECD-FD567519FA40}" name="region" dataDxfId="33"/>
@@ -2565,34 +2583,34 @@
     <tableColumn id="13" xr3:uid="{64EF0381-B0C5-4226-B34E-0F9752A4A840}" name="ticker" dataDxfId="19">
       <calculatedColumnFormula>data[[#This Row],[factor_name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{073BDADC-3AC0-4FF9-9654-A316B2345A90}" name="short_name_yf" dataDxfId="4">
+    <tableColumn id="18" xr3:uid="{073BDADC-3AC0-4FF9-9654-A316B2345A90}" name="short_name_yf" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[shortName],"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{3A563104-B6B0-465C-9D22-154F5FEA1B83}" name="long_name_yf" dataDxfId="6">
+    <tableColumn id="19" xr3:uid="{3A563104-B6B0-465C-9D22-154F5FEA1B83}" name="long_name_yf" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[longName],"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A3F200A1-E769-49BA-8121-88EAA1180E80}" name="summary_yf" dataDxfId="5">
+    <tableColumn id="17" xr3:uid="{A3F200A1-E769-49BA-8121-88EAA1180E80}" name="summary_yf" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[longBusinessSummary],"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{D49341AB-DA48-473E-8CCB-3A3D04AED743}" name="note" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918301C-859F-40B7-9C3E-90E8F0495E68}" name="data_old" displayName="data_old" ref="A1:I45" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:I45" xr:uid="{6DAD1482-C63D-400D-9F51-F22A8E35CAD8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{B19D2B17-9AC9-4F1B-B32E-D4F72AAE469F}" name="asset_class" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{2C7CF29D-8E72-4B0C-A212-31F2A25D75C9}" name="region" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{C7E89EEC-2B5D-4C94-9327-1AC8E33DE708}" name="factor_name" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{B3F9004A-8BEB-463E-A746-8189A2AC2B3E}" name="factor_name_new" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{51CD7FB3-58FE-4906-B73C-7726C0A9C471}" name="description_override" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3CFF990B-3164-4533-821F-08CE7C6D82CA}" name="Description_GPT" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DD86D53E-A9B4-4387-ABF9-F2625E77982D}" name="Underlying" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D56FFF9A-72FF-42A4-B3D2-2F27AB16AF7A}" name="Active" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8476DFDE-B4B1-4FD9-99B4-DF1F2ABBD7D5}" name="description" dataDxfId="4">
       <calculatedColumnFormula>IF(data_old[[#This Row],[description_override]]="",data_old[[#This Row],[Description_GPT]],data_old[[#This Row],[description_override]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5606,13 +5624,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29859C-7358-4E2F-B5CC-7696F1DAC449}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:Y88"/>
+  <dimension ref="A1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5758,7 +5776,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="2"/>
       <c r="V2" t="b" cm="1">
-        <f t="array" ref="V2:V88">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
+        <f t="array" ref="V2:V90">MOD(_xlfn.SEQUENCE(ROWS(data[])),3)=1</f>
         <v>1</v>
       </c>
     </row>
@@ -11413,9 +11431,129 @@
         <v>0</v>
       </c>
     </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4">
+        <v>1</v>
+      </c>
+      <c r="I89" s="4">
+        <v>0</v>
+      </c>
+      <c r="J89" s="4">
+        <v>0</v>
+      </c>
+      <c r="K89" s="4">
+        <v>0</v>
+      </c>
+      <c r="L89" s="12" t="str" cm="1">
+        <f t="array" ref="L89">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="O89" s="12" cm="1">
+        <f t="array" ref="O89">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",1,1)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="P89" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q89" s="12" t="str">
+        <f>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[shortName],"-")</f>
+        <v>-</v>
+      </c>
+      <c r="R89" s="12" t="str">
+        <f>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[longName],"-")</f>
+        <v>-</v>
+      </c>
+      <c r="S89" s="12" t="str">
+        <f>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[longBusinessSummary],"-")</f>
+        <v>-</v>
+      </c>
+      <c r="T89" s="12"/>
+      <c r="V89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4">
+        <v>1</v>
+      </c>
+      <c r="I90" s="4">
+        <v>0</v>
+      </c>
+      <c r="J90" s="4">
+        <v>0</v>
+      </c>
+      <c r="K90" s="4">
+        <v>0</v>
+      </c>
+      <c r="L90" s="12" t="str" cm="1">
+        <f t="array" ref="L90">_xlfn.IFS(data[[#This Row],[description_override]]&lt;&gt;"",data[[#This Row],[description_override]],data[[#This Row],[Description_GPT]]&lt;&gt;"",data[[#This Row],[Description_GPT]],data[[#This Row],[Underlying]]&lt;&gt;"",data[[#This Row],[Underlying]],TRUE,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="N90" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="O90" s="12" cm="1">
+        <f t="array" ref="O90">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",1,1)</f>
+        <v>-0.01</v>
+      </c>
+      <c r="P90" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q90" s="12" t="str">
+        <f>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[shortName],"-")</f>
+        <v>-</v>
+      </c>
+      <c r="R90" s="12" t="str">
+        <f>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[longName],"-")</f>
+        <v>-</v>
+      </c>
+      <c r="S90" s="12" t="str">
+        <f>_xlfn.XLOOKUP(data[[#This Row],[ticker]],yf_desc[ticker],yf_desc[longBusinessSummary],"-")</f>
+        <v>-</v>
+      </c>
+      <c r="T90" s="12"/>
+      <c r="V90" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A81:F81 X81 O88 H81:R81 A82:R87 S2:T87 A2:R80">
+  <conditionalFormatting sqref="A2:R80 S2:T87 A81:F81 H81:R81 X81 A82:R87 O88">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>$V2</formula>
     </cfRule>
@@ -11601,7 +11739,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A64DEF-E706-4B9C-B282-71F34F86B3DF}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
@@ -11649,11 +11787,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A73">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
+        <f t="array" ref="A2:A75">_xlfn._xlws.FILTER(data[factor_name],data[Active])</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J73">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J75">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -13951,6 +14089,70 @@
       </c>
       <c r="J73">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" t="str">
+        <v>BTC</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C74" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="str">
+        <v>-</v>
+      </c>
+      <c r="G74" t="str">
+        <v>lmxl</v>
+      </c>
+      <c r="H74" t="str">
+        <v>BTC1_price</v>
+      </c>
+      <c r="I74" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J74">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" t="str">
+        <v>BTC_vol</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C75" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="str">
+        <v>-</v>
+      </c>
+      <c r="G75" t="str">
+        <v>lmxl</v>
+      </c>
+      <c r="H75" t="str">
+        <v>BTC1_atm</v>
+      </c>
+      <c r="I75" t="str">
+        <v>normal</v>
+      </c>
+      <c r="J75">
+        <v>-0.01</v>
       </c>
     </row>
   </sheetData>
@@ -16061,7 +16263,7 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977BD7F-9323-4F6D-98BF-C1B39119DCDE}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
@@ -16109,11 +16311,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A72">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
+        <f t="array" ref="A2:A74">_xlfn._xlws.FILTER(data[factor_name],data[Active]*(data[client]=0))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J72">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
+        <f t="array" ref="B2:J74">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:J1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -18379,6 +18581,70 @@
       </c>
       <c r="J72">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" t="str">
+        <v>BTC</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C73" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" t="str">
+        <v>-</v>
+      </c>
+      <c r="G73" t="str">
+        <v>lmxl</v>
+      </c>
+      <c r="H73" t="str">
+        <v>BTC1_price</v>
+      </c>
+      <c r="I73" t="str">
+        <v>lognormal</v>
+      </c>
+      <c r="J73">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" t="str">
+        <v>BTC_vol</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C74" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="str">
+        <v>-</v>
+      </c>
+      <c r="G74" t="str">
+        <v>lmxl</v>
+      </c>
+      <c r="H74" t="str">
+        <v>BTC1_atm</v>
+      </c>
+      <c r="I74" t="str">
+        <v>normal</v>
+      </c>
+      <c r="J74">
+        <v>-0.01</v>
       </c>
     </row>
   </sheetData>
@@ -18600,7 +18866,7 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A08F2F-299B-47F7-8064-36693758F4E3}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -18630,11 +18896,11 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A66">_xlfn._xlws.FILTER(data[factor_name],data[Active]*NOT(data[composite]))</f>
+        <f t="array" ref="A2:A68">_xlfn._xlws.FILTER(data[factor_name],data[Active]*NOT(data[composite]))</f>
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:E66">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:E1,data[#Headers]))</f>
+        <f t="array" ref="B2:E68">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(B1:E1,data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -19733,6 +19999,40 @@
       </c>
       <c r="E66" t="str">
         <v>Economic Policy Uncertainty Index for United States</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="str">
+        <v>BTC</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Currencies</v>
+      </c>
+      <c r="C67" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="str">
+        <v>BTC_vol</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Vol</v>
+      </c>
+      <c r="C68" t="str">
+        <v>USD</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68" t="str">
+        <v>-</v>
       </c>
     </row>
   </sheetData>
@@ -26374,7 +26674,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <f ca="1">TODAY()-1</f>
-        <v>45830</v>
+        <v>45844</v>
       </c>
       <c r="B2">
         <v>0.20547945205479451</v>

</xml_diff>